<commit_message>
Done Asgn 2 test case
</commit_message>
<xml_diff>
--- a/Middle Assignment/TestDesignTechique_PhamHongAnh.xlsx
+++ b/Middle Assignment/TestDesignTechique_PhamHongAnh.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NashTech\Rookies\NashTech_Homework\Middle Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5232032-1C57-4D25-A19F-12CA09B45397}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8EF652-29EB-46E2-947F-EC308CEE96C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="490" windowWidth="19160" windowHeight="10310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment 1" sheetId="1" r:id="rId1"/>
@@ -847,7 +847,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B26" authorId="0" shapeId="0" xr:uid="{989CC71A-0CBC-406A-9DCF-BD2454AF6A10}">
+    <comment ref="B27" authorId="0" shapeId="0" xr:uid="{989CC71A-0CBC-406A-9DCF-BD2454AF6A10}">
       <text>
         <r>
           <rPr>
@@ -876,7 +876,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="393">
   <si>
     <t>ID</t>
   </si>
@@ -1310,9 +1310,6 @@
     <t>When entering more than 6 numeric characters</t>
   </si>
   <si>
-    <t>When entering exactly 6 numeric characters</t>
-  </si>
-  <si>
     <t>When clicking on the Eye icon</t>
   </si>
   <si>
@@ -1478,9 +1475,6 @@
     <t>When entering only special characters</t>
   </si>
   <si>
-    <t>When entering alphabetic and numerical values only</t>
-  </si>
-  <si>
     <t>When entering alphabetic and special values only</t>
   </si>
   <si>
@@ -1517,9 +1511,6 @@
     <t>When selecting a day and a year only</t>
   </si>
   <si>
-    <t>Check default - The checkbox is unchecked</t>
-  </si>
-  <si>
     <t>When clicking on the checkbox</t>
   </si>
   <si>
@@ -1532,9 +1523,6 @@
     <t>When entering 50 alphanumeric characters</t>
   </si>
   <si>
-    <t>= check no SMS</t>
-  </si>
-  <si>
     <t>When entering more than 50 characters</t>
   </si>
   <si>
@@ -1571,9 +1559,6 @@
     <t>When clicking on "Privacy Policy"</t>
   </si>
   <si>
-    <t>When entering a valid password</t>
-  </si>
-  <si>
     <t>When copying a password and pasting it in the text field</t>
   </si>
   <si>
@@ -1583,9 +1568,6 @@
     <t>When entering a lowercase alphabetic value</t>
   </si>
   <si>
-    <t>Check sorting + num of values trong step</t>
-  </si>
-  <si>
     <t>When entering date by keyboard</t>
   </si>
   <si>
@@ -1626,12 +1608,6 @@
   </si>
   <si>
     <t>The placeholder shows "Please enter your phone number"</t>
-  </si>
-  <si>
-    <t>Hiểu sai ý?</t>
-  </si>
-  <si>
-    <t>2. Pop-up message shows Error message "Please enter a valid phone number"</t>
   </si>
   <si>
     <t>1. Enter a phone number 0123456789
@@ -1640,9 +1616,6 @@
   <si>
     <t>2.1 The text field becomes empty
 2.2 The | symbol returns to the left side of the text field</t>
-  </si>
-  <si>
-    <t>Fake phone num to see code?</t>
   </si>
   <si>
     <t>2. The slide to get SMS code becomes a text field with a placeholder
@@ -1652,68 +1625,6 @@
     <t>1. Enter a valid phone number 0888888888
 2. Slide to get SMS code
 3. Observe the placeholder in the SMS verification field</t>
-  </si>
-  <si>
-    <t>1. Enter a valid phone number 0888888888
-2. Slide to get SMS code
-3. Enter no SMS verification code
-4. Click the sign up button</t>
-  </si>
-  <si>
-    <t>4. Pop-up error message shows "Please enter Phone number"</t>
-  </si>
-  <si>
-    <t>3. Error message the SMS verification field "Please enter 6 digits"</t>
-  </si>
-  <si>
-    <t>1. Enter a valid phone number 0888888888
-2. Slide to get SMS code
-3. Enter a random verification code 112233 (6 digits)</t>
-  </si>
-  <si>
-    <t>1. Enter a valid phone number 0888888888
-2. Slide to get SMS code
-3. Enter a random verification code 11223344 (8 digits)</t>
-  </si>
-  <si>
-    <t>1. Enter a valid phone number 0888888888
-2. Slide to get SMS code
-3. Enter a random verification code 11223 (5 digits)</t>
-  </si>
-  <si>
-    <t>Field validation có cần click sign up?</t>
-  </si>
-  <si>
-    <t>3. No error message under the SMS verification field</t>
-  </si>
-  <si>
-    <t>1. Enter a valid phone number 0888888888
-2. Slide to get SMS code
-3. Enter a random verification code 11 223 (6 digits)</t>
-  </si>
-  <si>
-    <t>3. The SMS verification field does not allow a blank space</t>
-  </si>
-  <si>
-    <t>1. Enter a valid phone number 0888888888
-2. Slide to get SMS code
-3. Enter a special character #</t>
-  </si>
-  <si>
-    <t>3. Error message under the SMS verification field "Please enter 6 digits"</t>
-  </si>
-  <si>
-    <t>3.1 The SMS verification field does not allow a special value
-3.2 Error message under the SMS verification field "You can't leave this field empty"</t>
-  </si>
-  <si>
-    <t>1. Enter a valid phone number 0888888888
-2. Slide to get SMS code
-3. Enter an alphabetic character a</t>
-  </si>
-  <si>
-    <t>3.1 The SMS verification field does not allow an alphabetic value
-3.2 Error message under the SMS verification field "You can't leave this field empty"</t>
   </si>
   <si>
     <t>1. Enter a valid phone number 0888888888
@@ -1726,54 +1637,14 @@
 4.2 The | symbol returns to the left side of the text field</t>
   </si>
   <si>
-    <t>Chỉ test behavior của field</t>
-  </si>
-  <si>
     <t>1. Enter no numerical, alphabetical or special value
 2. Click the "Sign up" button</t>
   </si>
   <si>
-    <t>1. Enter 0123456789
-2. Click the "Sign up" button</t>
-  </si>
-  <si>
-    <t>1. Enter 012345678910
-2. Click the "Sign up" button</t>
-  </si>
-  <si>
-    <t>1. Enter 012345
-2. Click the "Sign up" button</t>
-  </si>
-  <si>
-    <t>1. Copy phone number 0123456789
-2. Paste the phone number into the text field
-3. Click the "Sign up" button</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Enter a phone number 01234 5678
-2. Click the "Sign up" button
-</t>
-  </si>
-  <si>
-    <t>1. Error message under the text field "Please enter a valid phone number"
-2. Pop-up message shows "Please enter the sms code"</t>
-  </si>
-  <si>
-    <t>1. Enter a special character #
-2. Click the "Sign up" button</t>
-  </si>
-  <si>
-    <t>1. Enter an alphabetic character a
-2. Click the "Sign up" button</t>
-  </si>
-  <si>
     <t>3. Pop-up message shows "Please enter the sms code"</t>
   </si>
   <si>
     <t>2. The button can slide</t>
-  </si>
-  <si>
-    <t>2. Pop-up message shows "Please enter the sms code"</t>
   </si>
   <si>
     <t>1. Type 111111111111111111111111111111111
@@ -1821,21 +1692,10 @@
 2. Click the "Sign up" button</t>
   </si>
   <si>
-    <t>1. Error message under the password field shows "Password should contain alphabetic and numeric character"
-2. "Sign up" button is not clickable</t>
-  </si>
-  <si>
-    <t>Có cần enter các field khác valid không?</t>
-  </si>
-  <si>
     <t>Observe the placeholder in the password field</t>
   </si>
   <si>
     <t>The placeholder shows "Minimum 6 characters with a number and a letter"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error message under the password field shows "Password should contain alphabetic and numeric character"
-</t>
   </si>
   <si>
     <t>1. Type 111111111111111111111111111111111
@@ -1847,84 +1707,602 @@
 3. Click the "Sign up" button</t>
   </si>
   <si>
-    <t xml:space="preserve">Bỏ sign up button vì chỉ check field </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type in the field "password012345678901234567890123456789012345678912" (50 characters)
-</t>
-  </si>
-  <si>
-    <t>Type in the field "password"</t>
-  </si>
-  <si>
-    <t>Type in the field "passwo" (6 characters)</t>
-  </si>
-  <si>
     <t>1. Enter valid data for other fields
 2. Type nothing in the field
 3. Click the "Sign up" button</t>
   </si>
   <si>
-    <t>3. Pop-up message shows "Please enter phone verification code"</t>
-  </si>
-  <si>
-    <t>No error message under the password field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type in the field "password0123456789012345678901234567890123456789123" (51 characters)
+    <t>1. Type in the field a character (a)
+2. Click on the Eye icon</t>
+  </si>
+  <si>
+    <t>1. Type in the field a character (a)
+2. Click on the (x) button</t>
+  </si>
+  <si>
+    <t>1. Observe the placeholders in the Month field
+2. Observe the placeholders in the Day field
+3. Observe the placeholders in the Year field</t>
+  </si>
+  <si>
+    <t>1. The placeholder shows "Month"
+2. The placeholder shows "Day"
+3. The placeholder shows "Year"</t>
+  </si>
+  <si>
+    <t>1. Click the Month field
+2. Scroll the bar to ensure it works</t>
+  </si>
+  <si>
+    <t>1. Click the Year field
+2. Scroll the bar from top to bottom
+3. Observe if years from 1900 to the present year (2022) are shown</t>
+  </si>
+  <si>
+    <t>1. Enter valid data for other fields
+2. Select an invalid date (February 31 2022)
+3. Click the "Sign up" button</t>
+  </si>
+  <si>
+    <t>3. Error message under the birthday field shows "Please select the correct birthday"</t>
+  </si>
+  <si>
+    <t>1. Enter valid data for other fields
+2. Select an valid date (January 1 2022)
+3. Click the "Sign up" button</t>
+  </si>
+  <si>
+    <t>3.1 Sign up successfully
+3.2 The sign up page becomes the homepage</t>
+  </si>
+  <si>
+    <t>1. Enter valid data for other fields
+2. Select no date
+3. Click the "Sign up" button</t>
+  </si>
+  <si>
+    <t>1. Enter valid data for other fields
+2. Select only January in Month field
+3. Click the "Sign up" button</t>
+  </si>
+  <si>
+    <t>3. Error message under the birthday field shows "You can't leave this empty"</t>
+  </si>
+  <si>
+    <t>1. Enter valid data for other fields
+2. Select only 1 in Day field
+3. Click the "Sign up" button</t>
+  </si>
+  <si>
+    <t>1. Enter valid data for other fields
+2. Select only 2000 in Year field
+3. Click the "Sign up" button</t>
+  </si>
+  <si>
+    <t>1. Enter valid data for other fields
+2. Select January in Month field
+3. Select 1 in Day field
+4. Click the "Sign up" button</t>
+  </si>
+  <si>
+    <t>1. Enter valid data for other fields
+2. Select January in Month field
+3. Select 2000 in Year field
+4. Click the "Sign up" button</t>
+  </si>
+  <si>
+    <t>4. Error message under the birthday field shows "You can't leave this empty"</t>
+  </si>
+  <si>
+    <t>1. Enter valid data for other fields
+2. Select 1 in Day field
+3. Select 2000 in Year field
+4. Click the "Sign up" button</t>
+  </si>
+  <si>
+    <t>1. Enter valid data for other fields
+2. Select 31 in Day field
+3. Select December in Month field
+4. Select 2000 in Year field
+5. Click the "Sign up" button</t>
+  </si>
+  <si>
+    <t>5. Error message under the birthday field shows "Wrong birthday format"</t>
+  </si>
+  <si>
+    <t>Enter 1 into the Day format</t>
+  </si>
+  <si>
+    <t>Entering date by keyboard is not possible</t>
+  </si>
+  <si>
+    <t>Observe the placeholders in the Gender field</t>
+  </si>
+  <si>
+    <t>The placeholder shows "Select"</t>
+  </si>
+  <si>
+    <t>1. Click the Gender field
+2. Scroll the bar to ensure it works</t>
+  </si>
+  <si>
+    <t>1. Click the Gender field
+2. Scroll the bar from top to bottom
+3. Observe if Male and Female are shown</t>
+  </si>
+  <si>
+    <t>1. Enter valid data for other fields
+2. Select Male in Gender field
+3. Click the "Sign up" button</t>
+  </si>
+  <si>
+    <t>1. Enter valid data for other fields
+2. Select no gender in Gender field
+3. Click the "Sign up" button</t>
+  </si>
+  <si>
+    <t>Observe the placeholders in the Full name field</t>
+  </si>
+  <si>
+    <t>The placeholder shows "First Last"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Enter valid data for other fields
+2. Enter name Nguyen Van (9 characters)
+3. Click the "Sign up" button
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Error message under the password field shows "The length of Password should be 6-50 characters"
+    <t xml:space="preserve">1. Enter valid data for other fields
+2. Enter name Nguyen (6 characters)
+3. Click the "Sign up" button
 </t>
   </si>
   <si>
-    <t>Type in the field "pass" (4 characters)</t>
+    <t xml:space="preserve">1. Enter valid data for other fields
+2. Enter name AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA (50 characters)
+3. Click the "Sign up" button
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Enter valid data for other fields
+2. Enter name Nguy (4 characters)
+3. Click the "Sign up" button
+</t>
+  </si>
+  <si>
+    <t>2. Error message under the Full name field "The name length should be 2-50 characters"
+3. The "Sign up" button cannot be clicked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Enter valid data for other fields
+2. Enter name NguyeNguyeNguyeNguyeNguyeNguyeNguyeNguyeNguyeNguyen (51 characters)
+3. Click the "Sign up" button
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Enter valid data for other fields
+2. Entera blank space
+3. Click the "Sign up" button
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Enter valid data for other fields
+2. Enter name NguyenVan (8 characters)
+3. Click the "Sign up" button
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Enter valid data for other fields
+2. Copy a name NguyenVan (8 characters)
+3. Paste the name into the Full name field
+4. Click the "Sign up" button
+</t>
+  </si>
+  <si>
+    <t>4.1 Sign up successfully
+4.2 The sign up page becomes the homepage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Enter valid data for other fields
+2. Enter name NguyenVan (8 characters)
+3. Click the close (x) button
+</t>
+  </si>
+  <si>
+    <t>3.1 The text field becomes empty
+3.2 The | symbol returns to the left side of the text field</t>
+  </si>
+  <si>
+    <t>2. The slide button becomes the SMS verification field
+5.1 Sign up successfully
+5.2 The sign up page becomes the homepage</t>
+  </si>
+  <si>
+    <t>2. Pop-up error message shows "Please enter a valid phone number"
+3. Pop-up error message shows "Please enter a sms code"</t>
+  </si>
+  <si>
+    <t>1. Enter no value into the phone number field
+2. Slide the SMS verification button to get the SMS code
+3. Enter valid information into other fields
+4. Click the Signup button</t>
+  </si>
+  <si>
+    <t>1. Enter an already existing phone number into phone number field
+2. Slide the SMS verification button to get the SMS code
+3. Enter valid information into other required fields
+4. Click the Signup button</t>
+  </si>
+  <si>
+    <t>4. Pop-up error message shows "This phone number is linked to another account, please enter another number"</t>
+  </si>
+  <si>
+    <t>When signing up fail after entering an invalid SMS code</t>
+  </si>
+  <si>
+    <t>1. Enter a valid phone number (0888888888) into the phone number field
+2. Slide the SMS verification button to get the SMS code
+3. After receiving the SMS verification code, enter the code into the SMS verification field
+4. Enter valid data for other fields
+5. Click the "Sign up" button</t>
+  </si>
+  <si>
+    <t>1. Enter an invalid phone number (01234) into the phone number field
+2. Slide the SMS verification button to get the SMS code
+3. Click the Signup button</t>
+  </si>
+  <si>
+    <t>1. Enter a valid phone number (0888888888) into the phone number field
+2. Slide the SMS verification button to get the SMS code
+3. After receiving the SMS verification code, enter an invalid code into the SMS verification field
+4. Enter valid data for other fields
+5. Click the "Sign up" button</t>
+  </si>
+  <si>
+    <t>5. Pop-up error message shows "Invalid verification code"</t>
+  </si>
+  <si>
+    <t>1. Enter an invalid phone number the phone number field
+2. Slide the SMS verification button to get the SMS code
+3. Enter invalid information into other fields
+4. Click the Signup button</t>
+  </si>
+  <si>
+    <t>1. Enter no value into the phone number field
+2. Slide the SMS verification button to get the SMS code
+3. Enter no information into other fields
+4. Click the Signup button</t>
+  </si>
+  <si>
+    <t>2. Pop-up message shows Error message "Please enter a valid phone number"
+4. Pop-up message shows Error message "Please enter sms code"</t>
+  </si>
+  <si>
+    <t>2. Error message shows "Please enter Phone number"
+4. Pop-up error message shows "Please enter a sms code"</t>
+  </si>
+  <si>
+    <t>2. Error message under the phone number field shows "Please enter Phone number"
+4. Pop-up message shows Error message "Please enter sms code"</t>
+  </si>
+  <si>
+    <t>3. Pop-up message shows "Please enter Password value"</t>
+  </si>
+  <si>
+    <t>3. Error message under the Full name field "Please enter Full name"</t>
+  </si>
+  <si>
+    <t>Click on the "Facebook" button</t>
+  </si>
+  <si>
+    <t>Click on the "Google" button</t>
+  </si>
+  <si>
+    <t>A new screen shows up to sign up with a Facebook account</t>
+  </si>
+  <si>
+    <t>A new screen shows up to sign up with a Google account</t>
+  </si>
+  <si>
+    <t>Click on the "Sign up with Email" button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A new screen shows up to sign up with an Email </t>
+  </si>
+  <si>
+    <t>Observe the initial status of the checkbox</t>
+  </si>
+  <si>
+    <t>The box is unchecked</t>
+  </si>
+  <si>
+    <t>Click on the checkbox</t>
+  </si>
+  <si>
+    <t>The box is checked</t>
+  </si>
+  <si>
+    <t>Check default - Check the default status of the checkbox</t>
+  </si>
+  <si>
+    <t>Click on the "Term of Use" line</t>
+  </si>
+  <si>
+    <t>A new tab appears showing terms of use</t>
+  </si>
+  <si>
+    <t>Click on the "Privacy Policy" line</t>
+  </si>
+  <si>
+    <t>A new tab appears showing privacy policy</t>
+  </si>
+  <si>
+    <t>3. Pop-up message shows Error message "Please enter a valid phone number"</t>
+  </si>
+  <si>
+    <t>1. Enter 0123456789
+2. Enter valid data for other required fields
+3. Click the "Sign up" button</t>
+  </si>
+  <si>
+    <t>1. Enter 012345678910
+2. Enter valid data for other required fields
+3. Click the "Sign up" button</t>
+  </si>
+  <si>
+    <t>1. Enter 012345
+2. Enter valid data for other required fields
+3. Click the "Sign up" button</t>
+  </si>
+  <si>
+    <t>1. Copy phone number 0123456789
+2. Paste the phone number into the text field
+3. Enter valid data for other required fields
+4. Click the "Sign up" button</t>
+  </si>
+  <si>
+    <t>4. Pop-up message shows "Please enter the sms code"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Enter a phone number 01234 5678
+2. Enter valid data for other required fields
+3. Click the "Sign up" button
+</t>
+  </si>
+  <si>
+    <t>2. Error message under the text field "Please enter a valid phone number"
+3. Pop-up message shows "Please enter the sms code"</t>
+  </si>
+  <si>
+    <t>1. Enter a special character #
+2. Enter valid data for other required fields
+3. Click the "Sign up" button</t>
+  </si>
+  <si>
+    <t>1. Enter an alphabetic character a
+2. Enter valid data for other required fields
+3. Click the "Sign up" button</t>
+  </si>
+  <si>
+    <t>1. Enter a valid phone number 0888888888
+2. Slide to get SMS code
+3. Enter no SMS verification code
+4. Enter valid data for other required fields
+5. Click the sign up button</t>
+  </si>
+  <si>
+    <t>5. Pop-up error message shows "Please enter SMS Verification code"</t>
+  </si>
+  <si>
+    <t>1. Enter a valid phone number 0888888888
+2. Slide to get SMS code
+3. Enter a random verification code 11223 (5 digits)
+4. Enter valid data for other required fields
+5. Click the "Sign up" button</t>
+  </si>
+  <si>
+    <t>3. Error message the SMS verification field "Please enter 6 digits"
+5. The "Sign up" button cannot be clicked</t>
+  </si>
+  <si>
+    <t>1. Enter a valid phone number 0888888888
+2. Slide to get SMS code
+3. Enter a random verification code 112233 (6 digits)
+4. Enter valid data for other required fields
+5. Click the "Sign up" button</t>
+  </si>
+  <si>
+    <t>1. Enter a valid phone number 0888888888
+2. Slide to get SMS code
+3. Enter a random verification code 11223344 (8 digits)
+4. Enter valid data for other required fields
+5. Click the "Sign up" button</t>
+  </si>
+  <si>
+    <t>When entering 6 numeric characters</t>
+  </si>
+  <si>
+    <t>1. Enter a valid phone number 0888888888
+2. Slide to get SMS code
+3. Enter a random verification code with a blank space 11 223 (7 digits)
+4. Enter valid data for other required fields
+5. Click the "Sign up" button</t>
+  </si>
+  <si>
+    <t>3. The SMS verification field does not allow a blank space
+5. Pop-up error message shows "Invalid verification code"</t>
+  </si>
+  <si>
+    <t>3 The SMS verification field does not allow a special value
+5. Pop-up error message shows "Invalid verification code"</t>
+  </si>
+  <si>
+    <t>1. Enter a valid phone number 0888888888
+2. Slide to get SMS code
+3. Enter a special character #
+4. Enter valid data for other required fields
+5. Click the "Sign up" button</t>
+  </si>
+  <si>
+    <t>1. Enter a valid phone number 0888888888
+2. Slide to get SMS code
+3. Enter an alphabetic character a
+4. Enter valid data for other required fields
+5. Click the "Sign up" button</t>
+  </si>
+  <si>
+    <t>3. The SMS verification field does not allow an alphabetic value
+5. Pop-up error message shows "Invalid verification code"</t>
+  </si>
+  <si>
+    <t>1. Type in the field "password"
+2. Enter valid information for other fields
+3. Click on the "Sign up" button</t>
+  </si>
+  <si>
+    <t>1. Type in the field "passwo" (6 characters)
+2. Enter valid information for other fields
+3. Click on the "Sign up" button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Type in the field "passwordsspasswordsspasswordsspasswordsspasswordss" (50 characters)
+2. Enter valid information for other fields
+3. Click on the "Sign up" button
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Type in the field "passwordsspasswordsspasswordsspasswordsspasswordss1" (51 characters)
+2. Enter valid information for other fields
+3. Click on the "Sign up" button
+</t>
+  </si>
+  <si>
+    <t>1. Type in the field "pass" (4 characters)
+2. Enter valid information for other fields
+3. Click on the "Sign up" button</t>
+  </si>
+  <si>
+    <t>1. Error message under the password field shows "Password should contain alphabetic and numeric character"
+3. "Sign up" button is not clickable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Error message under the password field shows "The length of Password should be 6-50 characters"
+3. "Sign up" button is not clickable
+</t>
   </si>
   <si>
     <t>1. Error message under the password field shows "The length of Password should be 6-50 characters"
-2. Error message under the password field shows "Password should contain alphabetic and numeric character"</t>
-  </si>
-  <si>
-    <t>1. Type in the field a special character # (1 character)
-2. Continue typing 5 more # into the field (######) (6 characters in total)</t>
-  </si>
-  <si>
-    <t>1. Type in the field a numerical value 1 (1 character)
-2. Continue typing 5 more 1 into the field (111111) (6 characters in total)</t>
-  </si>
-  <si>
-    <t>Error message under the password field shows "The length of Password should be 6-50 characters"</t>
-  </si>
-  <si>
-    <t>Type in the field an alphabetic and numerical character 1a#</t>
-  </si>
-  <si>
-    <t>1. Type in the field an uppercase alphabetic character A</t>
-  </si>
-  <si>
-    <t>1. Type in the field an alphabetic and numerical character 1a
-2. Type 4 more alphabetic characters (1aaaaa)</t>
-  </si>
-  <si>
-    <t>1. Error message under the password field shows "The length of Password should be 6-50 characters"
-2. No error message is shown</t>
-  </si>
-  <si>
-    <t>1. Type in the field an alphabetic and numerical character a#
-2. Type 4 more alphabetic characters (a#aaaa)</t>
-  </si>
-  <si>
-    <t>1. Type in the field an alphabetic and numerical character 1#</t>
-  </si>
-  <si>
-    <t>Type in a blank space and "password" into the field ( password) (9 characters in total)</t>
-  </si>
-  <si>
-    <t>Error message under the password field shows "Password should contain alphabetic and numeric character"</t>
-  </si>
-  <si>
-    <t>Type in 6 alphabetic values aaaaaa</t>
+3. "Sign up" button is not clickable</t>
+  </si>
+  <si>
+    <t>1. Type in a blank space between characters into the field ( password) (9 characters in total)
+2. Enter valid information for other fields
+3. Click on the "Sign up" button</t>
+  </si>
+  <si>
+    <t>1. Type in 6 alphabetic values aaaaaa
+2. Enter valid information for other fields
+3. Click on the "Sign up" button</t>
+  </si>
+  <si>
+    <t>1. Type only numerical values into the field (111111)
+2. Enter valid information for other fields
+3. Click on the "Sign up" button</t>
+  </si>
+  <si>
+    <t>1. Type in 6 special values into the field (######) 
+2. Enter valid information for other fields
+3. Click on the "Sign up" button</t>
+  </si>
+  <si>
+    <t>1. Type in the field an alphabetic and numerical character 1aaaaa
+2. Enter valid information for other fields
+3. Click on the "Sign up" button</t>
+  </si>
+  <si>
+    <t>1. Type in a 6-digit password with both alphabetic and special values (a#aaaa)
+2. Enter valid information for other fields
+3. Click on the "Sign up" button</t>
+  </si>
+  <si>
+    <t>1. Type in a 6-digit password with numeric and special characters (1#1111)
+2. Enter valid information for other fields
+3. Click on the "Sign up" button</t>
+  </si>
+  <si>
+    <t>1. Type in the field a 6-digit password with alphabetic, numerical, and special characters (1a#111)
+2. Enter valid information for other fields
+3. Click on the "Sign up" button</t>
+  </si>
+  <si>
+    <t>1. Type in a 6-digit password with an uppercase alphabetic character (A1aaaa)
+2. Enter valid information for other fields
+3. Click on the "Sign up" button</t>
+  </si>
+  <si>
+    <t>1. Type in a 6-digit password with a lowercase alphabetic character (a1aaaa)
+2. Enter valid information for other fields
+3. Click on the "Sign up" button</t>
+  </si>
+  <si>
+    <t>When entering alphabetic and numerical values only (A valid password)</t>
+  </si>
+  <si>
+    <t>1. Copy a password 1a#aaa
+2. Paste the phone number into the password field
+3. Enter valid information for other fields
+4. Click on the "Sign up" button</t>
+  </si>
+  <si>
+    <t>2. The letter (a) is shown instead of a dot symbol (•)</t>
+  </si>
+  <si>
+    <t>2. The scroll bar shows all values from top to bottom</t>
+  </si>
+  <si>
+    <t>1. Click the Month field
+2. Scroll the bar from top to bottom
+3. Observe if all months from January to December are shown
+4. Observe if all months are sorted from January to December</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. All months from January to December are shown in the drop down bar
+4. All months from January to December are sorted in the drop down bar </t>
+  </si>
+  <si>
+    <t>1. Click the Day field
+2. Scroll the bar from top to bottom
+3. Observe if all days from 1 to 31 are shown
+4. Observe if all days are sorted from 1 to 31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. All days from 1 to 31 are shown in the drop down bar
+4. All days from 1 to 31 are sorted in the drop down bar </t>
+  </si>
+  <si>
+    <t>When the verification code expires</t>
+  </si>
+  <si>
+    <t>1. Enter a valid phone number 0888888888
+2. Slide to get SMS code
+3. Wait for the code to expires
+4. Enter valid data for other required fields
+5. Click the sign up button</t>
+  </si>
+  <si>
+    <t>3. The "Resend" button appears at the right side of the field
+5. Error message shows "Please enter SMS verification code"</t>
+  </si>
+  <si>
+    <t>3. All years from 1900 to 2022 are shown in the drop down bar</t>
+  </si>
+  <si>
+    <t>3. Male and Female are shown</t>
+  </si>
+  <si>
+    <t>2. The slide button becomes the SMS verification field
+5. Pop-up error message shows "Invalid verification code"</t>
   </si>
 </sst>
 </file>
@@ -2286,6 +2664,9 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2294,9 +2675,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -14823,14 +15201,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{861DB058-9ABC-4928-81FB-0309C7B8DB85}">
   <dimension ref="A1:Z203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="28" customWidth="1"/>
-    <col min="2" max="2" width="33" style="31" customWidth="1"/>
+    <col min="2" max="2" width="35.453125" style="31" customWidth="1"/>
     <col min="3" max="3" width="49.26953125" style="31" customWidth="1"/>
     <col min="4" max="4" width="49.08984375" style="31" customWidth="1"/>
     <col min="5" max="5" width="12.1796875" style="33" customWidth="1"/>
@@ -14888,16 +15266,16 @@
     </row>
     <row r="2" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="38" t="s">
-        <v>159</v>
-      </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
+        <v>158</v>
+      </c>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
       <c r="J2" s="26"/>
       <c r="K2" s="26"/>
       <c r="L2" s="26"/>
@@ -14918,7 +15296,7 @@
     </row>
     <row r="3" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="40" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B3" s="46"/>
       <c r="C3" s="46"/>
@@ -14946,7 +15324,7 @@
       <c r="Y3" s="26"/>
       <c r="Z3" s="26"/>
     </row>
-    <row r="4" spans="1:26" s="10" customFormat="1" ht="83" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" s="10" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>1</v>
       </c>
@@ -14954,14 +15332,12 @@
         <v>121</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>297</v>
+        <v>260</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>278</v>
-      </c>
-      <c r="E4" s="32" t="s">
-        <v>243</v>
-      </c>
+        <v>245</v>
+      </c>
+      <c r="E4" s="32"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
@@ -14973,13 +15349,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="E5" s="32"/>
       <c r="F5" s="13"/>
@@ -14993,45 +15369,41 @@
         <v>3</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>298</v>
+        <v>261</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>279</v>
-      </c>
-      <c r="E6" s="32" t="s">
-        <v>267</v>
-      </c>
+        <v>244</v>
+      </c>
+      <c r="E6" s="32"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
       <c r="I6" s="32"/>
     </row>
-    <row r="7" spans="1:26" s="10" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" s="10" customFormat="1" ht="53" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="27">
         <f ca="1">IF(OFFSET(A7,-1,0) ="",OFFSET(A7,-2,0)+1,OFFSET(A7,-1,0)+1 )</f>
         <v>4</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>269</v>
+        <v>339</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>244</v>
-      </c>
-      <c r="E7" s="32" t="s">
-        <v>299</v>
-      </c>
+        <v>338</v>
+      </c>
+      <c r="E7" s="32"/>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
       <c r="I7" s="32"/>
     </row>
-    <row r="8" spans="1:26" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" s="10" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="27">
         <f ca="1">IF(OFFSET(A8,-1,0) ="",OFFSET(A8,-2,0)+1,OFFSET(A8,-1,0)+1 )</f>
         <v>5</v>
@@ -15040,10 +15412,10 @@
         <v>133</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>270</v>
+        <v>340</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>244</v>
+        <v>338</v>
       </c>
       <c r="E8" s="32"/>
       <c r="F8" s="13"/>
@@ -15051,7 +15423,7 @@
       <c r="H8" s="13"/>
       <c r="I8" s="32"/>
     </row>
-    <row r="9" spans="1:26" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" s="10" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27">
         <f t="shared" ref="A9:A83" ca="1" si="0">IF(OFFSET(A9,-1,0) ="",OFFSET(A9,-2,0)+1,OFFSET(A9,-1,0)+1 )</f>
         <v>6</v>
@@ -15060,10 +15432,10 @@
         <v>134</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>271</v>
+        <v>341</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>244</v>
+        <v>338</v>
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="13"/>
@@ -15071,7 +15443,7 @@
       <c r="H9" s="13"/>
       <c r="I9" s="32"/>
     </row>
-    <row r="10" spans="1:26" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" s="10" customFormat="1" ht="66.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>7</v>
@@ -15080,10 +15452,10 @@
         <v>123</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>272</v>
+        <v>342</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>277</v>
+        <v>343</v>
       </c>
       <c r="E10" s="32"/>
       <c r="F10" s="13"/>
@@ -15100,13 +15472,13 @@
         <v>124</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>273</v>
+        <v>344</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>274</v>
+        <v>345</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
@@ -15122,10 +15494,10 @@
         <v>125</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>275</v>
+        <v>346</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>274</v>
+        <v>345</v>
       </c>
       <c r="E12" s="32"/>
       <c r="F12" s="13"/>
@@ -15142,10 +15514,10 @@
         <v>132</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>276</v>
+        <v>347</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>274</v>
+        <v>345</v>
       </c>
       <c r="E13" s="32"/>
       <c r="F13" s="13"/>
@@ -15159,13 +15531,13 @@
         <v>11</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="E14" s="32"/>
       <c r="F14" s="13"/>
@@ -15209,99 +15581,93 @@
         <v>12</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>248</v>
-      </c>
-      <c r="E16" s="32" t="s">
-        <v>247</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="E16" s="32"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
       <c r="I16" s="32"/>
     </row>
-    <row r="17" spans="1:26" s="10" customFormat="1" ht="52" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" s="10" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="27">
         <f ca="1">IF(OFFSET(A17,-1,0) ="",OFFSET(A17,-2,0)+1,OFFSET(A17,-1,0)+1 )</f>
         <v>13</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>250</v>
+        <v>348</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>251</v>
-      </c>
-      <c r="E17" s="34" t="s">
-        <v>211</v>
-      </c>
+        <v>349</v>
+      </c>
+      <c r="E17" s="34"/>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
       <c r="I17" s="32"/>
     </row>
-    <row r="18" spans="1:26" s="10" customFormat="1" ht="51.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" s="10" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">IF(OFFSET(A18,-1,0) ="",OFFSET(A18,-2,0)+1,OFFSET(A18,-1,0)+1 )</f>
         <v>14</v>
       </c>
-      <c r="B18" s="29" t="s">
-        <v>135</v>
+      <c r="B18" s="30" t="s">
+        <v>387</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>255</v>
+        <v>388</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>252</v>
-      </c>
-      <c r="E18" s="32"/>
+        <v>389</v>
+      </c>
+      <c r="E18" s="34"/>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
       <c r="I18" s="32"/>
     </row>
-    <row r="19" spans="1:26" s="10" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" s="10" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>15</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>254</v>
+        <v>350</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>261</v>
-      </c>
-      <c r="E19" s="32" t="s">
-        <v>256</v>
-      </c>
+        <v>351</v>
+      </c>
+      <c r="E19" s="32"/>
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
       <c r="I19" s="32"/>
     </row>
-    <row r="20" spans="1:26" s="10" customFormat="1" ht="52" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" s="10" customFormat="1" ht="75.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>16</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>253</v>
+        <v>353</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>257</v>
+        <v>351</v>
       </c>
       <c r="E20" s="32"/>
       <c r="F20" s="13"/>
@@ -15309,19 +15675,19 @@
       <c r="H20" s="13"/>
       <c r="I20" s="32"/>
     </row>
-    <row r="21" spans="1:26" s="10" customFormat="1" ht="53" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" s="10" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>17</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>126</v>
+        <v>354</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>258</v>
+        <v>352</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>259</v>
+        <v>315</v>
       </c>
       <c r="E21" s="32"/>
       <c r="F21" s="13"/>
@@ -15329,19 +15695,19 @@
       <c r="H21" s="13"/>
       <c r="I21" s="32"/>
     </row>
-    <row r="22" spans="1:26" s="10" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" s="10" customFormat="1" ht="86" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>18</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>260</v>
+        <v>355</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>262</v>
+        <v>356</v>
       </c>
       <c r="E22" s="32"/>
       <c r="F22" s="13"/>
@@ -15349,19 +15715,19 @@
       <c r="H22" s="13"/>
       <c r="I22" s="32"/>
     </row>
-    <row r="23" spans="1:26" s="10" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" s="10" customFormat="1" ht="73" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>19</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>263</v>
+        <v>358</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>264</v>
+        <v>357</v>
       </c>
       <c r="E23" s="32"/>
       <c r="F23" s="13"/>
@@ -15369,19 +15735,19 @@
       <c r="H23" s="13"/>
       <c r="I23" s="32"/>
     </row>
-    <row r="24" spans="1:26" s="10" customFormat="1" ht="57.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" s="10" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="27">
-        <f ca="1">IF(OFFSET(A24,-1,0) ="",OFFSET(A24,-2,0)+1,OFFSET(A24,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>20</v>
       </c>
-      <c r="B24" s="15" t="s">
-        <v>139</v>
+      <c r="B24" s="29" t="s">
+        <v>132</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>265</v>
+        <v>359</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>266</v>
+        <v>360</v>
       </c>
       <c r="E24" s="32"/>
       <c r="F24" s="13"/>
@@ -15389,71 +15755,69 @@
       <c r="H24" s="13"/>
       <c r="I24" s="32"/>
     </row>
-    <row r="25" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="45" t="s">
+    <row r="25" spans="1:26" s="10" customFormat="1" ht="57.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="27">
+        <f ca="1">IF(OFFSET(A25,-1,0) ="",OFFSET(A25,-2,0)+1,OFFSET(A25,-1,0)+1 )</f>
+        <v>21</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>241</v>
+      </c>
+      <c r="D25" s="30" t="s">
+        <v>242</v>
+      </c>
+      <c r="E25" s="32"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="32"/>
+    </row>
+    <row r="26" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="45" t="s">
         <v>127</v>
       </c>
-      <c r="B25" s="46"/>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="46"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="46"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="26"/>
-      <c r="N25" s="26"/>
-      <c r="O25" s="26"/>
-      <c r="P25" s="26"/>
-      <c r="Q25" s="26"/>
-      <c r="R25" s="26"/>
-      <c r="S25" s="26"/>
-      <c r="T25" s="26"/>
-      <c r="U25" s="26"/>
-      <c r="V25" s="26"/>
-      <c r="W25" s="26"/>
-      <c r="X25" s="26"/>
-      <c r="Y25" s="26"/>
-      <c r="Z25" s="26"/>
-    </row>
-    <row r="26" spans="1:26" s="10" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="27">
-        <f ca="1">IF(OFFSET(A26,-2,0) ="",OFFSET(A26,-2,0)+1,OFFSET(A26,-2,0)+1 )</f>
-        <v>21</v>
-      </c>
-      <c r="B26" s="30" t="s">
-        <v>221</v>
-      </c>
-      <c r="C26" s="29" t="s">
-        <v>303</v>
-      </c>
-      <c r="D26" s="30" t="s">
-        <v>304</v>
-      </c>
-      <c r="E26" s="32" t="s">
-        <v>293</v>
-      </c>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="32"/>
-    </row>
-    <row r="27" spans="1:26" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="46"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="26"/>
+      <c r="N26" s="26"/>
+      <c r="O26" s="26"/>
+      <c r="P26" s="26"/>
+      <c r="Q26" s="26"/>
+      <c r="R26" s="26"/>
+      <c r="S26" s="26"/>
+      <c r="T26" s="26"/>
+      <c r="U26" s="26"/>
+      <c r="V26" s="26"/>
+      <c r="W26" s="26"/>
+      <c r="X26" s="26"/>
+      <c r="Y26" s="26"/>
+      <c r="Z26" s="26"/>
+    </row>
+    <row r="27" spans="1:26" s="10" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="27">
-        <f ca="1">IF(OFFSET(A27,-1,0) ="",OFFSET(A27,-2,0)+1,OFFSET(A27,-1,0)+1 )</f>
+        <f ca="1">IF(OFFSET(A27,-2,0) ="",OFFSET(A27,-2,0)+1,OFFSET(A27,-2,0)+1 )</f>
         <v>22</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>140</v>
-      </c>
-      <c r="C27" s="30" t="s">
-        <v>294</v>
+        <v>217</v>
+      </c>
+      <c r="C27" s="29" t="s">
+        <v>262</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>295</v>
+        <v>321</v>
       </c>
       <c r="E27" s="32"/>
       <c r="F27" s="13"/>
@@ -15461,19 +15825,19 @@
       <c r="H27" s="13"/>
       <c r="I27" s="32"/>
     </row>
-    <row r="28" spans="1:26" s="10" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="27">
         <f ca="1">IF(OFFSET(A28,-1,0) ="",OFFSET(A28,-2,0)+1,OFFSET(A28,-1,0)+1 )</f>
         <v>23</v>
       </c>
-      <c r="B28" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="C28" s="29" t="s">
-        <v>301</v>
+      <c r="B28" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>258</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>292</v>
+        <v>259</v>
       </c>
       <c r="E28" s="32"/>
       <c r="F28" s="13"/>
@@ -15481,41 +15845,39 @@
       <c r="H28" s="13"/>
       <c r="I28" s="32"/>
     </row>
-    <row r="29" spans="1:26" s="10" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" s="10" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">IF(OFFSET(A29,-1,0) ="",OFFSET(A29,-2,0)+1,OFFSET(A29,-1,0)+1 )</f>
         <v>24</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>302</v>
+        <v>361</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>296</v>
-      </c>
-      <c r="E29" s="32" t="s">
-        <v>293</v>
-      </c>
+        <v>366</v>
+      </c>
+      <c r="E29" s="32"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
       <c r="I29" s="32"/>
     </row>
-    <row r="30" spans="1:26" s="10" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" s="10" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>25</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>300</v>
+        <v>362</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>305</v>
+        <v>366</v>
       </c>
       <c r="E30" s="32"/>
       <c r="F30" s="13"/>
@@ -15523,19 +15885,19 @@
       <c r="H30" s="13"/>
       <c r="I30" s="32"/>
     </row>
-    <row r="31" spans="1:26" s="10" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" s="10" customFormat="1" ht="84.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>26</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>212</v>
+        <v>130</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>306</v>
+        <v>363</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>307</v>
+        <v>366</v>
       </c>
       <c r="E31" s="32"/>
       <c r="F31" s="13"/>
@@ -15543,19 +15905,19 @@
       <c r="H31" s="13"/>
       <c r="I31" s="32"/>
     </row>
-    <row r="32" spans="1:26" s="10" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" s="10" customFormat="1" ht="81.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>27</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>308</v>
+        <v>364</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>307</v>
+        <v>367</v>
       </c>
       <c r="E32" s="32"/>
       <c r="F32" s="13"/>
@@ -15563,19 +15925,19 @@
       <c r="H32" s="13"/>
       <c r="I32" s="32"/>
     </row>
-    <row r="33" spans="1:9" s="10" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" s="10" customFormat="1" ht="53" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>28</v>
       </c>
       <c r="B33" s="29" t="s">
-        <v>131</v>
+        <v>209</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>319</v>
+        <v>365</v>
       </c>
       <c r="D33" s="30" t="s">
-        <v>320</v>
+        <v>368</v>
       </c>
       <c r="E33" s="32"/>
       <c r="F33" s="13"/>
@@ -15583,19 +15945,19 @@
       <c r="H33" s="13"/>
       <c r="I33" s="32"/>
     </row>
-    <row r="34" spans="1:9" s="10" customFormat="1" ht="42.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" s="10" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>29</v>
       </c>
       <c r="B34" s="29" t="s">
-        <v>167</v>
+        <v>131</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>321</v>
+        <v>369</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>320</v>
+        <v>366</v>
       </c>
       <c r="E34" s="32"/>
       <c r="F34" s="13"/>
@@ -15603,19 +15965,19 @@
       <c r="H34" s="13"/>
       <c r="I34" s="32"/>
     </row>
-    <row r="35" spans="1:9" s="10" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" s="10" customFormat="1" ht="42.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>30</v>
       </c>
       <c r="B35" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>311</v>
+        <v>370</v>
       </c>
       <c r="D35" s="30" t="s">
-        <v>309</v>
+        <v>366</v>
       </c>
       <c r="E35" s="32"/>
       <c r="F35" s="13"/>
@@ -15623,19 +15985,19 @@
       <c r="H35" s="13"/>
       <c r="I35" s="32"/>
     </row>
-    <row r="36" spans="1:9" s="10" customFormat="1" ht="77" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" s="10" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>31</v>
       </c>
       <c r="B36" s="29" t="s">
-        <v>192</v>
+        <v>167</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>310</v>
+        <v>371</v>
       </c>
       <c r="D36" s="30" t="s">
-        <v>309</v>
+        <v>366</v>
       </c>
       <c r="E36" s="32"/>
       <c r="F36" s="13"/>
@@ -15643,19 +16005,19 @@
       <c r="H36" s="13"/>
       <c r="I36" s="32"/>
     </row>
-    <row r="37" spans="1:9" s="10" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" s="10" customFormat="1" ht="77" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>32</v>
       </c>
       <c r="B37" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="C37" s="30" t="s">
-        <v>315</v>
+        <v>191</v>
+      </c>
+      <c r="C37" s="29" t="s">
+        <v>372</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>316</v>
+        <v>366</v>
       </c>
       <c r="E37" s="32"/>
       <c r="F37" s="13"/>
@@ -15663,19 +16025,19 @@
       <c r="H37" s="13"/>
       <c r="I37" s="32"/>
     </row>
-    <row r="38" spans="1:9" s="10" customFormat="1" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" s="10" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>33</v>
       </c>
       <c r="B38" s="29" t="s">
-        <v>194</v>
+        <v>379</v>
       </c>
       <c r="C38" s="30" t="s">
-        <v>317</v>
+        <v>373</v>
       </c>
       <c r="D38" s="30" t="s">
-        <v>309</v>
+        <v>272</v>
       </c>
       <c r="E38" s="32"/>
       <c r="F38" s="13"/>
@@ -15683,19 +16045,19 @@
       <c r="H38" s="13"/>
       <c r="I38" s="32"/>
     </row>
-    <row r="39" spans="1:9" s="10" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" s="10" customFormat="1" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>34</v>
       </c>
       <c r="B39" s="29" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C39" s="30" t="s">
-        <v>318</v>
+        <v>374</v>
       </c>
       <c r="D39" s="30" t="s">
-        <v>312</v>
+        <v>366</v>
       </c>
       <c r="E39" s="32"/>
       <c r="F39" s="13"/>
@@ -15703,19 +16065,19 @@
       <c r="H39" s="13"/>
       <c r="I39" s="32"/>
     </row>
-    <row r="40" spans="1:9" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" s="10" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>35</v>
       </c>
       <c r="B40" s="29" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="C40" s="30" t="s">
-        <v>313</v>
+        <v>375</v>
       </c>
       <c r="D40" s="30" t="s">
-        <v>312</v>
+        <v>366</v>
       </c>
       <c r="E40" s="32"/>
       <c r="F40" s="13"/>
@@ -15723,98 +16085,120 @@
       <c r="H40" s="13"/>
       <c r="I40" s="32"/>
     </row>
-    <row r="41" spans="1:9" s="10" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" s="10" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>36</v>
       </c>
       <c r="B41" s="29" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="C41" s="30" t="s">
-        <v>314</v>
-      </c>
-      <c r="D41" s="30"/>
+        <v>376</v>
+      </c>
+      <c r="D41" s="30" t="s">
+        <v>272</v>
+      </c>
       <c r="E41" s="32"/>
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
       <c r="I41" s="32"/>
     </row>
-    <row r="42" spans="1:9" s="10" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" s="10" customFormat="1" ht="64" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>37</v>
       </c>
       <c r="B42" s="29" t="s">
-        <v>227</v>
-      </c>
-      <c r="C42" s="30"/>
-      <c r="D42" s="30"/>
+        <v>221</v>
+      </c>
+      <c r="C42" s="30" t="s">
+        <v>377</v>
+      </c>
+      <c r="D42" s="30" t="s">
+        <v>272</v>
+      </c>
       <c r="E42" s="32"/>
       <c r="F42" s="13"/>
       <c r="G42" s="13"/>
       <c r="H42" s="13"/>
       <c r="I42" s="32"/>
     </row>
-    <row r="43" spans="1:9" s="10" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" s="10" customFormat="1" ht="59.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>38</v>
       </c>
       <c r="B43" s="29" t="s">
-        <v>224</v>
-      </c>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30"/>
+        <v>222</v>
+      </c>
+      <c r="C43" s="30" t="s">
+        <v>378</v>
+      </c>
+      <c r="D43" s="30" t="s">
+        <v>272</v>
+      </c>
       <c r="E43" s="32"/>
       <c r="F43" s="13"/>
       <c r="G43" s="13"/>
       <c r="H43" s="13"/>
       <c r="I43" s="32"/>
     </row>
-    <row r="44" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" s="10" customFormat="1" ht="66.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>39</v>
       </c>
       <c r="B44" s="29" t="s">
-        <v>225</v>
-      </c>
-      <c r="C44" s="30"/>
-      <c r="D44" s="30"/>
+        <v>220</v>
+      </c>
+      <c r="C44" s="30" t="s">
+        <v>380</v>
+      </c>
+      <c r="D44" s="30" t="s">
+        <v>303</v>
+      </c>
       <c r="E44" s="32"/>
       <c r="F44" s="13"/>
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
       <c r="I44" s="32"/>
     </row>
-    <row r="45" spans="1:9" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>40</v>
       </c>
       <c r="B45" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="C45" s="30"/>
-      <c r="D45" s="30"/>
+        <v>137</v>
+      </c>
+      <c r="C45" s="30" t="s">
+        <v>263</v>
+      </c>
+      <c r="D45" s="30" t="s">
+        <v>381</v>
+      </c>
       <c r="E45" s="32"/>
       <c r="F45" s="13"/>
       <c r="G45" s="13"/>
       <c r="H45" s="13"/>
       <c r="I45" s="32"/>
     </row>
-    <row r="46" spans="1:9" s="10" customFormat="1" ht="24.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>41</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="C46" s="30"/>
-      <c r="D46" s="30"/>
+        <v>138</v>
+      </c>
+      <c r="C46" s="30" t="s">
+        <v>264</v>
+      </c>
+      <c r="D46" s="30" t="s">
+        <v>238</v>
+      </c>
       <c r="E46" s="32"/>
       <c r="F46" s="13"/>
       <c r="G46" s="13"/>
@@ -15823,7 +16207,7 @@
     </row>
     <row r="47" spans="1:9" s="10" customFormat="1" ht="21.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="45" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B47" s="46"/>
       <c r="C47" s="46"/>
@@ -15834,16 +16218,20 @@
       <c r="H47" s="46"/>
       <c r="I47" s="46"/>
     </row>
-    <row r="48" spans="1:9" s="10" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" s="10" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="27">
         <f ca="1">IF(OFFSET(A48,-2,0) ="",OFFSET(A48,-2,0)+1,OFFSET(A48,-2,0)+1 )</f>
         <v>42</v>
       </c>
       <c r="B48" s="30" t="s">
-        <v>140</v>
-      </c>
-      <c r="C48" s="30"/>
-      <c r="D48" s="30"/>
+        <v>139</v>
+      </c>
+      <c r="C48" s="30" t="s">
+        <v>265</v>
+      </c>
+      <c r="D48" s="30" t="s">
+        <v>266</v>
+      </c>
       <c r="E48" s="32"/>
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
@@ -15856,220 +16244,274 @@
         <v>43</v>
       </c>
       <c r="B49" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
+        <v>141</v>
+      </c>
+      <c r="C49" s="30" t="s">
+        <v>267</v>
+      </c>
+      <c r="D49" s="30" t="s">
+        <v>382</v>
+      </c>
       <c r="E49" s="32"/>
       <c r="F49" s="13"/>
       <c r="G49" s="13"/>
       <c r="H49" s="13"/>
       <c r="I49" s="32"/>
     </row>
-    <row r="50" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" s="10" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>44</v>
       </c>
       <c r="B50" s="30" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C50" s="30" t="s">
-        <v>228</v>
-      </c>
-      <c r="D50" s="30"/>
-      <c r="E50" s="32"/>
+        <v>383</v>
+      </c>
+      <c r="D50" s="30" t="s">
+        <v>384</v>
+      </c>
+      <c r="E50" s="30"/>
       <c r="F50" s="13"/>
       <c r="G50" s="13"/>
       <c r="H50" s="13"/>
       <c r="I50" s="32"/>
     </row>
-    <row r="51" spans="1:9" s="10" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" s="10" customFormat="1" ht="68.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>45</v>
       </c>
       <c r="B51" s="30" t="s">
-        <v>198</v>
-      </c>
-      <c r="C51" s="30"/>
-      <c r="D51" s="30"/>
+        <v>196</v>
+      </c>
+      <c r="C51" s="30" t="s">
+        <v>385</v>
+      </c>
+      <c r="D51" s="30" t="s">
+        <v>386</v>
+      </c>
       <c r="E51" s="32"/>
       <c r="F51" s="13"/>
       <c r="G51" s="13"/>
       <c r="H51" s="13"/>
       <c r="I51" s="32"/>
     </row>
-    <row r="52" spans="1:9" s="10" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" s="10" customFormat="1" ht="53.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>46</v>
       </c>
       <c r="B52" s="30" t="s">
-        <v>199</v>
-      </c>
-      <c r="C52" s="30"/>
-      <c r="D52" s="30"/>
+        <v>197</v>
+      </c>
+      <c r="C52" s="30" t="s">
+        <v>268</v>
+      </c>
+      <c r="D52" s="30" t="s">
+        <v>390</v>
+      </c>
       <c r="E52" s="32"/>
       <c r="F52" s="13"/>
       <c r="G52" s="13"/>
       <c r="H52" s="13"/>
       <c r="I52" s="32"/>
     </row>
-    <row r="53" spans="1:9" s="10" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" s="10" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>47</v>
       </c>
       <c r="B53" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="C53" s="30"/>
-      <c r="D53" s="30"/>
+        <v>142</v>
+      </c>
+      <c r="C53" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="D53" s="30" t="s">
+        <v>270</v>
+      </c>
       <c r="E53" s="32"/>
       <c r="F53" s="13"/>
       <c r="G53" s="13"/>
       <c r="H53" s="13"/>
       <c r="I53" s="32"/>
     </row>
-    <row r="54" spans="1:9" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" s="10" customFormat="1" ht="44.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>48</v>
       </c>
       <c r="B54" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="C54" s="30"/>
-      <c r="D54" s="30"/>
+        <v>143</v>
+      </c>
+      <c r="C54" s="29" t="s">
+        <v>271</v>
+      </c>
+      <c r="D54" s="30" t="s">
+        <v>272</v>
+      </c>
       <c r="E54" s="32"/>
       <c r="F54" s="13"/>
       <c r="G54" s="13"/>
       <c r="H54" s="13"/>
       <c r="I54" s="32"/>
     </row>
-    <row r="55" spans="1:9" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" s="10" customFormat="1" ht="44.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>49</v>
       </c>
       <c r="B55" s="30" t="s">
-        <v>145</v>
-      </c>
-      <c r="C55" s="30"/>
-      <c r="D55" s="30"/>
+        <v>144</v>
+      </c>
+      <c r="C55" s="29" t="s">
+        <v>273</v>
+      </c>
+      <c r="D55" s="30" t="s">
+        <v>272</v>
+      </c>
       <c r="E55" s="32"/>
       <c r="F55" s="13"/>
       <c r="G55" s="13"/>
       <c r="H55" s="13"/>
       <c r="I55" s="32"/>
     </row>
-    <row r="56" spans="1:9" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" s="10" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>50</v>
       </c>
       <c r="B56" s="30" t="s">
-        <v>200</v>
-      </c>
-      <c r="C56" s="30"/>
-      <c r="D56" s="30"/>
+        <v>198</v>
+      </c>
+      <c r="C56" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="D56" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="E56" s="32"/>
       <c r="F56" s="13"/>
       <c r="G56" s="13"/>
       <c r="H56" s="13"/>
       <c r="I56" s="32"/>
     </row>
-    <row r="57" spans="1:9" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" s="10" customFormat="1" ht="38.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>51</v>
       </c>
       <c r="B57" s="30" t="s">
-        <v>201</v>
-      </c>
-      <c r="C57" s="30"/>
-      <c r="D57" s="30"/>
+        <v>199</v>
+      </c>
+      <c r="C57" s="29" t="s">
+        <v>276</v>
+      </c>
+      <c r="D57" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="E57" s="32"/>
       <c r="F57" s="13"/>
       <c r="G57" s="13"/>
       <c r="H57" s="13"/>
       <c r="I57" s="32"/>
     </row>
-    <row r="58" spans="1:9" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" s="10" customFormat="1" ht="45.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>52</v>
       </c>
       <c r="B58" s="30" t="s">
-        <v>202</v>
-      </c>
-      <c r="C58" s="30"/>
-      <c r="D58" s="30"/>
+        <v>200</v>
+      </c>
+      <c r="C58" s="29" t="s">
+        <v>277</v>
+      </c>
+      <c r="D58" s="30" t="s">
+        <v>275</v>
+      </c>
       <c r="E58" s="32"/>
       <c r="F58" s="13"/>
       <c r="G58" s="13"/>
       <c r="H58" s="13"/>
       <c r="I58" s="32"/>
     </row>
-    <row r="59" spans="1:9" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" s="10" customFormat="1" ht="53.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>53</v>
       </c>
       <c r="B59" s="30" t="s">
-        <v>203</v>
-      </c>
-      <c r="C59" s="30"/>
-      <c r="D59" s="30"/>
+        <v>201</v>
+      </c>
+      <c r="C59" s="29" t="s">
+        <v>278</v>
+      </c>
+      <c r="D59" s="30" t="s">
+        <v>280</v>
+      </c>
       <c r="E59" s="32"/>
       <c r="F59" s="13"/>
       <c r="G59" s="13"/>
       <c r="H59" s="13"/>
       <c r="I59" s="32"/>
     </row>
-    <row r="60" spans="1:9" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" s="10" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>54</v>
       </c>
       <c r="B60" s="30" t="s">
-        <v>204</v>
-      </c>
-      <c r="C60" s="30"/>
-      <c r="D60" s="30"/>
+        <v>202</v>
+      </c>
+      <c r="C60" s="29" t="s">
+        <v>279</v>
+      </c>
+      <c r="D60" s="30" t="s">
+        <v>280</v>
+      </c>
       <c r="E60" s="32"/>
       <c r="F60" s="13"/>
       <c r="G60" s="13"/>
       <c r="H60" s="13"/>
       <c r="I60" s="32"/>
     </row>
-    <row r="61" spans="1:9" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" s="10" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>55</v>
       </c>
       <c r="B61" s="30" t="s">
-        <v>205</v>
-      </c>
-      <c r="C61" s="30"/>
-      <c r="D61" s="30"/>
+        <v>203</v>
+      </c>
+      <c r="C61" s="29" t="s">
+        <v>281</v>
+      </c>
+      <c r="D61" s="30" t="s">
+        <v>280</v>
+      </c>
       <c r="E61" s="32"/>
       <c r="F61" s="13"/>
       <c r="G61" s="13"/>
       <c r="H61" s="13"/>
       <c r="I61" s="32"/>
     </row>
-    <row r="62" spans="1:9" s="10" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" s="10" customFormat="1" ht="71.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>56</v>
       </c>
       <c r="B62" s="30" t="s">
-        <v>230</v>
-      </c>
-      <c r="C62" s="30"/>
-      <c r="D62" s="30"/>
+        <v>224</v>
+      </c>
+      <c r="C62" s="29" t="s">
+        <v>282</v>
+      </c>
+      <c r="D62" s="30" t="s">
+        <v>283</v>
+      </c>
       <c r="E62" s="32"/>
       <c r="F62" s="13"/>
       <c r="G62" s="13"/>
@@ -16082,10 +16524,14 @@
         <v>57</v>
       </c>
       <c r="B63" s="30" t="s">
-        <v>229</v>
-      </c>
-      <c r="C63" s="30"/>
-      <c r="D63" s="30"/>
+        <v>223</v>
+      </c>
+      <c r="C63" s="30" t="s">
+        <v>284</v>
+      </c>
+      <c r="D63" s="30" t="s">
+        <v>285</v>
+      </c>
       <c r="E63" s="32"/>
       <c r="F63" s="13"/>
       <c r="G63" s="13"/>
@@ -16094,7 +16540,7 @@
     </row>
     <row r="64" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="45" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B64" s="46"/>
       <c r="C64" s="46"/>
@@ -16111,10 +16557,14 @@
         <v>58</v>
       </c>
       <c r="B65" s="30" t="s">
-        <v>140</v>
-      </c>
-      <c r="C65" s="30"/>
-      <c r="D65" s="30"/>
+        <v>139</v>
+      </c>
+      <c r="C65" s="30" t="s">
+        <v>286</v>
+      </c>
+      <c r="D65" s="30" t="s">
+        <v>287</v>
+      </c>
       <c r="E65" s="32"/>
       <c r="F65" s="13"/>
       <c r="G65" s="13"/>
@@ -16127,58 +16577,74 @@
         <v>59</v>
       </c>
       <c r="B66" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="C66" s="30"/>
-      <c r="D66" s="30"/>
+        <v>141</v>
+      </c>
+      <c r="C66" s="30" t="s">
+        <v>288</v>
+      </c>
+      <c r="D66" s="30" t="s">
+        <v>382</v>
+      </c>
       <c r="E66" s="32"/>
       <c r="F66" s="13"/>
       <c r="G66" s="13"/>
       <c r="H66" s="13"/>
       <c r="I66" s="32"/>
     </row>
-    <row r="67" spans="1:9" s="10" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" s="10" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>60</v>
       </c>
       <c r="B67" s="30" t="s">
-        <v>187</v>
-      </c>
-      <c r="C67" s="30"/>
-      <c r="D67" s="30"/>
+        <v>186</v>
+      </c>
+      <c r="C67" s="30" t="s">
+        <v>289</v>
+      </c>
+      <c r="D67" s="30" t="s">
+        <v>391</v>
+      </c>
       <c r="E67" s="32"/>
       <c r="F67" s="13"/>
       <c r="G67" s="13"/>
       <c r="H67" s="13"/>
       <c r="I67" s="32"/>
     </row>
-    <row r="68" spans="1:9" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" s="10" customFormat="1" ht="50" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>61</v>
       </c>
       <c r="B68" s="30" t="s">
-        <v>146</v>
-      </c>
-      <c r="C68" s="30"/>
-      <c r="D68" s="30"/>
+        <v>145</v>
+      </c>
+      <c r="C68" s="29" t="s">
+        <v>290</v>
+      </c>
+      <c r="D68" s="30" t="s">
+        <v>272</v>
+      </c>
       <c r="E68" s="32"/>
       <c r="F68" s="13"/>
       <c r="G68" s="13"/>
       <c r="H68" s="13"/>
       <c r="I68" s="32"/>
     </row>
-    <row r="69" spans="1:9" s="10" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" s="10" customFormat="1" ht="47.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>62</v>
       </c>
       <c r="B69" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="C69" s="30"/>
-      <c r="D69" s="30"/>
+        <v>146</v>
+      </c>
+      <c r="C69" s="29" t="s">
+        <v>291</v>
+      </c>
+      <c r="D69" s="30" t="s">
+        <v>272</v>
+      </c>
       <c r="E69" s="32"/>
       <c r="F69" s="13"/>
       <c r="G69" s="13"/>
@@ -16187,7 +16653,7 @@
     </row>
     <row r="70" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="45" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B70" s="46"/>
       <c r="C70" s="46"/>
@@ -16204,129 +16670,161 @@
         <v>63</v>
       </c>
       <c r="B71" s="30" t="s">
-        <v>140</v>
-      </c>
-      <c r="C71" s="30"/>
-      <c r="D71" s="30"/>
+        <v>139</v>
+      </c>
+      <c r="C71" s="30" t="s">
+        <v>292</v>
+      </c>
+      <c r="D71" s="30" t="s">
+        <v>293</v>
+      </c>
       <c r="E71" s="32"/>
       <c r="F71" s="13"/>
       <c r="G71" s="13"/>
       <c r="H71" s="13"/>
       <c r="I71" s="32"/>
     </row>
-    <row r="72" spans="1:9" s="10" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>64</v>
       </c>
       <c r="B72" s="30" t="s">
-        <v>208</v>
-      </c>
-      <c r="C72" s="30"/>
-      <c r="D72" s="30"/>
+        <v>205</v>
+      </c>
+      <c r="C72" s="29" t="s">
+        <v>262</v>
+      </c>
+      <c r="D72" s="30" t="s">
+        <v>322</v>
+      </c>
       <c r="E72" s="32"/>
       <c r="F72" s="13"/>
       <c r="G72" s="13"/>
       <c r="H72" s="13"/>
       <c r="I72" s="32"/>
     </row>
-    <row r="73" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" s="10" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>65</v>
       </c>
       <c r="B73" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="C73" s="30"/>
-      <c r="D73" s="30"/>
+        <v>149</v>
+      </c>
+      <c r="C73" s="30" t="s">
+        <v>295</v>
+      </c>
+      <c r="D73" s="30" t="s">
+        <v>272</v>
+      </c>
       <c r="E73" s="32"/>
       <c r="F73" s="13"/>
       <c r="G73" s="13"/>
       <c r="H73" s="13"/>
       <c r="I73" s="32"/>
     </row>
-    <row r="74" spans="1:9" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" s="10" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>66</v>
       </c>
       <c r="B74" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="C74" s="30"/>
-      <c r="D74" s="30"/>
+        <v>150</v>
+      </c>
+      <c r="C74" s="30" t="s">
+        <v>294</v>
+      </c>
+      <c r="D74" s="30" t="s">
+        <v>272</v>
+      </c>
       <c r="E74" s="32"/>
       <c r="F74" s="13"/>
       <c r="G74" s="13"/>
       <c r="H74" s="13"/>
       <c r="I74" s="32"/>
     </row>
-    <row r="75" spans="1:9" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" s="10" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>67</v>
       </c>
       <c r="B75" s="29" t="s">
-        <v>210</v>
-      </c>
-      <c r="C75" s="30"/>
-      <c r="D75" s="30"/>
+        <v>207</v>
+      </c>
+      <c r="C75" s="30" t="s">
+        <v>296</v>
+      </c>
+      <c r="D75" s="30" t="s">
+        <v>272</v>
+      </c>
       <c r="E75" s="32"/>
       <c r="F75" s="13"/>
       <c r="G75" s="13"/>
       <c r="H75" s="13"/>
       <c r="I75" s="32"/>
     </row>
-    <row r="76" spans="1:9" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" s="10" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>68</v>
       </c>
       <c r="B76" s="29" t="s">
-        <v>231</v>
-      </c>
-      <c r="C76" s="30"/>
-      <c r="D76" s="30"/>
+        <v>225</v>
+      </c>
+      <c r="C76" s="30" t="s">
+        <v>297</v>
+      </c>
+      <c r="D76" s="30" t="s">
+        <v>298</v>
+      </c>
       <c r="E76" s="32"/>
       <c r="F76" s="13"/>
       <c r="G76" s="13"/>
       <c r="H76" s="13"/>
       <c r="I76" s="32"/>
     </row>
-    <row r="77" spans="1:9" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" s="10" customFormat="1" ht="83" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>69</v>
       </c>
       <c r="B77" s="29" t="s">
-        <v>232</v>
-      </c>
-      <c r="C77" s="30"/>
-      <c r="D77" s="30"/>
+        <v>226</v>
+      </c>
+      <c r="C77" s="30" t="s">
+        <v>299</v>
+      </c>
+      <c r="D77" s="30" t="s">
+        <v>298</v>
+      </c>
       <c r="E77" s="32"/>
       <c r="F77" s="13"/>
       <c r="G77" s="13"/>
       <c r="H77" s="13"/>
       <c r="I77" s="32"/>
     </row>
-    <row r="78" spans="1:9" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" s="10" customFormat="1" ht="83" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>70</v>
       </c>
       <c r="B78" s="29" t="s">
-        <v>233</v>
-      </c>
-      <c r="C78" s="30"/>
-      <c r="D78" s="30"/>
+        <v>227</v>
+      </c>
+      <c r="C78" s="30" t="s">
+        <v>299</v>
+      </c>
+      <c r="D78" s="30" t="s">
+        <v>298</v>
+      </c>
       <c r="E78" s="32"/>
       <c r="F78" s="13"/>
       <c r="G78" s="13"/>
       <c r="H78" s="13"/>
       <c r="I78" s="32"/>
     </row>
-    <row r="79" spans="1:9" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" s="10" customFormat="1" ht="62.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>71</v>
@@ -16334,72 +16832,92 @@
       <c r="B79" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="C79" s="30"/>
-      <c r="D79" s="30"/>
+      <c r="C79" s="30" t="s">
+        <v>300</v>
+      </c>
+      <c r="D79" s="30" t="s">
+        <v>298</v>
+      </c>
       <c r="E79" s="32"/>
       <c r="F79" s="13"/>
       <c r="G79" s="13"/>
       <c r="H79" s="13"/>
       <c r="I79" s="32"/>
     </row>
-    <row r="80" spans="1:9" s="10" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" s="10" customFormat="1" ht="63.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>72</v>
       </c>
       <c r="B80" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="C80" s="30"/>
-      <c r="D80" s="30"/>
+        <v>151</v>
+      </c>
+      <c r="C80" s="30" t="s">
+        <v>294</v>
+      </c>
+      <c r="D80" s="30" t="s">
+        <v>272</v>
+      </c>
       <c r="E80" s="32"/>
       <c r="F80" s="13"/>
       <c r="G80" s="13"/>
       <c r="H80" s="13"/>
       <c r="I80" s="32"/>
     </row>
-    <row r="81" spans="1:9" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" s="10" customFormat="1" ht="56.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>73</v>
       </c>
       <c r="B81" s="30" t="s">
-        <v>153</v>
-      </c>
-      <c r="C81" s="30"/>
-      <c r="D81" s="30"/>
+        <v>152</v>
+      </c>
+      <c r="C81" s="30" t="s">
+        <v>301</v>
+      </c>
+      <c r="D81" s="30" t="s">
+        <v>272</v>
+      </c>
       <c r="E81" s="32"/>
       <c r="F81" s="13"/>
       <c r="G81" s="13"/>
       <c r="H81" s="13"/>
       <c r="I81" s="32"/>
     </row>
-    <row r="82" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" s="10" customFormat="1" ht="78.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="27">
         <f ca="1">IF(OFFSET(A82,-1,0) ="",OFFSET(A82,-2,0)+1,OFFSET(A82,-1,0)+1 )</f>
         <v>74</v>
       </c>
       <c r="B82" s="29" t="s">
-        <v>234</v>
-      </c>
-      <c r="C82" s="29"/>
-      <c r="D82" s="30"/>
+        <v>228</v>
+      </c>
+      <c r="C82" s="30" t="s">
+        <v>302</v>
+      </c>
+      <c r="D82" s="30" t="s">
+        <v>303</v>
+      </c>
       <c r="E82" s="32"/>
       <c r="F82" s="13"/>
       <c r="G82" s="13"/>
       <c r="H82" s="13"/>
       <c r="I82" s="32"/>
     </row>
-    <row r="83" spans="1:9" s="10" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" s="10" customFormat="1" ht="61" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>75</v>
       </c>
       <c r="B83" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="C83" s="30"/>
-      <c r="D83" s="30"/>
+        <v>138</v>
+      </c>
+      <c r="C83" s="30" t="s">
+        <v>304</v>
+      </c>
+      <c r="D83" s="30" t="s">
+        <v>305</v>
+      </c>
       <c r="E83" s="32"/>
       <c r="F83" s="13"/>
       <c r="G83" s="13"/>
@@ -16408,20 +16926,20 @@
     </row>
     <row r="84" spans="1:9" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="38" t="s">
-        <v>160</v>
-      </c>
-      <c r="B84" s="50"/>
-      <c r="C84" s="50"/>
-      <c r="D84" s="50"/>
-      <c r="E84" s="50"/>
-      <c r="F84" s="50"/>
-      <c r="G84" s="50"/>
-      <c r="H84" s="50"/>
-      <c r="I84" s="50"/>
+        <v>159</v>
+      </c>
+      <c r="B84" s="47"/>
+      <c r="C84" s="47"/>
+      <c r="D84" s="47"/>
+      <c r="E84" s="47"/>
+      <c r="F84" s="47"/>
+      <c r="G84" s="47"/>
+      <c r="H84" s="47"/>
+      <c r="I84" s="47"/>
     </row>
     <row r="85" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="45" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B85" s="46"/>
       <c r="C85" s="46"/>
@@ -16432,114 +16950,140 @@
       <c r="H85" s="46"/>
       <c r="I85" s="46"/>
     </row>
-    <row r="86" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" s="10" customFormat="1" ht="98" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="27">
         <f ca="1">IF(OFFSET(A86,-3,0) ="",OFFSET(A86,-3,0)+1,OFFSET(A86,-3,0)+1 )</f>
         <v>76</v>
       </c>
       <c r="B86" s="30" t="s">
-        <v>235</v>
-      </c>
-      <c r="C86" s="30"/>
-      <c r="D86" s="30"/>
+        <v>229</v>
+      </c>
+      <c r="C86" s="30" t="s">
+        <v>312</v>
+      </c>
+      <c r="D86" s="30" t="s">
+        <v>306</v>
+      </c>
       <c r="E86" s="32"/>
       <c r="F86" s="13"/>
       <c r="G86" s="13"/>
       <c r="H86" s="13"/>
       <c r="I86" s="32"/>
     </row>
-    <row r="87" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" s="10" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="27">
         <f t="shared" ref="A87:A99" ca="1" si="1">IF(OFFSET(A87,-1,0) ="",OFFSET(A87,-2,0)+1,OFFSET(A87,-1,0)+1 )</f>
         <v>77</v>
       </c>
       <c r="B87" s="30" t="s">
-        <v>238</v>
-      </c>
-      <c r="C87" s="30"/>
-      <c r="D87" s="30"/>
+        <v>232</v>
+      </c>
+      <c r="C87" s="30" t="s">
+        <v>313</v>
+      </c>
+      <c r="D87" s="30" t="s">
+        <v>307</v>
+      </c>
       <c r="E87" s="32"/>
       <c r="F87" s="13"/>
       <c r="G87" s="13"/>
       <c r="H87" s="13"/>
       <c r="I87" s="32"/>
     </row>
-    <row r="88" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" s="10" customFormat="1" ht="54.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="27">
         <f t="shared" ca="1" si="1"/>
         <v>78</v>
       </c>
       <c r="B88" s="30" t="s">
-        <v>237</v>
-      </c>
-      <c r="C88" s="30"/>
-      <c r="D88" s="30"/>
+        <v>231</v>
+      </c>
+      <c r="C88" s="30" t="s">
+        <v>308</v>
+      </c>
+      <c r="D88" s="30" t="s">
+        <v>319</v>
+      </c>
       <c r="E88" s="32"/>
       <c r="F88" s="13"/>
       <c r="G88" s="13"/>
       <c r="H88" s="13"/>
       <c r="I88" s="32"/>
     </row>
-    <row r="89" spans="1:9" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" s="10" customFormat="1" ht="65.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="27">
         <f t="shared" ca="1" si="1"/>
         <v>79</v>
       </c>
       <c r="B89" s="30" t="s">
-        <v>236</v>
-      </c>
-      <c r="C89" s="30"/>
-      <c r="D89" s="30"/>
+        <v>230</v>
+      </c>
+      <c r="C89" s="30" t="s">
+        <v>309</v>
+      </c>
+      <c r="D89" s="30" t="s">
+        <v>310</v>
+      </c>
       <c r="E89" s="32"/>
       <c r="F89" s="13"/>
       <c r="G89" s="13"/>
       <c r="H89" s="13"/>
       <c r="I89" s="32"/>
     </row>
-    <row r="90" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" s="10" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="27">
         <f t="shared" ca="1" si="1"/>
         <v>80</v>
       </c>
       <c r="B90" s="30" t="s">
-        <v>190</v>
+        <v>311</v>
       </c>
       <c r="C90" s="30" t="s">
-        <v>170</v>
-      </c>
-      <c r="D90" s="30"/>
+        <v>314</v>
+      </c>
+      <c r="D90" s="30" t="s">
+        <v>392</v>
+      </c>
       <c r="E90" s="32"/>
       <c r="F90" s="13"/>
       <c r="G90" s="13"/>
       <c r="H90" s="13"/>
       <c r="I90" s="32"/>
     </row>
-    <row r="91" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" s="10" customFormat="1" ht="63.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="27">
         <f t="shared" ca="1" si="1"/>
         <v>81</v>
       </c>
       <c r="B91" s="30" t="s">
-        <v>239</v>
-      </c>
-      <c r="C91" s="30"/>
-      <c r="D91" s="30"/>
+        <v>233</v>
+      </c>
+      <c r="C91" s="30" t="s">
+        <v>316</v>
+      </c>
+      <c r="D91" s="30" t="s">
+        <v>318</v>
+      </c>
       <c r="E91" s="32"/>
       <c r="F91" s="13"/>
       <c r="G91" s="13"/>
       <c r="H91" s="13"/>
       <c r="I91" s="32"/>
     </row>
-    <row r="92" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" s="10" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="27">
         <f t="shared" ca="1" si="1"/>
         <v>82</v>
       </c>
       <c r="B92" s="30" t="s">
-        <v>240</v>
-      </c>
-      <c r="C92" s="30"/>
-      <c r="D92" s="30"/>
+        <v>234</v>
+      </c>
+      <c r="C92" s="30" t="s">
+        <v>317</v>
+      </c>
+      <c r="D92" s="30" t="s">
+        <v>320</v>
+      </c>
       <c r="E92" s="32"/>
       <c r="F92" s="13"/>
       <c r="G92" s="13"/>
@@ -16552,10 +17096,14 @@
         <v>83</v>
       </c>
       <c r="B93" s="30" t="s">
-        <v>179</v>
-      </c>
-      <c r="C93" s="30"/>
-      <c r="D93" s="30"/>
+        <v>178</v>
+      </c>
+      <c r="C93" s="30" t="s">
+        <v>323</v>
+      </c>
+      <c r="D93" s="30" t="s">
+        <v>325</v>
+      </c>
       <c r="E93" s="32"/>
       <c r="F93" s="13"/>
       <c r="G93" s="13"/>
@@ -16568,10 +17116,14 @@
         <v>84</v>
       </c>
       <c r="B94" s="30" t="s">
-        <v>180</v>
-      </c>
-      <c r="C94" s="30"/>
-      <c r="D94" s="30"/>
+        <v>179</v>
+      </c>
+      <c r="C94" s="30" t="s">
+        <v>324</v>
+      </c>
+      <c r="D94" s="30" t="s">
+        <v>326</v>
+      </c>
       <c r="E94" s="32"/>
       <c r="F94" s="13"/>
       <c r="G94" s="13"/>
@@ -16584,10 +17136,14 @@
         <v>85</v>
       </c>
       <c r="B95" s="29" t="s">
-        <v>196</v>
-      </c>
-      <c r="C95" s="30"/>
-      <c r="D95" s="30"/>
+        <v>194</v>
+      </c>
+      <c r="C95" s="30" t="s">
+        <v>327</v>
+      </c>
+      <c r="D95" s="30" t="s">
+        <v>328</v>
+      </c>
       <c r="E95" s="32"/>
       <c r="F95" s="13"/>
       <c r="G95" s="13"/>
@@ -16600,10 +17156,14 @@
         <v>86</v>
       </c>
       <c r="B96" s="29" t="s">
-        <v>206</v>
-      </c>
-      <c r="C96" s="30"/>
-      <c r="D96" s="30"/>
+        <v>333</v>
+      </c>
+      <c r="C96" s="30" t="s">
+        <v>329</v>
+      </c>
+      <c r="D96" s="30" t="s">
+        <v>332</v>
+      </c>
       <c r="E96" s="32"/>
       <c r="F96" s="13"/>
       <c r="G96" s="13"/>
@@ -16616,10 +17176,14 @@
         <v>87</v>
       </c>
       <c r="B97" s="29" t="s">
-        <v>207</v>
-      </c>
-      <c r="C97" s="30"/>
-      <c r="D97" s="30"/>
+        <v>204</v>
+      </c>
+      <c r="C97" s="30" t="s">
+        <v>331</v>
+      </c>
+      <c r="D97" s="30" t="s">
+        <v>330</v>
+      </c>
       <c r="E97" s="32"/>
       <c r="F97" s="13"/>
       <c r="G97" s="13"/>
@@ -16632,10 +17196,14 @@
         <v>88</v>
       </c>
       <c r="B98" s="29" t="s">
-        <v>222</v>
-      </c>
-      <c r="C98" s="30"/>
-      <c r="D98" s="30"/>
+        <v>218</v>
+      </c>
+      <c r="C98" s="30" t="s">
+        <v>334</v>
+      </c>
+      <c r="D98" s="30" t="s">
+        <v>335</v>
+      </c>
       <c r="E98" s="32"/>
       <c r="F98" s="13"/>
       <c r="G98" s="13"/>
@@ -16648,10 +17216,14 @@
         <v>89</v>
       </c>
       <c r="B99" s="29" t="s">
-        <v>223</v>
-      </c>
-      <c r="C99" s="30"/>
-      <c r="D99" s="30"/>
+        <v>219</v>
+      </c>
+      <c r="C99" s="30" t="s">
+        <v>336</v>
+      </c>
+      <c r="D99" s="30" t="s">
+        <v>337</v>
+      </c>
       <c r="E99" s="32"/>
       <c r="F99" s="13"/>
       <c r="G99" s="13"/>
@@ -16659,34 +17231,34 @@
       <c r="I99" s="32"/>
     </row>
     <row r="105" spans="1:26" s="10" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="47" t="s">
-        <v>191</v>
-      </c>
-      <c r="B105" s="48"/>
-      <c r="C105" s="48"/>
-      <c r="D105" s="48"/>
-      <c r="E105" s="48"/>
-      <c r="F105" s="48"/>
-      <c r="G105" s="48"/>
-      <c r="H105" s="48"/>
-      <c r="I105" s="49"/>
+      <c r="A105" s="48" t="s">
+        <v>190</v>
+      </c>
+      <c r="B105" s="49"/>
+      <c r="C105" s="49"/>
+      <c r="D105" s="49"/>
+      <c r="E105" s="49"/>
+      <c r="F105" s="49"/>
+      <c r="G105" s="49"/>
+      <c r="H105" s="49"/>
+      <c r="I105" s="50"/>
     </row>
     <row r="106" spans="1:26" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="38" t="s">
-        <v>188</v>
-      </c>
-      <c r="B106" s="50"/>
-      <c r="C106" s="50"/>
-      <c r="D106" s="50"/>
-      <c r="E106" s="50"/>
-      <c r="F106" s="50"/>
-      <c r="G106" s="50"/>
-      <c r="H106" s="50"/>
-      <c r="I106" s="50"/>
+        <v>187</v>
+      </c>
+      <c r="B106" s="47"/>
+      <c r="C106" s="47"/>
+      <c r="D106" s="47"/>
+      <c r="E106" s="47"/>
+      <c r="F106" s="47"/>
+      <c r="G106" s="47"/>
+      <c r="H106" s="47"/>
+      <c r="I106" s="47"/>
     </row>
     <row r="107" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="45" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B107" s="46"/>
       <c r="C107" s="46"/>
@@ -16724,7 +17296,7 @@
       </c>
       <c r="C108" s="30"/>
       <c r="D108" s="30" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E108" s="32"/>
       <c r="F108" s="13"/>
@@ -16738,7 +17310,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B109" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C109" s="30"/>
       <c r="D109" s="30"/>
@@ -16754,7 +17326,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B110" s="15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C110" s="30"/>
       <c r="D110" s="30"/>
@@ -16766,7 +17338,7 @@
     </row>
     <row r="111" spans="1:26" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="45" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B111" s="46"/>
       <c r="C111" s="46"/>
@@ -16783,7 +17355,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B112" s="30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C112" s="30"/>
       <c r="D112" s="30"/>
@@ -16799,7 +17371,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B113" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C113" s="30"/>
       <c r="D113" s="30"/>
@@ -16811,7 +17383,7 @@
     </row>
     <row r="114" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="45" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B114" s="46"/>
       <c r="C114" s="46"/>
@@ -16828,7 +17400,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B115" s="30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C115" s="30"/>
       <c r="D115" s="30"/>
@@ -16840,7 +17412,7 @@
     </row>
     <row r="116" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="45" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B116" s="46"/>
       <c r="C116" s="46"/>
@@ -16857,7 +17429,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B117" s="30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C117" s="30"/>
       <c r="D117" s="30"/>
@@ -16869,7 +17441,7 @@
     </row>
     <row r="118" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="45" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B118" s="46"/>
       <c r="C118" s="46"/>
@@ -16886,7 +17458,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B119" s="30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C119" s="30"/>
       <c r="D119" s="30"/>
@@ -16902,7 +17474,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B120" s="30" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C120" s="30"/>
       <c r="D120" s="30"/>
@@ -16918,7 +17490,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B121" s="30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C121" s="30"/>
       <c r="D121" s="30"/>
@@ -16930,7 +17502,7 @@
     </row>
     <row r="122" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="45" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B122" s="46"/>
       <c r="C122" s="46"/>
@@ -16947,7 +17519,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B123" s="30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C123" s="30"/>
       <c r="D123" s="30"/>
@@ -16963,7 +17535,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B124" s="30" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C124" s="30"/>
       <c r="D124" s="30"/>
@@ -16979,7 +17551,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B125" s="30" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C125" s="30"/>
       <c r="D125" s="30"/>
@@ -16995,10 +17567,10 @@
         <v>#VALUE!</v>
       </c>
       <c r="B126" s="30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C126" s="30" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D126" s="30"/>
       <c r="E126" s="32"/>
@@ -17009,7 +17581,7 @@
     </row>
     <row r="127" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="45" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B127" s="46"/>
       <c r="C127" s="46"/>
@@ -17026,7 +17598,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B128" s="30" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C128" s="30"/>
       <c r="D128" s="30"/>
@@ -17038,7 +17610,7 @@
     </row>
     <row r="129" spans="1:26" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="45" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B129" s="46"/>
       <c r="C129" s="46"/>
@@ -17055,7 +17627,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="B130" s="30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C130" s="30"/>
       <c r="D130" s="30"/>
@@ -17067,7 +17639,7 @@
     </row>
     <row r="131" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" s="45" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B131" s="46"/>
       <c r="C131" s="46"/>
@@ -17104,10 +17676,10 @@
         <v>121</v>
       </c>
       <c r="C132" s="30" t="s">
-        <v>280</v>
+        <v>246</v>
       </c>
       <c r="D132" s="30" t="s">
-        <v>278</v>
+        <v>245</v>
       </c>
       <c r="E132" s="32"/>
       <c r="F132" s="13"/>
@@ -17121,13 +17693,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="B133" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C133" s="30" t="s">
-        <v>281</v>
+        <v>247</v>
       </c>
       <c r="D133" s="30" t="s">
-        <v>282</v>
+        <v>248</v>
       </c>
       <c r="E133" s="32"/>
       <c r="F133" s="13"/>
@@ -17141,13 +17713,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="B134" s="30" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C134" s="30" t="s">
-        <v>268</v>
+        <v>243</v>
       </c>
       <c r="D134" s="30" t="s">
-        <v>283</v>
+        <v>249</v>
       </c>
       <c r="E134" s="32"/>
       <c r="F134" s="13"/>
@@ -17161,13 +17733,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="B135" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C135" s="30" t="s">
-        <v>284</v>
+        <v>250</v>
       </c>
       <c r="D135" s="30" t="s">
-        <v>288</v>
+        <v>254</v>
       </c>
       <c r="E135" s="32"/>
       <c r="F135" s="13"/>
@@ -17181,13 +17753,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="B136" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C136" s="30" t="s">
-        <v>285</v>
+        <v>251</v>
       </c>
       <c r="D136" s="30" t="s">
-        <v>289</v>
+        <v>255</v>
       </c>
       <c r="E136" s="32"/>
       <c r="F136" s="13"/>
@@ -17201,13 +17773,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="B137" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C137" s="30" t="s">
-        <v>286</v>
+        <v>252</v>
       </c>
       <c r="D137" s="30" t="s">
-        <v>289</v>
+        <v>255</v>
       </c>
       <c r="E137" s="32"/>
       <c r="F137" s="13"/>
@@ -17221,13 +17793,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="B138" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C138" s="30" t="s">
-        <v>287</v>
+        <v>253</v>
       </c>
       <c r="D138" s="30" t="s">
-        <v>289</v>
+        <v>255</v>
       </c>
       <c r="E138" s="32"/>
       <c r="F138" s="13"/>
@@ -17241,13 +17813,13 @@
         <v>#VALUE!</v>
       </c>
       <c r="B139" s="15" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C139" s="30" t="s">
-        <v>290</v>
+        <v>256</v>
       </c>
       <c r="D139" s="30" t="s">
-        <v>288</v>
+        <v>254</v>
       </c>
       <c r="E139" s="32"/>
       <c r="F139" s="13"/>
@@ -17261,10 +17833,10 @@
         <v>#VALUE!</v>
       </c>
       <c r="B140" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C140" s="30" t="s">
-        <v>291</v>
+        <v>257</v>
       </c>
       <c r="D140" s="30"/>
       <c r="E140" s="32"/>
@@ -17968,12 +18540,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A131:I131"/>
-    <mergeCell ref="A25:I25"/>
-    <mergeCell ref="A84:I84"/>
-    <mergeCell ref="A47:I47"/>
-    <mergeCell ref="A64:I64"/>
-    <mergeCell ref="A70:I70"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A15:I15"/>
@@ -17988,6 +18554,12 @@
     <mergeCell ref="A116:I116"/>
     <mergeCell ref="A118:I118"/>
     <mergeCell ref="A111:I111"/>
+    <mergeCell ref="A131:I131"/>
+    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="A84:I84"/>
+    <mergeCell ref="A47:I47"/>
+    <mergeCell ref="A64:I64"/>
+    <mergeCell ref="A70:I70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -18046,7 +18618,7 @@
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
@@ -18059,7 +18631,7 @@
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -18072,7 +18644,7 @@
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>

</xml_diff>

<commit_message>
1st draft Assignment 3 Test Des
</commit_message>
<xml_diff>
--- a/Middle Assignment/TestDesignTechique_PhamHongAnh.xlsx
+++ b/Middle Assignment/TestDesignTechique_PhamHongAnh.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NashTech\Rookies\NashTech_Homework\Middle Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8EF652-29EB-46E2-947F-EC308CEE96C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE7B92C-2602-439D-BCC6-9E54BBC3E7ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10" yWindow="20" windowWidth="18710" windowHeight="10000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment 1" sheetId="1" r:id="rId1"/>
@@ -875,8 +875,139 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>ADMIN</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{427E75BA-A1D9-48BF-A11C-437E2A2B00E9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>ADMIN:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Use action verbs e.g., check…
+Chỉ xét view</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{D3680262-4AEF-4470-9F4C-246D2938922D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>ADMIN:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+output -&gt; user thấy kết quả thôi</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B58" authorId="0" shapeId="0" xr:uid="{7669F4CE-5AC5-462A-8F27-5B6BC685918F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>ADMIN:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Tách thành 2 cases riêng</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B59" authorId="0" shapeId="0" xr:uid="{44C63921-84DC-4DF1-B03C-5B2AD55E4B3D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>ADMIN:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Tách thành 2 cases riêng</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B71" authorId="0" shapeId="0" xr:uid="{44778E83-60C9-48E6-8A5E-C1A9873612BC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>ADMIN:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Decision table</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="471">
   <si>
     <t>ID</t>
   </si>
@@ -2303,6 +2434,240 @@
   <si>
     <t>2. The slide button becomes the SMS verification field
 5. Pop-up error message shows "Invalid verification code"</t>
+  </si>
+  <si>
+    <t>Search box</t>
+  </si>
+  <si>
+    <t>Check default - Check if the search box is clickable</t>
+  </si>
+  <si>
+    <t>Check default - Check if users can type in the search box</t>
+  </si>
+  <si>
+    <t>Check default - Check the placeholder of the search box</t>
+  </si>
+  <si>
+    <t>Check default - Check if the search icon is visible</t>
+  </si>
+  <si>
+    <t>When entering a numerical value only</t>
+  </si>
+  <si>
+    <t>When entering a special character only</t>
+  </si>
+  <si>
+    <t>When entering an alphabetic value only</t>
+  </si>
+  <si>
+    <t>When entering an alphabetic value and a numerical value</t>
+  </si>
+  <si>
+    <t>When entering an alphabetic value and a special value</t>
+  </si>
+  <si>
+    <t>When entering an numerical value and a special value</t>
+  </si>
+  <si>
+    <t>When entering a numerical value, a special value and an alphbetic value</t>
+  </si>
+  <si>
+    <t>When entering no value</t>
+  </si>
+  <si>
+    <t>Thêm slide SMS</t>
+  </si>
+  <si>
+    <t>When copying a text and pasting it to the search box</t>
+  </si>
+  <si>
+    <t>Check default - Check when clicking on the search box</t>
+  </si>
+  <si>
+    <t>Check if the suggestion drop-down bar works when entering a keyword</t>
+  </si>
+  <si>
+    <t>Check if related keywords are added to the search result when selecting a suggestion</t>
+  </si>
+  <si>
+    <t>When search criteria are not matched</t>
+  </si>
+  <si>
+    <t>Check the number of suggestions</t>
+  </si>
+  <si>
+    <t>When entering an uppercase value</t>
+  </si>
+  <si>
+    <t>When entering a lowercase value</t>
+  </si>
+  <si>
+    <t>Check the order of suggestions</t>
+  </si>
+  <si>
+    <t>Check the number of letters required for auto complete</t>
+  </si>
+  <si>
+    <t>Check if suggested product titles have the same words as the keywords</t>
+  </si>
+  <si>
+    <t>Check if the "Clear" button in the suggestion drop-down bar is visible</t>
+  </si>
+  <si>
+    <t>Check if the "Clear" button in the suggestion drop-down bar works</t>
+  </si>
+  <si>
+    <t>When entering only a Product Name</t>
+  </si>
+  <si>
+    <t>When entering only a Category Name</t>
+  </si>
+  <si>
+    <t>When entering a Product Name and a Category Name</t>
+  </si>
+  <si>
+    <t>When entering a Product Name and a Brand Name</t>
+  </si>
+  <si>
+    <t>When entering a Product Name and a Supplier Name</t>
+  </si>
+  <si>
+    <t>When entering a Category Name and a Brand Name</t>
+  </si>
+  <si>
+    <t>When entering a Category Name and a Supplier Name</t>
+  </si>
+  <si>
+    <t>When entering a Brand Name and a Supplier Name</t>
+  </si>
+  <si>
+    <t>When entering a Product Name, a Category Name and a Brand Name</t>
+  </si>
+  <si>
+    <t>When entering a Product Name, a Category Name and a Supplier Name</t>
+  </si>
+  <si>
+    <t>When entering a Product Name, a Brand Name and a Supplier Name</t>
+  </si>
+  <si>
+    <t>When entering a Category Name, a Brand Name and a Supplier Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When entering only a Supplier Name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">When entering only a Brand Name </t>
+  </si>
+  <si>
+    <t>When there is more than 10 items in the pagination</t>
+  </si>
+  <si>
+    <t>Check default - Check if pagination is visible</t>
+  </si>
+  <si>
+    <t>Check the order of pagination</t>
+  </si>
+  <si>
+    <t>Check if higher numbers appear when going to the next page</t>
+  </si>
+  <si>
+    <t>Check if lower numbers appear when going to the previous page</t>
+  </si>
+  <si>
+    <t>When there is 10 items on each page</t>
+  </si>
+  <si>
+    <t>When there is fewer than 10 items on each page</t>
+  </si>
+  <si>
+    <t>Check items displayed on a page</t>
+  </si>
+  <si>
+    <t>When there is no item on a page</t>
+  </si>
+  <si>
+    <t>When clicking on the &gt; button in the pagination</t>
+  </si>
+  <si>
+    <t>When clicking on the &lt; button in the pagination</t>
+  </si>
+  <si>
+    <t>Pagination</t>
+  </si>
+  <si>
+    <t>Sort by</t>
+  </si>
+  <si>
+    <t>Check if the Search Suggestion works</t>
+  </si>
+  <si>
+    <t>Check if the Search History works when logging in</t>
+  </si>
+  <si>
+    <t>Check if the Search History works when not loggin in</t>
+  </si>
+  <si>
+    <t>Check if similar characters are bolded in the Search Suggestion</t>
+  </si>
+  <si>
+    <t>Check default - Check if the drop-down bar works</t>
+  </si>
+  <si>
+    <t>Check the order of the values in the drop-down bar</t>
+  </si>
+  <si>
+    <t>Check if all values in the drop-down bar are visible</t>
+  </si>
+  <si>
+    <t>Check if all values in the drop-down bar are clickable</t>
+  </si>
+  <si>
+    <t>Check if the &gt; button is enabled on the first page</t>
+  </si>
+  <si>
+    <t>Check if the &lt; button is disabled on the first page</t>
+  </si>
+  <si>
+    <t>Check if the &lt; button is enabled on the last page</t>
+  </si>
+  <si>
+    <t>Check if the &gt; button is disabled on the last page</t>
+  </si>
+  <si>
+    <t>Check the &gt; button when selecting the close-to-last page</t>
+  </si>
+  <si>
+    <t>Check the &lt; button when selecting the close-to-first page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check default - Check if the Search Box is visible on every page </t>
+  </si>
+  <si>
+    <t>Check default - Check if the down arrow (V) is visible</t>
+  </si>
+  <si>
+    <t>trùng với entering no value?</t>
+  </si>
+  <si>
+    <t>Check the number of the latest search keywords</t>
+  </si>
+  <si>
+    <t>Check the order of the latest search keywords</t>
+  </si>
+  <si>
+    <t>Check if page numbers can be clicked on</t>
+  </si>
+  <si>
+    <t>Check the default value in the drop-down bar</t>
+  </si>
+  <si>
+    <t>Check the placeholder when choosing values</t>
+  </si>
+  <si>
+    <t>Check when sorting by "Price low to high" works</t>
+  </si>
+  <si>
+    <t>Check when sorting by "Price high to low" works</t>
   </si>
 </sst>
 </file>
@@ -2658,13 +3023,13 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2896,8 +3261,8 @@
   </sheetPr>
   <dimension ref="A1:Z1039"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49:B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15201,8 +15566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{861DB058-9ABC-4928-81FB-0309C7B8DB85}">
   <dimension ref="A1:Z203"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -15268,14 +15633,14 @@
       <c r="A2" s="38" t="s">
         <v>158</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
       <c r="J2" s="26"/>
       <c r="K2" s="26"/>
       <c r="L2" s="26"/>
@@ -15377,7 +15742,9 @@
       <c r="D6" s="30" t="s">
         <v>244</v>
       </c>
-      <c r="E6" s="32"/>
+      <c r="E6" s="32" t="s">
+        <v>406</v>
+      </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
@@ -15546,7 +15913,7 @@
       <c r="I14" s="32"/>
     </row>
     <row r="15" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="47" t="s">
         <v>122</v>
       </c>
       <c r="B15" s="46"/>
@@ -15776,7 +16143,7 @@
       <c r="I25" s="32"/>
     </row>
     <row r="26" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="45" t="s">
+      <c r="A26" s="47" t="s">
         <v>127</v>
       </c>
       <c r="B26" s="46"/>
@@ -16206,7 +16573,7 @@
       <c r="I46" s="32"/>
     </row>
     <row r="47" spans="1:9" s="10" customFormat="1" ht="21.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="45" t="s">
+      <c r="A47" s="47" t="s">
         <v>140</v>
       </c>
       <c r="B47" s="46"/>
@@ -16539,7 +16906,7 @@
       <c r="I63" s="32"/>
     </row>
     <row r="64" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="45" t="s">
+      <c r="A64" s="47" t="s">
         <v>147</v>
       </c>
       <c r="B64" s="46"/>
@@ -16652,7 +17019,7 @@
       <c r="I69" s="32"/>
     </row>
     <row r="70" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="45" t="s">
+      <c r="A70" s="47" t="s">
         <v>148</v>
       </c>
       <c r="B70" s="46"/>
@@ -16928,17 +17295,17 @@
       <c r="A84" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="B84" s="47"/>
-      <c r="C84" s="47"/>
-      <c r="D84" s="47"/>
-      <c r="E84" s="47"/>
-      <c r="F84" s="47"/>
-      <c r="G84" s="47"/>
-      <c r="H84" s="47"/>
-      <c r="I84" s="47"/>
+      <c r="B84" s="45"/>
+      <c r="C84" s="45"/>
+      <c r="D84" s="45"/>
+      <c r="E84" s="45"/>
+      <c r="F84" s="45"/>
+      <c r="G84" s="45"/>
+      <c r="H84" s="45"/>
+      <c r="I84" s="45"/>
     </row>
     <row r="85" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="45" t="s">
+      <c r="A85" s="47" t="s">
         <v>165</v>
       </c>
       <c r="B85" s="46"/>
@@ -17247,17 +17614,17 @@
       <c r="A106" s="38" t="s">
         <v>187</v>
       </c>
-      <c r="B106" s="47"/>
-      <c r="C106" s="47"/>
-      <c r="D106" s="47"/>
-      <c r="E106" s="47"/>
-      <c r="F106" s="47"/>
-      <c r="G106" s="47"/>
-      <c r="H106" s="47"/>
-      <c r="I106" s="47"/>
+      <c r="B106" s="45"/>
+      <c r="C106" s="45"/>
+      <c r="D106" s="45"/>
+      <c r="E106" s="45"/>
+      <c r="F106" s="45"/>
+      <c r="G106" s="45"/>
+      <c r="H106" s="45"/>
+      <c r="I106" s="45"/>
     </row>
     <row r="107" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="45" t="s">
+      <c r="A107" s="47" t="s">
         <v>168</v>
       </c>
       <c r="B107" s="46"/>
@@ -17337,7 +17704,7 @@
       <c r="I110" s="32"/>
     </row>
     <row r="111" spans="1:26" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="45" t="s">
+      <c r="A111" s="47" t="s">
         <v>153</v>
       </c>
       <c r="B111" s="46"/>
@@ -17382,7 +17749,7 @@
       <c r="I113" s="32"/>
     </row>
     <row r="114" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="45" t="s">
+      <c r="A114" s="47" t="s">
         <v>156</v>
       </c>
       <c r="B114" s="46"/>
@@ -17411,7 +17778,7 @@
       <c r="I115" s="32"/>
     </row>
     <row r="116" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="45" t="s">
+      <c r="A116" s="47" t="s">
         <v>177</v>
       </c>
       <c r="B116" s="46"/>
@@ -17440,7 +17807,7 @@
       <c r="I117" s="32"/>
     </row>
     <row r="118" spans="1:9" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="45" t="s">
+      <c r="A118" s="47" t="s">
         <v>180</v>
       </c>
       <c r="B118" s="46"/>
@@ -17501,7 +17868,7 @@
       <c r="I121" s="32"/>
     </row>
     <row r="122" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="45" t="s">
+      <c r="A122" s="47" t="s">
         <v>184</v>
       </c>
       <c r="B122" s="46"/>
@@ -17580,7 +17947,7 @@
       <c r="I126" s="32"/>
     </row>
     <row r="127" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="45" t="s">
+      <c r="A127" s="47" t="s">
         <v>181</v>
       </c>
       <c r="B127" s="46"/>
@@ -17609,7 +17976,7 @@
       <c r="I128" s="32"/>
     </row>
     <row r="129" spans="1:26" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="45" t="s">
+      <c r="A129" s="47" t="s">
         <v>182</v>
       </c>
       <c r="B129" s="46"/>
@@ -17638,7 +18005,7 @@
       <c r="I130" s="32"/>
     </row>
     <row r="131" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A131" s="45" t="s">
+      <c r="A131" s="47" t="s">
         <v>164</v>
       </c>
       <c r="B131" s="46"/>
@@ -18540,6 +18907,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A131:I131"/>
+    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="A84:I84"/>
+    <mergeCell ref="A47:I47"/>
+    <mergeCell ref="A64:I64"/>
+    <mergeCell ref="A70:I70"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A15:I15"/>
@@ -18554,12 +18927,6 @@
     <mergeCell ref="A116:I116"/>
     <mergeCell ref="A118:I118"/>
     <mergeCell ref="A111:I111"/>
-    <mergeCell ref="A131:I131"/>
-    <mergeCell ref="A26:I26"/>
-    <mergeCell ref="A84:I84"/>
-    <mergeCell ref="A47:I47"/>
-    <mergeCell ref="A64:I64"/>
-    <mergeCell ref="A70:I70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -18568,14 +18935,3216 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2157BC9-A210-4D6F-8D8A-C479F47A0035}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2157BC9-A210-4D6F-8D8A-C479F47A0035}">
+  <dimension ref="A1:I247"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="28"/>
+    <col min="2" max="2" width="35.453125" style="31" customWidth="1"/>
+    <col min="3" max="3" width="49.26953125" style="31" customWidth="1"/>
+    <col min="4" max="4" width="49.08984375" style="31" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" style="33" customWidth="1"/>
+    <col min="6" max="6" width="17" style="28" customWidth="1"/>
+    <col min="7" max="7" width="14.54296875" style="28" customWidth="1"/>
+    <col min="8" max="8" width="17.08984375" style="28" customWidth="1"/>
+    <col min="9" max="9" width="15.1796875" style="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="21.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>393</v>
+      </c>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+    </row>
+    <row r="3" spans="1:9" ht="38.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>1</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>394</v>
+      </c>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="32"/>
+    </row>
+    <row r="4" spans="1:9" ht="38.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="27">
+        <f ca="1">IF(OFFSET(A4,-1,0) ="",OFFSET(A4,-2,0)+1,OFFSET(A4,-1,0)+1 )</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>408</v>
+      </c>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="32"/>
+    </row>
+    <row r="5" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="27">
+        <f ca="1">IF(OFFSET(A5,-1,0) ="",OFFSET(A5,-2,0)+1,OFFSET(A5,-1,0)+1 )</f>
+        <v>3</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>395</v>
+      </c>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="32"/>
+    </row>
+    <row r="6" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="27">
+        <f ca="1">IF(OFFSET(A6,-1,0) ="",OFFSET(A6,-2,0)+1,OFFSET(A6,-1,0)+1 )</f>
+        <v>4</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>396</v>
+      </c>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="32"/>
+    </row>
+    <row r="7" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="27">
+        <f ca="1">IF(OFFSET(A7,-1,0) ="",OFFSET(A7,-2,0)+1,OFFSET(A7,-1,0)+1 )</f>
+        <v>5</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>397</v>
+      </c>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="32"/>
+    </row>
+    <row r="8" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="27">
+        <f ca="1">IF(OFFSET(A8,-1,0) ="",OFFSET(A8,-2,0)+1,OFFSET(A8,-1,0)+1 )</f>
+        <v>6</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>461</v>
+      </c>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="32"/>
+    </row>
+    <row r="9" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="27">
+        <f ca="1">IF(OFFSET(A9,-1,0) ="",OFFSET(A9,-2,0)+1,OFFSET(A9,-1,0)+1 )</f>
+        <v>7</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>447</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>463</v>
+      </c>
+      <c r="D9" s="30"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="32"/>
+    </row>
+    <row r="10" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="27">
+        <f ca="1">IF(OFFSET(A10,-1,0) ="",OFFSET(A10,-2,0)+1,OFFSET(A10,-1,0)+1 )</f>
+        <v>8</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>448</v>
+      </c>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="32"/>
+    </row>
+    <row r="11" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="27">
+        <f ca="1">IF(OFFSET(A11,-1,0) ="",OFFSET(A11,-2,0)+1,OFFSET(A11,-1,0)+1 )</f>
+        <v>9</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>449</v>
+      </c>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="32"/>
+    </row>
+    <row r="12" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="27">
+        <f ca="1">IF(OFFSET(A12,-1,0) ="",OFFSET(A12,-2,0)+1,OFFSET(A12,-1,0)+1 )</f>
+        <v>10</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>464</v>
+      </c>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="32"/>
+    </row>
+    <row r="13" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="27">
+        <f ca="1">IF(OFFSET(A13,-1,0) ="",OFFSET(A13,-2,0)+1,OFFSET(A13,-1,0)+1 )</f>
+        <v>11</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>465</v>
+      </c>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="32"/>
+    </row>
+    <row r="14" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="27">
+        <f ca="1">IF(OFFSET(A14,-1,0) ="",OFFSET(A14,-2,0)+1,OFFSET(A14,-1,0)+1 )</f>
+        <v>12</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>418</v>
+      </c>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="32"/>
+    </row>
+    <row r="15" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="27">
+        <f ca="1">IF(OFFSET(A15,-1,0) ="",OFFSET(A15,-2,0)+1,OFFSET(A15,-1,0)+1 )</f>
+        <v>13</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>419</v>
+      </c>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="32"/>
+    </row>
+    <row r="16" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="27">
+        <f t="shared" ref="A16:A107" ca="1" si="0">IF(OFFSET(A16,-1,0) ="",OFFSET(A16,-2,0)+1,OFFSET(A16,-1,0)+1 )</f>
+        <v>14</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>227</v>
+      </c>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="32"/>
+    </row>
+    <row r="17" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>405</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="32"/>
+    </row>
+    <row r="18" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>407</v>
+      </c>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="32"/>
+    </row>
+    <row r="19" spans="1:9" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>420</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="32"/>
+    </row>
+    <row r="20" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>421</v>
+      </c>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="32"/>
+    </row>
+    <row r="21" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>433</v>
+      </c>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="32"/>
+    </row>
+    <row r="22" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>432</v>
+      </c>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="32"/>
+    </row>
+    <row r="23" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B23" s="30" t="s">
+        <v>422</v>
+      </c>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="32"/>
+    </row>
+    <row r="24" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>423</v>
+      </c>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="32"/>
+    </row>
+    <row r="25" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B25" s="30" t="s">
+        <v>424</v>
+      </c>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="32"/>
+    </row>
+    <row r="26" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>425</v>
+      </c>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="32"/>
+    </row>
+    <row r="27" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B27" s="30" t="s">
+        <v>426</v>
+      </c>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="32"/>
+    </row>
+    <row r="28" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B28" s="30" t="s">
+        <v>427</v>
+      </c>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="32"/>
+    </row>
+    <row r="29" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B29" s="30" t="s">
+        <v>428</v>
+      </c>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="32"/>
+    </row>
+    <row r="30" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>429</v>
+      </c>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="32"/>
+    </row>
+    <row r="31" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B31" s="30" t="s">
+        <v>430</v>
+      </c>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="32"/>
+    </row>
+    <row r="32" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B32" s="30" t="s">
+        <v>431</v>
+      </c>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="32"/>
+    </row>
+    <row r="33" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B33" s="30" t="s">
+        <v>409</v>
+      </c>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="32"/>
+    </row>
+    <row r="34" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B34" s="30" t="s">
+        <v>416</v>
+      </c>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="32"/>
+    </row>
+    <row r="35" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B35" s="30" t="s">
+        <v>417</v>
+      </c>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="32"/>
+    </row>
+    <row r="36" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B36" s="30" t="s">
+        <v>412</v>
+      </c>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="32"/>
+    </row>
+    <row r="37" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B37" s="30" t="s">
+        <v>415</v>
+      </c>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="32"/>
+    </row>
+    <row r="38" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B38" s="30" t="s">
+        <v>450</v>
+      </c>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="32"/>
+    </row>
+    <row r="39" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B39" s="30" t="s">
+        <v>410</v>
+      </c>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="32"/>
+    </row>
+    <row r="40" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="27">
+        <f ca="1">IF(OFFSET(A40,-1,0) ="",OFFSET(A40,-2,0)+1,OFFSET(A40,-1,0)+1 )</f>
+        <v>38</v>
+      </c>
+      <c r="B40" s="30" t="s">
+        <v>411</v>
+      </c>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="32"/>
+    </row>
+    <row r="41" spans="1:9" ht="21.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="38" t="s">
+        <v>445</v>
+      </c>
+      <c r="B41" s="45"/>
+      <c r="C41" s="45"/>
+      <c r="D41" s="45"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="45"/>
+      <c r="G41" s="45"/>
+      <c r="H41" s="45"/>
+      <c r="I41" s="45"/>
+    </row>
+    <row r="42" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="27">
+        <f ca="1">IF(OFFSET(A42,-2,0) ="",OFFSET(A42,-2,0)+1,OFFSET(A42,-2,0)+1 )</f>
+        <v>39</v>
+      </c>
+      <c r="B42" s="30" t="s">
+        <v>435</v>
+      </c>
+      <c r="C42" s="30"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="32"/>
+    </row>
+    <row r="43" spans="1:9" ht="21.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="27">
+        <f ca="1">IF(OFFSET(A43,-1,0) ="",OFFSET(A43,-2,0)+1,OFFSET(A43,-1,0)+1 )</f>
+        <v>40</v>
+      </c>
+      <c r="B43" s="30" t="s">
+        <v>466</v>
+      </c>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="32"/>
+    </row>
+    <row r="44" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B44" s="30" t="s">
+        <v>441</v>
+      </c>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="32"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="32"/>
+    </row>
+    <row r="45" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B45" s="30" t="s">
+        <v>436</v>
+      </c>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="32"/>
+    </row>
+    <row r="46" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B46" s="30" t="s">
+        <v>437</v>
+      </c>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="32"/>
+    </row>
+    <row r="47" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B47" s="30" t="s">
+        <v>438</v>
+      </c>
+      <c r="C47" s="30"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="32"/>
+    </row>
+    <row r="48" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B48" s="30" t="s">
+        <v>440</v>
+      </c>
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="32"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="32"/>
+    </row>
+    <row r="49" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B49" s="30" t="s">
+        <v>439</v>
+      </c>
+      <c r="C49" s="30"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="32"/>
+    </row>
+    <row r="50" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="27">
+        <f ca="1">IF(OFFSET(A50,-2,0) ="",OFFSET(A50,-2,0)+1,OFFSET(A50,-2,0)+1 )</f>
+        <v>46</v>
+      </c>
+      <c r="B50" s="30" t="s">
+        <v>434</v>
+      </c>
+      <c r="C50" s="30"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="32"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="32"/>
+    </row>
+    <row r="51" spans="1:9" ht="26.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="27">
+        <f ca="1">IF(OFFSET(A51,-1,0) ="",OFFSET(A51,-2,0)+1,OFFSET(A51,-1,0)+1 )</f>
+        <v>47</v>
+      </c>
+      <c r="B51" s="30" t="s">
+        <v>442</v>
+      </c>
+      <c r="C51" s="30"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="34"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="32"/>
+    </row>
+    <row r="52" spans="1:9" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="27">
+        <f ca="1">IF(OFFSET(A52,-1,0) ="",OFFSET(A52,-2,0)+1,OFFSET(A52,-1,0)+1 )</f>
+        <v>48</v>
+      </c>
+      <c r="B52" s="30" t="s">
+        <v>443</v>
+      </c>
+      <c r="C52" s="30"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="34"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="32"/>
+    </row>
+    <row r="53" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B53" s="30" t="s">
+        <v>444</v>
+      </c>
+      <c r="C53" s="30"/>
+      <c r="D53" s="30"/>
+      <c r="E53" s="32"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="32"/>
+    </row>
+    <row r="54" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B54" s="30" t="s">
+        <v>456</v>
+      </c>
+      <c r="C54" s="30"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="32"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="32"/>
+    </row>
+    <row r="55" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B55" s="30" t="s">
+        <v>455</v>
+      </c>
+      <c r="C55" s="30"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="32"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="32"/>
+    </row>
+    <row r="56" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B56" s="30" t="s">
+        <v>457</v>
+      </c>
+      <c r="C56" s="30"/>
+      <c r="D56" s="30"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="32"/>
+    </row>
+    <row r="57" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B57" s="30" t="s">
+        <v>458</v>
+      </c>
+      <c r="C57" s="30"/>
+      <c r="D57" s="30"/>
+      <c r="E57" s="32"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="32"/>
+    </row>
+    <row r="58" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>459</v>
+      </c>
+      <c r="C58" s="30"/>
+      <c r="D58" s="30"/>
+      <c r="E58" s="32"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="32"/>
+    </row>
+    <row r="59" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>460</v>
+      </c>
+      <c r="C59" s="30"/>
+      <c r="D59" s="30"/>
+      <c r="E59" s="32"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="32"/>
+    </row>
+    <row r="60" spans="1:9" ht="21.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="38" t="s">
+        <v>446</v>
+      </c>
+      <c r="B60" s="45"/>
+      <c r="C60" s="45"/>
+      <c r="D60" s="45"/>
+      <c r="E60" s="45"/>
+      <c r="F60" s="45"/>
+      <c r="G60" s="45"/>
+      <c r="H60" s="45"/>
+      <c r="I60" s="45"/>
+    </row>
+    <row r="61" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="27">
+        <f ca="1">IF(OFFSET(A61,-2,0) ="",OFFSET(A61,-2,0)+1,OFFSET(A61,-2,0)+1 )</f>
+        <v>56</v>
+      </c>
+      <c r="B61" s="29" t="s">
+        <v>451</v>
+      </c>
+      <c r="C61" s="30"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="32"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="32"/>
+    </row>
+    <row r="62" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B62" s="29" t="s">
+        <v>462</v>
+      </c>
+      <c r="C62" s="30"/>
+      <c r="D62" s="30"/>
+      <c r="E62" s="32"/>
+      <c r="F62" s="13"/>
+      <c r="G62" s="13"/>
+      <c r="H62" s="13"/>
+      <c r="I62" s="32"/>
+    </row>
+    <row r="63" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B63" s="29" t="s">
+        <v>453</v>
+      </c>
+      <c r="C63" s="30"/>
+      <c r="D63" s="30"/>
+      <c r="E63" s="32"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="13"/>
+      <c r="I63" s="32"/>
+    </row>
+    <row r="64" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="B64" s="29" t="s">
+        <v>454</v>
+      </c>
+      <c r="C64" s="30"/>
+      <c r="D64" s="30"/>
+      <c r="E64" s="32"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="13"/>
+      <c r="I64" s="32"/>
+    </row>
+    <row r="65" spans="1:9" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B65" s="29" t="s">
+        <v>452</v>
+      </c>
+      <c r="C65" s="30"/>
+      <c r="D65" s="30"/>
+      <c r="E65" s="32"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13"/>
+      <c r="I65" s="32"/>
+    </row>
+    <row r="66" spans="1:9" ht="25" x14ac:dyDescent="0.25">
+      <c r="A66" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="B66" s="29" t="s">
+        <v>467</v>
+      </c>
+      <c r="C66" s="30"/>
+      <c r="D66" s="30"/>
+      <c r="E66" s="32"/>
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13"/>
+      <c r="I66" s="32"/>
+    </row>
+    <row r="67" spans="1:9" ht="29.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="B67" s="29" t="s">
+        <v>468</v>
+      </c>
+      <c r="C67" s="30"/>
+      <c r="D67" s="30"/>
+      <c r="E67" s="32"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+      <c r="I67" s="32"/>
+    </row>
+    <row r="68" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="B68" s="29" t="s">
+        <v>469</v>
+      </c>
+      <c r="C68" s="30"/>
+      <c r="D68" s="30"/>
+      <c r="E68" s="32"/>
+      <c r="F68" s="13"/>
+      <c r="G68" s="13"/>
+      <c r="H68" s="13"/>
+      <c r="I68" s="32"/>
+    </row>
+    <row r="69" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="27">
+        <f ca="1">IF(OFFSET(A69,-1,0) ="",OFFSET(A69,-2,0)+1,OFFSET(A69,-1,0)+1 )</f>
+        <v>64</v>
+      </c>
+      <c r="B69" s="29" t="s">
+        <v>470</v>
+      </c>
+      <c r="C69" s="30"/>
+      <c r="D69" s="30"/>
+      <c r="E69" s="32"/>
+      <c r="F69" s="13"/>
+      <c r="G69" s="13"/>
+      <c r="H69" s="13"/>
+      <c r="I69" s="32"/>
+    </row>
+    <row r="70" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="A70" s="47"/>
+      <c r="B70" s="46"/>
+      <c r="C70" s="46"/>
+      <c r="D70" s="46"/>
+      <c r="E70" s="46"/>
+      <c r="F70" s="46"/>
+      <c r="G70" s="46"/>
+      <c r="H70" s="46"/>
+      <c r="I70" s="46"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="27">
+        <f ca="1">IF(OFFSET(A71,-2,0) ="",OFFSET(A71,-2,0)+1,OFFSET(A71,-2,0)+1 )</f>
+        <v>65</v>
+      </c>
+      <c r="B71" s="30"/>
+      <c r="C71" s="29"/>
+      <c r="D71" s="30"/>
+      <c r="E71" s="32"/>
+      <c r="F71" s="13"/>
+      <c r="G71" s="13"/>
+      <c r="H71" s="13"/>
+      <c r="I71" s="32"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="27">
+        <f ca="1">IF(OFFSET(A72,-1,0) ="",OFFSET(A72,-2,0)+1,OFFSET(A72,-1,0)+1 )</f>
+        <v>66</v>
+      </c>
+      <c r="B72" s="30"/>
+      <c r="C72" s="30"/>
+      <c r="D72" s="30"/>
+      <c r="E72" s="32"/>
+      <c r="F72" s="13"/>
+      <c r="G72" s="13"/>
+      <c r="H72" s="13"/>
+      <c r="I72" s="32"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="27">
+        <f ca="1">IF(OFFSET(A73,-1,0) ="",OFFSET(A73,-2,0)+1,OFFSET(A73,-1,0)+1 )</f>
+        <v>67</v>
+      </c>
+      <c r="B73" s="29"/>
+      <c r="C73" s="29"/>
+      <c r="D73" s="30"/>
+      <c r="E73" s="32"/>
+      <c r="F73" s="13"/>
+      <c r="G73" s="13"/>
+      <c r="H73" s="13"/>
+      <c r="I73" s="32"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="B74" s="29"/>
+      <c r="C74" s="29"/>
+      <c r="D74" s="30"/>
+      <c r="E74" s="32"/>
+      <c r="F74" s="13"/>
+      <c r="G74" s="13"/>
+      <c r="H74" s="13"/>
+      <c r="I74" s="32"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="B75" s="29"/>
+      <c r="C75" s="29"/>
+      <c r="D75" s="30"/>
+      <c r="E75" s="32"/>
+      <c r="F75" s="13"/>
+      <c r="G75" s="13"/>
+      <c r="H75" s="13"/>
+      <c r="I75" s="32"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="B76" s="29"/>
+      <c r="C76" s="29"/>
+      <c r="D76" s="30"/>
+      <c r="E76" s="32"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="13"/>
+      <c r="H76" s="13"/>
+      <c r="I76" s="32"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>71</v>
+      </c>
+      <c r="B77" s="29"/>
+      <c r="C77" s="29"/>
+      <c r="D77" s="30"/>
+      <c r="E77" s="32"/>
+      <c r="F77" s="13"/>
+      <c r="G77" s="13"/>
+      <c r="H77" s="13"/>
+      <c r="I77" s="32"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="B78" s="29"/>
+      <c r="C78" s="29"/>
+      <c r="D78" s="30"/>
+      <c r="E78" s="32"/>
+      <c r="F78" s="13"/>
+      <c r="G78" s="13"/>
+      <c r="H78" s="13"/>
+      <c r="I78" s="32"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="B79" s="29"/>
+      <c r="C79" s="29"/>
+      <c r="D79" s="30"/>
+      <c r="E79" s="32"/>
+      <c r="F79" s="13"/>
+      <c r="G79" s="13"/>
+      <c r="H79" s="13"/>
+      <c r="I79" s="32"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="B80" s="29"/>
+      <c r="C80" s="29"/>
+      <c r="D80" s="30"/>
+      <c r="E80" s="32"/>
+      <c r="F80" s="13"/>
+      <c r="G80" s="13"/>
+      <c r="H80" s="13"/>
+      <c r="I80" s="32"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="B81" s="29"/>
+      <c r="C81" s="29"/>
+      <c r="D81" s="30"/>
+      <c r="E81" s="32"/>
+      <c r="F81" s="13"/>
+      <c r="G81" s="13"/>
+      <c r="H81" s="13"/>
+      <c r="I81" s="32"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="B82" s="29"/>
+      <c r="C82" s="30"/>
+      <c r="D82" s="30"/>
+      <c r="E82" s="32"/>
+      <c r="F82" s="13"/>
+      <c r="G82" s="13"/>
+      <c r="H82" s="13"/>
+      <c r="I82" s="32"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="B83" s="29"/>
+      <c r="C83" s="30"/>
+      <c r="D83" s="30"/>
+      <c r="E83" s="32"/>
+      <c r="F83" s="13"/>
+      <c r="G83" s="13"/>
+      <c r="H83" s="13"/>
+      <c r="I83" s="32"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="B84" s="29"/>
+      <c r="C84" s="30"/>
+      <c r="D84" s="30"/>
+      <c r="E84" s="32"/>
+      <c r="F84" s="13"/>
+      <c r="G84" s="13"/>
+      <c r="H84" s="13"/>
+      <c r="I84" s="32"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>79</v>
+      </c>
+      <c r="B85" s="29"/>
+      <c r="C85" s="30"/>
+      <c r="D85" s="30"/>
+      <c r="E85" s="32"/>
+      <c r="F85" s="13"/>
+      <c r="G85" s="13"/>
+      <c r="H85" s="13"/>
+      <c r="I85" s="32"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="B86" s="29"/>
+      <c r="C86" s="30"/>
+      <c r="D86" s="30"/>
+      <c r="E86" s="32"/>
+      <c r="F86" s="13"/>
+      <c r="G86" s="13"/>
+      <c r="H86" s="13"/>
+      <c r="I86" s="32"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>81</v>
+      </c>
+      <c r="B87" s="29"/>
+      <c r="C87" s="30"/>
+      <c r="D87" s="30"/>
+      <c r="E87" s="32"/>
+      <c r="F87" s="13"/>
+      <c r="G87" s="13"/>
+      <c r="H87" s="13"/>
+      <c r="I87" s="32"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>82</v>
+      </c>
+      <c r="B88" s="29"/>
+      <c r="C88" s="30"/>
+      <c r="D88" s="30"/>
+      <c r="E88" s="32"/>
+      <c r="F88" s="13"/>
+      <c r="G88" s="13"/>
+      <c r="H88" s="13"/>
+      <c r="I88" s="32"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>83</v>
+      </c>
+      <c r="B89" s="30"/>
+      <c r="C89" s="30"/>
+      <c r="D89" s="30"/>
+      <c r="E89" s="32"/>
+      <c r="F89" s="13"/>
+      <c r="G89" s="13"/>
+      <c r="H89" s="13"/>
+      <c r="I89" s="32"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="B90" s="15"/>
+      <c r="C90" s="30"/>
+      <c r="D90" s="30"/>
+      <c r="E90" s="32"/>
+      <c r="F90" s="13"/>
+      <c r="G90" s="13"/>
+      <c r="H90" s="13"/>
+      <c r="I90" s="32"/>
+    </row>
+    <row r="91" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="A91" s="47"/>
+      <c r="B91" s="46"/>
+      <c r="C91" s="46"/>
+      <c r="D91" s="46"/>
+      <c r="E91" s="46"/>
+      <c r="F91" s="46"/>
+      <c r="G91" s="46"/>
+      <c r="H91" s="46"/>
+      <c r="I91" s="46"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="27">
+        <f ca="1">IF(OFFSET(A92,-2,0) ="",OFFSET(A92,-2,0)+1,OFFSET(A92,-2,0)+1 )</f>
+        <v>85</v>
+      </c>
+      <c r="B92" s="30"/>
+      <c r="C92" s="30"/>
+      <c r="D92" s="30"/>
+      <c r="E92" s="32"/>
+      <c r="F92" s="13"/>
+      <c r="G92" s="13"/>
+      <c r="H92" s="13"/>
+      <c r="I92" s="32"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>86</v>
+      </c>
+      <c r="B93" s="30"/>
+      <c r="C93" s="30"/>
+      <c r="D93" s="30"/>
+      <c r="E93" s="32"/>
+      <c r="F93" s="13"/>
+      <c r="G93" s="13"/>
+      <c r="H93" s="13"/>
+      <c r="I93" s="32"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>87</v>
+      </c>
+      <c r="B94" s="30"/>
+      <c r="C94" s="30"/>
+      <c r="D94" s="30"/>
+      <c r="E94" s="30"/>
+      <c r="F94" s="13"/>
+      <c r="G94" s="13"/>
+      <c r="H94" s="13"/>
+      <c r="I94" s="32"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="B95" s="30"/>
+      <c r="C95" s="30"/>
+      <c r="D95" s="30"/>
+      <c r="E95" s="32"/>
+      <c r="F95" s="13"/>
+      <c r="G95" s="13"/>
+      <c r="H95" s="13"/>
+      <c r="I95" s="32"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>89</v>
+      </c>
+      <c r="B96" s="30"/>
+      <c r="C96" s="30"/>
+      <c r="D96" s="30"/>
+      <c r="E96" s="32"/>
+      <c r="F96" s="13"/>
+      <c r="G96" s="13"/>
+      <c r="H96" s="13"/>
+      <c r="I96" s="32"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="B97" s="30"/>
+      <c r="C97" s="29"/>
+      <c r="D97" s="30"/>
+      <c r="E97" s="32"/>
+      <c r="F97" s="13"/>
+      <c r="G97" s="13"/>
+      <c r="H97" s="13"/>
+      <c r="I97" s="32"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>91</v>
+      </c>
+      <c r="B98" s="30"/>
+      <c r="C98" s="29"/>
+      <c r="D98" s="30"/>
+      <c r="E98" s="32"/>
+      <c r="F98" s="13"/>
+      <c r="G98" s="13"/>
+      <c r="H98" s="13"/>
+      <c r="I98" s="32"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="B99" s="30"/>
+      <c r="C99" s="29"/>
+      <c r="D99" s="30"/>
+      <c r="E99" s="32"/>
+      <c r="F99" s="13"/>
+      <c r="G99" s="13"/>
+      <c r="H99" s="13"/>
+      <c r="I99" s="32"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>93</v>
+      </c>
+      <c r="B100" s="30"/>
+      <c r="C100" s="29"/>
+      <c r="D100" s="30"/>
+      <c r="E100" s="32"/>
+      <c r="F100" s="13"/>
+      <c r="G100" s="13"/>
+      <c r="H100" s="13"/>
+      <c r="I100" s="32"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>94</v>
+      </c>
+      <c r="B101" s="30"/>
+      <c r="C101" s="29"/>
+      <c r="D101" s="30"/>
+      <c r="E101" s="32"/>
+      <c r="F101" s="13"/>
+      <c r="G101" s="13"/>
+      <c r="H101" s="13"/>
+      <c r="I101" s="32"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>95</v>
+      </c>
+      <c r="B102" s="30"/>
+      <c r="C102" s="29"/>
+      <c r="D102" s="30"/>
+      <c r="E102" s="32"/>
+      <c r="F102" s="13"/>
+      <c r="G102" s="13"/>
+      <c r="H102" s="13"/>
+      <c r="I102" s="32"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="B103" s="30"/>
+      <c r="C103" s="29"/>
+      <c r="D103" s="30"/>
+      <c r="E103" s="32"/>
+      <c r="F103" s="13"/>
+      <c r="G103" s="13"/>
+      <c r="H103" s="13"/>
+      <c r="I103" s="32"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>97</v>
+      </c>
+      <c r="B104" s="30"/>
+      <c r="C104" s="29"/>
+      <c r="D104" s="30"/>
+      <c r="E104" s="32"/>
+      <c r="F104" s="13"/>
+      <c r="G104" s="13"/>
+      <c r="H104" s="13"/>
+      <c r="I104" s="32"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>98</v>
+      </c>
+      <c r="B105" s="30"/>
+      <c r="C105" s="29"/>
+      <c r="D105" s="30"/>
+      <c r="E105" s="32"/>
+      <c r="F105" s="13"/>
+      <c r="G105" s="13"/>
+      <c r="H105" s="13"/>
+      <c r="I105" s="32"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>99</v>
+      </c>
+      <c r="B106" s="30"/>
+      <c r="C106" s="29"/>
+      <c r="D106" s="30"/>
+      <c r="E106" s="32"/>
+      <c r="F106" s="13"/>
+      <c r="G106" s="13"/>
+      <c r="H106" s="13"/>
+      <c r="I106" s="32"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="B107" s="30"/>
+      <c r="C107" s="30"/>
+      <c r="D107" s="30"/>
+      <c r="E107" s="32"/>
+      <c r="F107" s="13"/>
+      <c r="G107" s="13"/>
+      <c r="H107" s="13"/>
+      <c r="I107" s="32"/>
+    </row>
+    <row r="108" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="A108" s="47"/>
+      <c r="B108" s="46"/>
+      <c r="C108" s="46"/>
+      <c r="D108" s="46"/>
+      <c r="E108" s="46"/>
+      <c r="F108" s="46"/>
+      <c r="G108" s="46"/>
+      <c r="H108" s="46"/>
+      <c r="I108" s="46"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" s="27"/>
+      <c r="B109" s="30"/>
+      <c r="C109" s="30"/>
+      <c r="D109" s="30"/>
+      <c r="E109" s="32"/>
+      <c r="F109" s="13"/>
+      <c r="G109" s="13"/>
+      <c r="H109" s="13"/>
+      <c r="I109" s="32"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" s="27"/>
+      <c r="B110" s="30"/>
+      <c r="C110" s="30"/>
+      <c r="D110" s="30"/>
+      <c r="E110" s="32"/>
+      <c r="F110" s="13"/>
+      <c r="G110" s="13"/>
+      <c r="H110" s="13"/>
+      <c r="I110" s="32"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" s="27"/>
+      <c r="B111" s="30"/>
+      <c r="C111" s="30"/>
+      <c r="D111" s="30"/>
+      <c r="E111" s="32"/>
+      <c r="F111" s="13"/>
+      <c r="G111" s="13"/>
+      <c r="H111" s="13"/>
+      <c r="I111" s="32"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" s="27"/>
+      <c r="B112" s="30"/>
+      <c r="C112" s="29"/>
+      <c r="D112" s="30"/>
+      <c r="E112" s="32"/>
+      <c r="F112" s="13"/>
+      <c r="G112" s="13"/>
+      <c r="H112" s="13"/>
+      <c r="I112" s="32"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" s="27"/>
+      <c r="B113" s="30"/>
+      <c r="C113" s="29"/>
+      <c r="D113" s="30"/>
+      <c r="E113" s="32"/>
+      <c r="F113" s="13"/>
+      <c r="G113" s="13"/>
+      <c r="H113" s="13"/>
+      <c r="I113" s="32"/>
+    </row>
+    <row r="114" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="A114" s="47"/>
+      <c r="B114" s="46"/>
+      <c r="C114" s="46"/>
+      <c r="D114" s="46"/>
+      <c r="E114" s="46"/>
+      <c r="F114" s="46"/>
+      <c r="G114" s="46"/>
+      <c r="H114" s="46"/>
+      <c r="I114" s="46"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" s="27"/>
+      <c r="B115" s="30"/>
+      <c r="C115" s="30"/>
+      <c r="D115" s="30"/>
+      <c r="E115" s="32"/>
+      <c r="F115" s="13"/>
+      <c r="G115" s="13"/>
+      <c r="H115" s="13"/>
+      <c r="I115" s="32"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" s="27"/>
+      <c r="B116" s="30"/>
+      <c r="C116" s="29"/>
+      <c r="D116" s="30"/>
+      <c r="E116" s="32"/>
+      <c r="F116" s="13"/>
+      <c r="G116" s="13"/>
+      <c r="H116" s="13"/>
+      <c r="I116" s="32"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" s="27"/>
+      <c r="B117" s="29"/>
+      <c r="C117" s="30"/>
+      <c r="D117" s="30"/>
+      <c r="E117" s="32"/>
+      <c r="F117" s="13"/>
+      <c r="G117" s="13"/>
+      <c r="H117" s="13"/>
+      <c r="I117" s="32"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118" s="27"/>
+      <c r="B118" s="29"/>
+      <c r="C118" s="30"/>
+      <c r="D118" s="30"/>
+      <c r="E118" s="32"/>
+      <c r="F118" s="13"/>
+      <c r="G118" s="13"/>
+      <c r="H118" s="13"/>
+      <c r="I118" s="32"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119" s="27"/>
+      <c r="B119" s="29"/>
+      <c r="C119" s="30"/>
+      <c r="D119" s="30"/>
+      <c r="E119" s="32"/>
+      <c r="F119" s="13"/>
+      <c r="G119" s="13"/>
+      <c r="H119" s="13"/>
+      <c r="I119" s="32"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A120" s="27"/>
+      <c r="B120" s="29"/>
+      <c r="C120" s="30"/>
+      <c r="D120" s="30"/>
+      <c r="E120" s="32"/>
+      <c r="F120" s="13"/>
+      <c r="G120" s="13"/>
+      <c r="H120" s="13"/>
+      <c r="I120" s="32"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A121" s="27"/>
+      <c r="B121" s="29"/>
+      <c r="C121" s="30"/>
+      <c r="D121" s="30"/>
+      <c r="E121" s="32"/>
+      <c r="F121" s="13"/>
+      <c r="G121" s="13"/>
+      <c r="H121" s="13"/>
+      <c r="I121" s="32"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122" s="27"/>
+      <c r="B122" s="29"/>
+      <c r="C122" s="30"/>
+      <c r="D122" s="30"/>
+      <c r="E122" s="32"/>
+      <c r="F122" s="13"/>
+      <c r="G122" s="13"/>
+      <c r="H122" s="13"/>
+      <c r="I122" s="32"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123" s="27"/>
+      <c r="B123" s="29"/>
+      <c r="C123" s="30"/>
+      <c r="D123" s="30"/>
+      <c r="E123" s="32"/>
+      <c r="F123" s="13"/>
+      <c r="G123" s="13"/>
+      <c r="H123" s="13"/>
+      <c r="I123" s="32"/>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A124" s="27"/>
+      <c r="B124" s="30"/>
+      <c r="C124" s="30"/>
+      <c r="D124" s="30"/>
+      <c r="E124" s="32"/>
+      <c r="F124" s="13"/>
+      <c r="G124" s="13"/>
+      <c r="H124" s="13"/>
+      <c r="I124" s="32"/>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A125" s="27"/>
+      <c r="B125" s="30"/>
+      <c r="C125" s="30"/>
+      <c r="D125" s="30"/>
+      <c r="E125" s="32"/>
+      <c r="F125" s="13"/>
+      <c r="G125" s="13"/>
+      <c r="H125" s="13"/>
+      <c r="I125" s="32"/>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126" s="27"/>
+      <c r="B126" s="29"/>
+      <c r="C126" s="30"/>
+      <c r="D126" s="30"/>
+      <c r="E126" s="32"/>
+      <c r="F126" s="13"/>
+      <c r="G126" s="13"/>
+      <c r="H126" s="13"/>
+      <c r="I126" s="32"/>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A127" s="27"/>
+      <c r="B127" s="15"/>
+      <c r="C127" s="30"/>
+      <c r="D127" s="30"/>
+      <c r="E127" s="32"/>
+      <c r="F127" s="13"/>
+      <c r="G127" s="13"/>
+      <c r="H127" s="13"/>
+      <c r="I127" s="32"/>
+    </row>
+    <row r="128" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="A128" s="38"/>
+      <c r="B128" s="45"/>
+      <c r="C128" s="45"/>
+      <c r="D128" s="45"/>
+      <c r="E128" s="45"/>
+      <c r="F128" s="45"/>
+      <c r="G128" s="45"/>
+      <c r="H128" s="45"/>
+      <c r="I128" s="45"/>
+    </row>
+    <row r="129" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="A129" s="47"/>
+      <c r="B129" s="46"/>
+      <c r="C129" s="46"/>
+      <c r="D129" s="46"/>
+      <c r="E129" s="46"/>
+      <c r="F129" s="46"/>
+      <c r="G129" s="46"/>
+      <c r="H129" s="46"/>
+      <c r="I129" s="46"/>
+    </row>
+    <row r="130" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="27">
+        <f ca="1">IF(OFFSET(A130,-1,0) ="",OFFSET(A130,-2,0)+1,OFFSET(A130,-1,0)+1 )</f>
+        <v>1</v>
+      </c>
+      <c r="B130" s="30" t="s">
+        <v>400</v>
+      </c>
+      <c r="C130" s="30"/>
+      <c r="D130" s="30"/>
+      <c r="E130" s="32"/>
+      <c r="F130" s="13"/>
+      <c r="G130" s="13"/>
+      <c r="H130" s="13"/>
+      <c r="I130" s="32"/>
+    </row>
+    <row r="131" spans="1:9" ht="26.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="27">
+        <f ca="1">IF(OFFSET(A131,-1,0) ="",OFFSET(A131,-2,0)+1,OFFSET(A131,-1,0)+1 )</f>
+        <v>2</v>
+      </c>
+      <c r="B131" s="30" t="s">
+        <v>398</v>
+      </c>
+      <c r="C131" s="30"/>
+      <c r="D131" s="30"/>
+      <c r="E131" s="32"/>
+      <c r="F131" s="13"/>
+      <c r="G131" s="13"/>
+      <c r="H131" s="13"/>
+      <c r="I131" s="32"/>
+    </row>
+    <row r="132" spans="1:9" ht="21.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="27">
+        <f ca="1">IF(OFFSET(A132,-1,0) ="",OFFSET(A132,-2,0)+1,OFFSET(A132,-1,0)+1 )</f>
+        <v>3</v>
+      </c>
+      <c r="B132" s="30" t="s">
+        <v>399</v>
+      </c>
+      <c r="C132" s="30"/>
+      <c r="D132" s="30"/>
+      <c r="E132" s="32"/>
+      <c r="F132" s="13"/>
+      <c r="G132" s="13"/>
+      <c r="H132" s="13"/>
+      <c r="I132" s="32"/>
+    </row>
+    <row r="133" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="27">
+        <f ca="1">IF(OFFSET(A133,-1,0) ="",OFFSET(A133,-2,0)+1,OFFSET(A133,-1,0)+1 )</f>
+        <v>4</v>
+      </c>
+      <c r="B133" s="30" t="s">
+        <v>401</v>
+      </c>
+      <c r="C133" s="30"/>
+      <c r="D133" s="30"/>
+      <c r="E133" s="32"/>
+      <c r="F133" s="13"/>
+      <c r="G133" s="13"/>
+      <c r="H133" s="13"/>
+      <c r="I133" s="32"/>
+    </row>
+    <row r="134" spans="1:9" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="27">
+        <f ca="1">IF(OFFSET(A134,-1,0) ="",OFFSET(A134,-2,0)+1,OFFSET(A134,-1,0)+1 )</f>
+        <v>5</v>
+      </c>
+      <c r="B134" s="30" t="s">
+        <v>402</v>
+      </c>
+      <c r="C134" s="30"/>
+      <c r="D134" s="30"/>
+      <c r="E134" s="30"/>
+      <c r="F134" s="13"/>
+      <c r="G134" s="13"/>
+      <c r="H134" s="13"/>
+      <c r="I134" s="32"/>
+    </row>
+    <row r="135" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="27">
+        <f ca="1">IF(OFFSET(A135,-1,0) ="",OFFSET(A135,-2,0)+1,OFFSET(A135,-1,0)+1 )</f>
+        <v>6</v>
+      </c>
+      <c r="B135" s="30" t="s">
+        <v>403</v>
+      </c>
+      <c r="C135" s="30"/>
+      <c r="D135" s="30"/>
+      <c r="E135" s="32"/>
+      <c r="F135" s="13"/>
+      <c r="G135" s="13"/>
+      <c r="H135" s="13"/>
+      <c r="I135" s="32"/>
+    </row>
+    <row r="136" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="27">
+        <f ca="1">IF(OFFSET(A136,-1,0) ="",OFFSET(A136,-2,0)+1,OFFSET(A136,-1,0)+1 )</f>
+        <v>7</v>
+      </c>
+      <c r="B136" s="30" t="s">
+        <v>404</v>
+      </c>
+      <c r="C136" s="30"/>
+      <c r="D136" s="30"/>
+      <c r="E136" s="32"/>
+      <c r="F136" s="13"/>
+      <c r="G136" s="13"/>
+      <c r="H136" s="13"/>
+      <c r="I136" s="32"/>
+    </row>
+    <row r="137" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="27">
+        <f ca="1">IF(OFFSET(A137,-1,0) ="",OFFSET(A137,-2,0)+1,OFFSET(A137,-1,0)+1 )</f>
+        <v>8</v>
+      </c>
+      <c r="B137" s="30" t="s">
+        <v>413</v>
+      </c>
+      <c r="C137" s="30"/>
+      <c r="D137" s="30"/>
+      <c r="E137" s="32"/>
+      <c r="F137" s="13"/>
+      <c r="G137" s="13"/>
+      <c r="H137" s="13"/>
+      <c r="I137" s="32"/>
+    </row>
+    <row r="138" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="27">
+        <f ca="1">IF(OFFSET(A138,-1,0) ="",OFFSET(A138,-2,0)+1,OFFSET(A138,-1,0)+1 )</f>
+        <v>9</v>
+      </c>
+      <c r="B138" s="30" t="s">
+        <v>414</v>
+      </c>
+      <c r="C138" s="30"/>
+      <c r="D138" s="30"/>
+      <c r="E138" s="32"/>
+      <c r="F138" s="13"/>
+      <c r="G138" s="13"/>
+      <c r="H138" s="13"/>
+      <c r="I138" s="32"/>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A139" s="27"/>
+      <c r="B139" s="29"/>
+      <c r="C139" s="30"/>
+      <c r="D139" s="30"/>
+      <c r="E139" s="32"/>
+      <c r="F139" s="13"/>
+      <c r="G139" s="13"/>
+      <c r="H139" s="13"/>
+      <c r="I139" s="32"/>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A140" s="27"/>
+      <c r="B140" s="29"/>
+      <c r="C140" s="30"/>
+      <c r="D140" s="30"/>
+      <c r="E140" s="32"/>
+      <c r="F140" s="13"/>
+      <c r="G140" s="13"/>
+      <c r="H140" s="13"/>
+      <c r="I140" s="32"/>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A141" s="27"/>
+      <c r="B141" s="29"/>
+      <c r="C141" s="30"/>
+      <c r="D141" s="30"/>
+      <c r="E141" s="32"/>
+      <c r="F141" s="13"/>
+      <c r="G141" s="13"/>
+      <c r="H141" s="13"/>
+      <c r="I141" s="32"/>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A142" s="27"/>
+      <c r="B142" s="29"/>
+      <c r="C142" s="30"/>
+      <c r="D142" s="30"/>
+      <c r="E142" s="32"/>
+      <c r="F142" s="13"/>
+      <c r="G142" s="13"/>
+      <c r="H142" s="13"/>
+      <c r="I142" s="32"/>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A143" s="27"/>
+      <c r="B143" s="29"/>
+      <c r="C143" s="30"/>
+      <c r="D143" s="30"/>
+      <c r="E143" s="32"/>
+      <c r="F143" s="13"/>
+      <c r="G143" s="13"/>
+      <c r="H143" s="13"/>
+      <c r="I143" s="32"/>
+    </row>
+    <row r="149" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="A149" s="48"/>
+      <c r="B149" s="49"/>
+      <c r="C149" s="49"/>
+      <c r="D149" s="49"/>
+      <c r="E149" s="49"/>
+      <c r="F149" s="49"/>
+      <c r="G149" s="49"/>
+      <c r="H149" s="49"/>
+      <c r="I149" s="50"/>
+    </row>
+    <row r="150" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="A150" s="38"/>
+      <c r="B150" s="45"/>
+      <c r="C150" s="45"/>
+      <c r="D150" s="45"/>
+      <c r="E150" s="45"/>
+      <c r="F150" s="45"/>
+      <c r="G150" s="45"/>
+      <c r="H150" s="45"/>
+      <c r="I150" s="45"/>
+    </row>
+    <row r="151" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="A151" s="47"/>
+      <c r="B151" s="46"/>
+      <c r="C151" s="46"/>
+      <c r="D151" s="46"/>
+      <c r="E151" s="46"/>
+      <c r="F151" s="46"/>
+      <c r="G151" s="46"/>
+      <c r="H151" s="46"/>
+      <c r="I151" s="46"/>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A152" s="27"/>
+      <c r="B152" s="30"/>
+      <c r="C152" s="30"/>
+      <c r="D152" s="30"/>
+      <c r="E152" s="32"/>
+      <c r="F152" s="13"/>
+      <c r="G152" s="13"/>
+      <c r="H152" s="13"/>
+      <c r="I152" s="32"/>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A153" s="27"/>
+      <c r="B153" s="12"/>
+      <c r="C153" s="30"/>
+      <c r="D153" s="30"/>
+      <c r="E153" s="32"/>
+      <c r="F153" s="13"/>
+      <c r="G153" s="13"/>
+      <c r="H153" s="13"/>
+      <c r="I153" s="32"/>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A154" s="27"/>
+      <c r="B154" s="15"/>
+      <c r="C154" s="30"/>
+      <c r="D154" s="30"/>
+      <c r="E154" s="32"/>
+      <c r="F154" s="13"/>
+      <c r="G154" s="13"/>
+      <c r="H154" s="13"/>
+      <c r="I154" s="32"/>
+    </row>
+    <row r="155" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="A155" s="47"/>
+      <c r="B155" s="46"/>
+      <c r="C155" s="46"/>
+      <c r="D155" s="46"/>
+      <c r="E155" s="46"/>
+      <c r="F155" s="46"/>
+      <c r="G155" s="46"/>
+      <c r="H155" s="46"/>
+      <c r="I155" s="46"/>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A156" s="27"/>
+      <c r="B156" s="30"/>
+      <c r="C156" s="30"/>
+      <c r="D156" s="30"/>
+      <c r="E156" s="32"/>
+      <c r="F156" s="13"/>
+      <c r="G156" s="13"/>
+      <c r="H156" s="13"/>
+      <c r="I156" s="32"/>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A157" s="27"/>
+      <c r="B157" s="30"/>
+      <c r="C157" s="30"/>
+      <c r="D157" s="30"/>
+      <c r="E157" s="32"/>
+      <c r="F157" s="13"/>
+      <c r="G157" s="13"/>
+      <c r="H157" s="13"/>
+      <c r="I157" s="32"/>
+    </row>
+    <row r="158" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="A158" s="47"/>
+      <c r="B158" s="46"/>
+      <c r="C158" s="46"/>
+      <c r="D158" s="46"/>
+      <c r="E158" s="46"/>
+      <c r="F158" s="46"/>
+      <c r="G158" s="46"/>
+      <c r="H158" s="46"/>
+      <c r="I158" s="46"/>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A159" s="27"/>
+      <c r="B159" s="30"/>
+      <c r="C159" s="30"/>
+      <c r="D159" s="30"/>
+      <c r="E159" s="32"/>
+      <c r="F159" s="13"/>
+      <c r="G159" s="13"/>
+      <c r="H159" s="13"/>
+      <c r="I159" s="32"/>
+    </row>
+    <row r="160" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="A160" s="47"/>
+      <c r="B160" s="46"/>
+      <c r="C160" s="46"/>
+      <c r="D160" s="46"/>
+      <c r="E160" s="46"/>
+      <c r="F160" s="46"/>
+      <c r="G160" s="46"/>
+      <c r="H160" s="46"/>
+      <c r="I160" s="46"/>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A161" s="27"/>
+      <c r="B161" s="30"/>
+      <c r="C161" s="30"/>
+      <c r="D161" s="30"/>
+      <c r="E161" s="32"/>
+      <c r="F161" s="13"/>
+      <c r="G161" s="13"/>
+      <c r="H161" s="13"/>
+      <c r="I161" s="32"/>
+    </row>
+    <row r="162" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="A162" s="47"/>
+      <c r="B162" s="46"/>
+      <c r="C162" s="46"/>
+      <c r="D162" s="46"/>
+      <c r="E162" s="46"/>
+      <c r="F162" s="46"/>
+      <c r="G162" s="46"/>
+      <c r="H162" s="46"/>
+      <c r="I162" s="46"/>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A163" s="27"/>
+      <c r="B163" s="30"/>
+      <c r="C163" s="30"/>
+      <c r="D163" s="30"/>
+      <c r="E163" s="32"/>
+      <c r="F163" s="13"/>
+      <c r="G163" s="13"/>
+      <c r="H163" s="13"/>
+      <c r="I163" s="32"/>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A164" s="27"/>
+      <c r="B164" s="30"/>
+      <c r="C164" s="30"/>
+      <c r="D164" s="30"/>
+      <c r="E164" s="32"/>
+      <c r="F164" s="13"/>
+      <c r="G164" s="13"/>
+      <c r="H164" s="13"/>
+      <c r="I164" s="32"/>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A165" s="27"/>
+      <c r="B165" s="30"/>
+      <c r="C165" s="30"/>
+      <c r="D165" s="30"/>
+      <c r="E165" s="32"/>
+      <c r="F165" s="13"/>
+      <c r="G165" s="13"/>
+      <c r="H165" s="13"/>
+      <c r="I165" s="32"/>
+    </row>
+    <row r="166" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="A166" s="47"/>
+      <c r="B166" s="46"/>
+      <c r="C166" s="46"/>
+      <c r="D166" s="46"/>
+      <c r="E166" s="46"/>
+      <c r="F166" s="46"/>
+      <c r="G166" s="46"/>
+      <c r="H166" s="46"/>
+      <c r="I166" s="46"/>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A167" s="27"/>
+      <c r="B167" s="30"/>
+      <c r="C167" s="30"/>
+      <c r="D167" s="30"/>
+      <c r="E167" s="32"/>
+      <c r="F167" s="13"/>
+      <c r="G167" s="13"/>
+      <c r="H167" s="13"/>
+      <c r="I167" s="32"/>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A168" s="27"/>
+      <c r="B168" s="30"/>
+      <c r="C168" s="30"/>
+      <c r="D168" s="30"/>
+      <c r="E168" s="32"/>
+      <c r="F168" s="13"/>
+      <c r="G168" s="13"/>
+      <c r="H168" s="13"/>
+      <c r="I168" s="32"/>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A169" s="27"/>
+      <c r="B169" s="30"/>
+      <c r="C169" s="30"/>
+      <c r="D169" s="30"/>
+      <c r="E169" s="32"/>
+      <c r="F169" s="13"/>
+      <c r="G169" s="13"/>
+      <c r="H169" s="13"/>
+      <c r="I169" s="32"/>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A170" s="27"/>
+      <c r="B170" s="30"/>
+      <c r="C170" s="30"/>
+      <c r="D170" s="30"/>
+      <c r="E170" s="32"/>
+      <c r="F170" s="13"/>
+      <c r="G170" s="13"/>
+      <c r="H170" s="13"/>
+      <c r="I170" s="32"/>
+    </row>
+    <row r="171" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="A171" s="47"/>
+      <c r="B171" s="46"/>
+      <c r="C171" s="46"/>
+      <c r="D171" s="46"/>
+      <c r="E171" s="46"/>
+      <c r="F171" s="46"/>
+      <c r="G171" s="46"/>
+      <c r="H171" s="46"/>
+      <c r="I171" s="46"/>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A172" s="27"/>
+      <c r="B172" s="30"/>
+      <c r="C172" s="30"/>
+      <c r="D172" s="30"/>
+      <c r="E172" s="32"/>
+      <c r="F172" s="13"/>
+      <c r="G172" s="13"/>
+      <c r="H172" s="13"/>
+      <c r="I172" s="32"/>
+    </row>
+    <row r="173" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="A173" s="47"/>
+      <c r="B173" s="46"/>
+      <c r="C173" s="46"/>
+      <c r="D173" s="46"/>
+      <c r="E173" s="46"/>
+      <c r="F173" s="46"/>
+      <c r="G173" s="46"/>
+      <c r="H173" s="46"/>
+      <c r="I173" s="46"/>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A174" s="27"/>
+      <c r="B174" s="30"/>
+      <c r="C174" s="30"/>
+      <c r="D174" s="30"/>
+      <c r="E174" s="32"/>
+      <c r="F174" s="13"/>
+      <c r="G174" s="13"/>
+      <c r="H174" s="13"/>
+      <c r="I174" s="32"/>
+    </row>
+    <row r="175" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="A175" s="47"/>
+      <c r="B175" s="46"/>
+      <c r="C175" s="46"/>
+      <c r="D175" s="46"/>
+      <c r="E175" s="46"/>
+      <c r="F175" s="46"/>
+      <c r="G175" s="46"/>
+      <c r="H175" s="46"/>
+      <c r="I175" s="46"/>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A176" s="27"/>
+      <c r="B176" s="30"/>
+      <c r="C176" s="30"/>
+      <c r="D176" s="30"/>
+      <c r="E176" s="32"/>
+      <c r="F176" s="13"/>
+      <c r="G176" s="13"/>
+      <c r="H176" s="13"/>
+      <c r="I176" s="32"/>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A177" s="27"/>
+      <c r="B177" s="30"/>
+      <c r="C177" s="30"/>
+      <c r="D177" s="30"/>
+      <c r="E177" s="32"/>
+      <c r="F177" s="13"/>
+      <c r="G177" s="13"/>
+      <c r="H177" s="13"/>
+      <c r="I177" s="32"/>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A178" s="27"/>
+      <c r="B178" s="30"/>
+      <c r="C178" s="30"/>
+      <c r="D178" s="30"/>
+      <c r="E178" s="32"/>
+      <c r="F178" s="13"/>
+      <c r="G178" s="13"/>
+      <c r="H178" s="13"/>
+      <c r="I178" s="32"/>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A179" s="27"/>
+      <c r="B179" s="15"/>
+      <c r="C179" s="30"/>
+      <c r="D179" s="30"/>
+      <c r="E179" s="32"/>
+      <c r="F179" s="13"/>
+      <c r="G179" s="13"/>
+      <c r="H179" s="13"/>
+      <c r="I179" s="32"/>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A180" s="27"/>
+      <c r="B180" s="15"/>
+      <c r="C180" s="30"/>
+      <c r="D180" s="30"/>
+      <c r="E180" s="32"/>
+      <c r="F180" s="13"/>
+      <c r="G180" s="13"/>
+      <c r="H180" s="13"/>
+      <c r="I180" s="32"/>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A181" s="27"/>
+      <c r="B181" s="15"/>
+      <c r="C181" s="30"/>
+      <c r="D181" s="30"/>
+      <c r="E181" s="32"/>
+      <c r="F181" s="13"/>
+      <c r="G181" s="13"/>
+      <c r="H181" s="13"/>
+      <c r="I181" s="32"/>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A182" s="27"/>
+      <c r="B182" s="15"/>
+      <c r="C182" s="30"/>
+      <c r="D182" s="30"/>
+      <c r="E182" s="32"/>
+      <c r="F182" s="13"/>
+      <c r="G182" s="13"/>
+      <c r="H182" s="13"/>
+      <c r="I182" s="32"/>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A183" s="27"/>
+      <c r="B183" s="15"/>
+      <c r="C183" s="30"/>
+      <c r="D183" s="30"/>
+      <c r="E183" s="32"/>
+      <c r="F183" s="13"/>
+      <c r="G183" s="13"/>
+      <c r="H183" s="13"/>
+      <c r="I183" s="32"/>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A184" s="27"/>
+      <c r="B184" s="15"/>
+      <c r="C184" s="30"/>
+      <c r="D184" s="30"/>
+      <c r="E184" s="32"/>
+      <c r="F184" s="13"/>
+      <c r="G184" s="13"/>
+      <c r="H184" s="13"/>
+      <c r="I184" s="32"/>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A185" s="27"/>
+      <c r="B185" s="30"/>
+      <c r="C185" s="30"/>
+      <c r="D185" s="30"/>
+      <c r="E185" s="32"/>
+      <c r="F185" s="13"/>
+      <c r="G185" s="13"/>
+      <c r="H185" s="13"/>
+      <c r="I185" s="32"/>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A186" s="27"/>
+      <c r="B186" s="30"/>
+      <c r="C186" s="30"/>
+      <c r="D186" s="30"/>
+      <c r="E186" s="32"/>
+      <c r="F186" s="13"/>
+      <c r="G186" s="13"/>
+      <c r="H186" s="13"/>
+      <c r="I186" s="32"/>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A187" s="27"/>
+      <c r="B187" s="30"/>
+      <c r="C187" s="30"/>
+      <c r="D187" s="30"/>
+      <c r="E187" s="32"/>
+      <c r="F187" s="13"/>
+      <c r="G187" s="13"/>
+      <c r="H187" s="13"/>
+      <c r="I187" s="32"/>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A188" s="27"/>
+      <c r="B188" s="30"/>
+      <c r="C188" s="30"/>
+      <c r="D188" s="30"/>
+      <c r="E188" s="32"/>
+      <c r="F188" s="13"/>
+      <c r="G188" s="13"/>
+      <c r="H188" s="13"/>
+      <c r="I188" s="32"/>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A189" s="27"/>
+      <c r="B189" s="30"/>
+      <c r="C189" s="30"/>
+      <c r="D189" s="30"/>
+      <c r="E189" s="32"/>
+      <c r="F189" s="13"/>
+      <c r="G189" s="13"/>
+      <c r="H189" s="13"/>
+      <c r="I189" s="32"/>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A190" s="27"/>
+      <c r="B190" s="30"/>
+      <c r="C190" s="30"/>
+      <c r="D190" s="30"/>
+      <c r="E190" s="32"/>
+      <c r="F190" s="13"/>
+      <c r="G190" s="13"/>
+      <c r="H190" s="13"/>
+      <c r="I190" s="32"/>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A191" s="27"/>
+      <c r="B191" s="30"/>
+      <c r="C191" s="30"/>
+      <c r="D191" s="30"/>
+      <c r="E191" s="32"/>
+      <c r="F191" s="13"/>
+      <c r="G191" s="13"/>
+      <c r="H191" s="13"/>
+      <c r="I191" s="32"/>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A192" s="27"/>
+      <c r="B192" s="30"/>
+      <c r="C192" s="30"/>
+      <c r="D192" s="30"/>
+      <c r="E192" s="32"/>
+      <c r="F192" s="13"/>
+      <c r="G192" s="13"/>
+      <c r="H192" s="13"/>
+      <c r="I192" s="32"/>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A193" s="27"/>
+      <c r="B193" s="30"/>
+      <c r="C193" s="30"/>
+      <c r="D193" s="30"/>
+      <c r="E193" s="32"/>
+      <c r="F193" s="13"/>
+      <c r="G193" s="13"/>
+      <c r="H193" s="13"/>
+      <c r="I193" s="32"/>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A194" s="27"/>
+      <c r="B194" s="30"/>
+      <c r="C194" s="30"/>
+      <c r="D194" s="30"/>
+      <c r="E194" s="32"/>
+      <c r="F194" s="13"/>
+      <c r="G194" s="13"/>
+      <c r="H194" s="13"/>
+      <c r="I194" s="32"/>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A195" s="27"/>
+      <c r="B195" s="30"/>
+      <c r="C195" s="30"/>
+      <c r="D195" s="30"/>
+      <c r="E195" s="32"/>
+      <c r="F195" s="13"/>
+      <c r="G195" s="13"/>
+      <c r="H195" s="13"/>
+      <c r="I195" s="32"/>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A196" s="27"/>
+      <c r="B196" s="30"/>
+      <c r="C196" s="30"/>
+      <c r="D196" s="30"/>
+      <c r="E196" s="32"/>
+      <c r="F196" s="13"/>
+      <c r="G196" s="13"/>
+      <c r="H196" s="13"/>
+      <c r="I196" s="32"/>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A197" s="27"/>
+      <c r="B197" s="30"/>
+      <c r="C197" s="30"/>
+      <c r="D197" s="30"/>
+      <c r="E197" s="32"/>
+      <c r="F197" s="13"/>
+      <c r="G197" s="13"/>
+      <c r="H197" s="13"/>
+      <c r="I197" s="32"/>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A198" s="27"/>
+      <c r="B198" s="30"/>
+      <c r="C198" s="30"/>
+      <c r="D198" s="30"/>
+      <c r="E198" s="32"/>
+      <c r="F198" s="13"/>
+      <c r="G198" s="13"/>
+      <c r="H198" s="13"/>
+      <c r="I198" s="32"/>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A199" s="27"/>
+      <c r="B199" s="30"/>
+      <c r="C199" s="30"/>
+      <c r="D199" s="30"/>
+      <c r="E199" s="32"/>
+      <c r="F199" s="13"/>
+      <c r="G199" s="13"/>
+      <c r="H199" s="13"/>
+      <c r="I199" s="32"/>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A200" s="27"/>
+      <c r="B200" s="30"/>
+      <c r="C200" s="30"/>
+      <c r="D200" s="30"/>
+      <c r="E200" s="32"/>
+      <c r="F200" s="13"/>
+      <c r="G200" s="13"/>
+      <c r="H200" s="13"/>
+      <c r="I200" s="32"/>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A201" s="27"/>
+      <c r="B201" s="30"/>
+      <c r="C201" s="30"/>
+      <c r="D201" s="30"/>
+      <c r="E201" s="32"/>
+      <c r="F201" s="13"/>
+      <c r="G201" s="13"/>
+      <c r="H201" s="13"/>
+      <c r="I201" s="32"/>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A202" s="27"/>
+      <c r="B202" s="30"/>
+      <c r="C202" s="30"/>
+      <c r="D202" s="30"/>
+      <c r="E202" s="32"/>
+      <c r="F202" s="13"/>
+      <c r="G202" s="13"/>
+      <c r="H202" s="13"/>
+      <c r="I202" s="32"/>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A203" s="27"/>
+      <c r="B203" s="30"/>
+      <c r="C203" s="30"/>
+      <c r="D203" s="30"/>
+      <c r="E203" s="32"/>
+      <c r="F203" s="13"/>
+      <c r="G203" s="13"/>
+      <c r="H203" s="13"/>
+      <c r="I203" s="32"/>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A204" s="27"/>
+      <c r="B204" s="30"/>
+      <c r="C204" s="30"/>
+      <c r="D204" s="30"/>
+      <c r="E204" s="32"/>
+      <c r="F204" s="13"/>
+      <c r="G204" s="13"/>
+      <c r="H204" s="13"/>
+      <c r="I204" s="32"/>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A205" s="27"/>
+      <c r="B205" s="30"/>
+      <c r="C205" s="30"/>
+      <c r="D205" s="30"/>
+      <c r="E205" s="32"/>
+      <c r="F205" s="13"/>
+      <c r="G205" s="13"/>
+      <c r="H205" s="13"/>
+      <c r="I205" s="32"/>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A206" s="27"/>
+      <c r="B206" s="30"/>
+      <c r="C206" s="30"/>
+      <c r="D206" s="30"/>
+      <c r="E206" s="32"/>
+      <c r="F206" s="13"/>
+      <c r="G206" s="13"/>
+      <c r="H206" s="13"/>
+      <c r="I206" s="32"/>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A207" s="27"/>
+      <c r="B207" s="30"/>
+      <c r="C207" s="30"/>
+      <c r="D207" s="30"/>
+      <c r="E207" s="32"/>
+      <c r="F207" s="13"/>
+      <c r="G207" s="13"/>
+      <c r="H207" s="13"/>
+      <c r="I207" s="32"/>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A208" s="27"/>
+      <c r="B208" s="30"/>
+      <c r="C208" s="30"/>
+      <c r="D208" s="30"/>
+      <c r="E208" s="32"/>
+      <c r="F208" s="13"/>
+      <c r="G208" s="13"/>
+      <c r="H208" s="13"/>
+      <c r="I208" s="32"/>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A209" s="27"/>
+      <c r="B209" s="30"/>
+      <c r="C209" s="30"/>
+      <c r="D209" s="30"/>
+      <c r="E209" s="32"/>
+      <c r="F209" s="13"/>
+      <c r="G209" s="13"/>
+      <c r="H209" s="13"/>
+      <c r="I209" s="32"/>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A210" s="27"/>
+      <c r="B210" s="30"/>
+      <c r="C210" s="30"/>
+      <c r="D210" s="30"/>
+      <c r="E210" s="32"/>
+      <c r="F210" s="13"/>
+      <c r="G210" s="13"/>
+      <c r="H210" s="13"/>
+      <c r="I210" s="32"/>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A211" s="27"/>
+      <c r="B211" s="30"/>
+      <c r="C211" s="30"/>
+      <c r="D211" s="30"/>
+      <c r="E211" s="32"/>
+      <c r="F211" s="13"/>
+      <c r="G211" s="13"/>
+      <c r="H211" s="13"/>
+      <c r="I211" s="32"/>
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A212" s="27"/>
+      <c r="B212" s="30"/>
+      <c r="C212" s="30"/>
+      <c r="D212" s="30"/>
+      <c r="E212" s="32"/>
+      <c r="F212" s="13"/>
+      <c r="G212" s="13"/>
+      <c r="H212" s="13"/>
+      <c r="I212" s="32"/>
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A213" s="27"/>
+      <c r="B213" s="30"/>
+      <c r="C213" s="30"/>
+      <c r="D213" s="30"/>
+      <c r="E213" s="32"/>
+      <c r="F213" s="13"/>
+      <c r="G213" s="13"/>
+      <c r="H213" s="13"/>
+      <c r="I213" s="32"/>
+    </row>
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A214" s="27"/>
+      <c r="B214" s="30"/>
+      <c r="C214" s="30"/>
+      <c r="D214" s="30"/>
+      <c r="E214" s="32"/>
+      <c r="F214" s="13"/>
+      <c r="G214" s="13"/>
+      <c r="H214" s="13"/>
+      <c r="I214" s="32"/>
+    </row>
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A215" s="27"/>
+      <c r="B215" s="30"/>
+      <c r="C215" s="30"/>
+      <c r="D215" s="30"/>
+      <c r="E215" s="32"/>
+      <c r="F215" s="13"/>
+      <c r="G215" s="13"/>
+      <c r="H215" s="13"/>
+      <c r="I215" s="32"/>
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A216" s="27"/>
+      <c r="B216" s="30"/>
+      <c r="C216" s="30"/>
+      <c r="D216" s="30"/>
+      <c r="E216" s="32"/>
+      <c r="F216" s="13"/>
+      <c r="G216" s="13"/>
+      <c r="H216" s="13"/>
+      <c r="I216" s="32"/>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A217" s="27"/>
+      <c r="B217" s="30"/>
+      <c r="C217" s="30"/>
+      <c r="D217" s="30"/>
+      <c r="E217" s="32"/>
+      <c r="F217" s="13"/>
+      <c r="G217" s="13"/>
+      <c r="H217" s="13"/>
+      <c r="I217" s="32"/>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A218" s="27"/>
+      <c r="B218" s="30"/>
+      <c r="C218" s="30"/>
+      <c r="D218" s="30"/>
+      <c r="E218" s="32"/>
+      <c r="F218" s="13"/>
+      <c r="G218" s="13"/>
+      <c r="H218" s="13"/>
+      <c r="I218" s="32"/>
+    </row>
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A219" s="27"/>
+      <c r="B219" s="30"/>
+      <c r="C219" s="30"/>
+      <c r="D219" s="30"/>
+      <c r="E219" s="32"/>
+      <c r="F219" s="13"/>
+      <c r="G219" s="13"/>
+      <c r="H219" s="13"/>
+      <c r="I219" s="32"/>
+    </row>
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A220" s="27"/>
+      <c r="B220" s="30"/>
+      <c r="C220" s="30"/>
+      <c r="D220" s="30"/>
+      <c r="E220" s="32"/>
+      <c r="F220" s="13"/>
+      <c r="G220" s="13"/>
+      <c r="H220" s="13"/>
+      <c r="I220" s="32"/>
+    </row>
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A221" s="27"/>
+      <c r="B221" s="30"/>
+      <c r="C221" s="30"/>
+      <c r="D221" s="30"/>
+      <c r="E221" s="32"/>
+      <c r="F221" s="13"/>
+      <c r="G221" s="13"/>
+      <c r="H221" s="13"/>
+      <c r="I221" s="32"/>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A222" s="27"/>
+      <c r="B222" s="30"/>
+      <c r="C222" s="30"/>
+      <c r="D222" s="30"/>
+      <c r="E222" s="32"/>
+      <c r="F222" s="13"/>
+      <c r="G222" s="13"/>
+      <c r="H222" s="13"/>
+      <c r="I222" s="32"/>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A223" s="27"/>
+      <c r="B223" s="30"/>
+      <c r="C223" s="30"/>
+      <c r="D223" s="30"/>
+      <c r="E223" s="32"/>
+      <c r="F223" s="13"/>
+      <c r="G223" s="13"/>
+      <c r="H223" s="13"/>
+      <c r="I223" s="32"/>
+    </row>
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A224" s="27"/>
+      <c r="B224" s="30"/>
+      <c r="C224" s="30"/>
+      <c r="D224" s="30"/>
+      <c r="E224" s="32"/>
+      <c r="F224" s="13"/>
+      <c r="G224" s="13"/>
+      <c r="H224" s="13"/>
+      <c r="I224" s="32"/>
+    </row>
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A225" s="27"/>
+      <c r="B225" s="30"/>
+      <c r="C225" s="30"/>
+      <c r="D225" s="30"/>
+      <c r="E225" s="32"/>
+      <c r="F225" s="13"/>
+      <c r="G225" s="13"/>
+      <c r="H225" s="13"/>
+      <c r="I225" s="32"/>
+    </row>
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A226" s="27"/>
+      <c r="B226" s="30"/>
+      <c r="C226" s="30"/>
+      <c r="D226" s="30"/>
+      <c r="E226" s="32"/>
+      <c r="F226" s="13"/>
+      <c r="G226" s="13"/>
+      <c r="H226" s="13"/>
+      <c r="I226" s="32"/>
+    </row>
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A227" s="27"/>
+      <c r="B227" s="30"/>
+      <c r="C227" s="30"/>
+      <c r="D227" s="30"/>
+      <c r="E227" s="32"/>
+      <c r="F227" s="13"/>
+      <c r="G227" s="13"/>
+      <c r="H227" s="13"/>
+      <c r="I227" s="32"/>
+    </row>
+    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A228" s="27"/>
+      <c r="B228" s="30"/>
+      <c r="C228" s="30"/>
+      <c r="D228" s="30"/>
+      <c r="E228" s="32"/>
+      <c r="F228" s="13"/>
+      <c r="G228" s="13"/>
+      <c r="H228" s="13"/>
+      <c r="I228" s="32"/>
+    </row>
+    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A229" s="27"/>
+      <c r="B229" s="30"/>
+      <c r="C229" s="30"/>
+      <c r="D229" s="30"/>
+      <c r="E229" s="32"/>
+      <c r="F229" s="13"/>
+      <c r="G229" s="13"/>
+      <c r="H229" s="13"/>
+      <c r="I229" s="32"/>
+    </row>
+    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A230" s="27"/>
+      <c r="B230" s="30"/>
+      <c r="C230" s="30"/>
+      <c r="D230" s="30"/>
+      <c r="E230" s="32"/>
+      <c r="F230" s="13"/>
+      <c r="G230" s="13"/>
+      <c r="H230" s="13"/>
+      <c r="I230" s="32"/>
+    </row>
+    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A231" s="27"/>
+      <c r="B231" s="30"/>
+      <c r="C231" s="30"/>
+      <c r="D231" s="30"/>
+      <c r="E231" s="32"/>
+      <c r="F231" s="13"/>
+      <c r="G231" s="13"/>
+      <c r="H231" s="13"/>
+      <c r="I231" s="32"/>
+    </row>
+    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A232" s="27"/>
+      <c r="B232" s="30"/>
+      <c r="C232" s="30"/>
+      <c r="D232" s="30"/>
+      <c r="E232" s="32"/>
+      <c r="F232" s="13"/>
+      <c r="G232" s="13"/>
+      <c r="H232" s="13"/>
+      <c r="I232" s="32"/>
+    </row>
+    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A233" s="27"/>
+      <c r="B233" s="30"/>
+      <c r="C233" s="30"/>
+      <c r="D233" s="30"/>
+      <c r="E233" s="32"/>
+      <c r="F233" s="13"/>
+      <c r="G233" s="13"/>
+      <c r="H233" s="13"/>
+      <c r="I233" s="32"/>
+    </row>
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A234" s="27"/>
+      <c r="B234" s="30"/>
+      <c r="C234" s="30"/>
+      <c r="D234" s="30"/>
+      <c r="E234" s="32"/>
+      <c r="F234" s="13"/>
+      <c r="G234" s="13"/>
+      <c r="H234" s="13"/>
+      <c r="I234" s="32"/>
+    </row>
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A235" s="27"/>
+      <c r="B235" s="30"/>
+      <c r="C235" s="30"/>
+      <c r="D235" s="30"/>
+      <c r="E235" s="32"/>
+      <c r="F235" s="13"/>
+      <c r="G235" s="13"/>
+      <c r="H235" s="13"/>
+      <c r="I235" s="32"/>
+    </row>
+    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A236" s="27"/>
+      <c r="B236" s="30"/>
+      <c r="C236" s="30"/>
+      <c r="D236" s="30"/>
+      <c r="E236" s="32"/>
+      <c r="F236" s="13"/>
+      <c r="G236" s="13"/>
+      <c r="H236" s="13"/>
+      <c r="I236" s="32"/>
+    </row>
+    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A237" s="27"/>
+      <c r="B237" s="30"/>
+      <c r="C237" s="30"/>
+      <c r="D237" s="30"/>
+      <c r="E237" s="32"/>
+      <c r="F237" s="13"/>
+      <c r="G237" s="13"/>
+      <c r="H237" s="13"/>
+      <c r="I237" s="32"/>
+    </row>
+    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A238" s="27"/>
+      <c r="B238" s="30"/>
+      <c r="C238" s="30"/>
+      <c r="D238" s="30"/>
+      <c r="E238" s="32"/>
+      <c r="F238" s="13"/>
+      <c r="G238" s="13"/>
+      <c r="H238" s="13"/>
+      <c r="I238" s="32"/>
+    </row>
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A239" s="27"/>
+      <c r="B239" s="30"/>
+      <c r="C239" s="30"/>
+      <c r="D239" s="30"/>
+      <c r="E239" s="32"/>
+      <c r="F239" s="13"/>
+      <c r="G239" s="13"/>
+      <c r="H239" s="13"/>
+      <c r="I239" s="32"/>
+    </row>
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A240" s="27"/>
+      <c r="B240" s="30"/>
+      <c r="C240" s="30"/>
+      <c r="D240" s="30"/>
+      <c r="E240" s="32"/>
+      <c r="F240" s="13"/>
+      <c r="G240" s="13"/>
+      <c r="H240" s="13"/>
+      <c r="I240" s="32"/>
+    </row>
+    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A241" s="27"/>
+      <c r="B241" s="30"/>
+      <c r="C241" s="30"/>
+      <c r="D241" s="30"/>
+      <c r="E241" s="32"/>
+      <c r="F241" s="13"/>
+      <c r="G241" s="13"/>
+      <c r="H241" s="13"/>
+      <c r="I241" s="32"/>
+    </row>
+    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A242" s="27"/>
+      <c r="B242" s="30"/>
+      <c r="C242" s="30"/>
+      <c r="D242" s="30"/>
+      <c r="E242" s="32"/>
+      <c r="F242" s="13"/>
+      <c r="G242" s="13"/>
+      <c r="H242" s="13"/>
+      <c r="I242" s="32"/>
+    </row>
+    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A243" s="27"/>
+      <c r="B243" s="30"/>
+      <c r="C243" s="30"/>
+      <c r="D243" s="30"/>
+      <c r="E243" s="32"/>
+      <c r="F243" s="13"/>
+      <c r="G243" s="13"/>
+      <c r="H243" s="13"/>
+      <c r="I243" s="32"/>
+    </row>
+    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A244" s="27"/>
+      <c r="B244" s="30"/>
+      <c r="C244" s="30"/>
+      <c r="D244" s="30"/>
+      <c r="E244" s="32"/>
+      <c r="F244" s="13"/>
+      <c r="G244" s="13"/>
+      <c r="H244" s="13"/>
+      <c r="I244" s="32"/>
+    </row>
+    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A245" s="27"/>
+      <c r="B245" s="30"/>
+      <c r="C245" s="30"/>
+      <c r="D245" s="30"/>
+      <c r="E245" s="32"/>
+      <c r="F245" s="13"/>
+      <c r="G245" s="13"/>
+      <c r="H245" s="13"/>
+      <c r="I245" s="32"/>
+    </row>
+    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A246" s="27"/>
+      <c r="B246" s="30"/>
+      <c r="C246" s="30"/>
+      <c r="D246" s="30"/>
+      <c r="E246" s="32"/>
+      <c r="F246" s="13"/>
+      <c r="G246" s="13"/>
+      <c r="H246" s="13"/>
+      <c r="I246" s="32"/>
+    </row>
+    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A247" s="27"/>
+      <c r="B247" s="30"/>
+      <c r="C247" s="30"/>
+      <c r="D247" s="30"/>
+      <c r="E247" s="32"/>
+      <c r="F247" s="13"/>
+      <c r="G247" s="13"/>
+      <c r="H247" s="13"/>
+      <c r="I247" s="32"/>
+    </row>
+  </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="A171:I171"/>
+    <mergeCell ref="A173:I173"/>
+    <mergeCell ref="A175:I175"/>
+    <mergeCell ref="A41:I41"/>
+    <mergeCell ref="A60:I60"/>
+    <mergeCell ref="A151:I151"/>
+    <mergeCell ref="A155:I155"/>
+    <mergeCell ref="A158:I158"/>
+    <mergeCell ref="A160:I160"/>
+    <mergeCell ref="A162:I162"/>
+    <mergeCell ref="A166:I166"/>
+    <mergeCell ref="A108:I108"/>
+    <mergeCell ref="A114:I114"/>
+    <mergeCell ref="A128:I128"/>
+    <mergeCell ref="A129:I129"/>
+    <mergeCell ref="A149:I149"/>
+    <mergeCell ref="A150:I150"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A70:I70"/>
+    <mergeCell ref="A91:I91"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added a nunit folder
</commit_message>
<xml_diff>
--- a/Middle Assignment/TestDesignTechique_PhamHongAnh.xlsx
+++ b/Middle Assignment/TestDesignTechique_PhamHongAnh.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NashTech\Rookies\NashTech_Homework\Middle Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE7B92C-2602-439D-BCC6-9E54BBC3E7ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34221520-F4FF-4D5C-80F3-99C67679214D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10" yWindow="20" windowWidth="18710" windowHeight="10000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="20" windowWidth="18710" windowHeight="10000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment 1" sheetId="1" r:id="rId1"/>
@@ -1007,7 +1007,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="475">
   <si>
     <t>ID</t>
   </si>
@@ -2668,6 +2668,18 @@
   </si>
   <si>
     <t>Check when sorting by "Price high to low" works</t>
+  </si>
+  <si>
+    <t>case ký tự đặc biệt</t>
+  </si>
+  <si>
+    <t>Change page thì nội dung ko đổi</t>
+  </si>
+  <si>
+    <t>swap keywords</t>
+  </si>
+  <si>
+    <t>Pass, Not fail</t>
   </si>
 </sst>
 </file>
@@ -15566,8 +15578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{861DB058-9ABC-4928-81FB-0309C7B8DB85}">
   <dimension ref="A1:Z203"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -15764,7 +15776,9 @@
       <c r="D7" s="30" t="s">
         <v>338</v>
       </c>
-      <c r="E7" s="32"/>
+      <c r="E7" s="32" t="s">
+        <v>474</v>
+      </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
@@ -18938,8 +18952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2157BC9-A210-4D6F-8D8A-C479F47A0035}">
   <dimension ref="A1:I247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -19014,7 +19028,7 @@
     </row>
     <row r="4" spans="1:9" ht="38.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27">
-        <f ca="1">IF(OFFSET(A4,-1,0) ="",OFFSET(A4,-2,0)+1,OFFSET(A4,-1,0)+1 )</f>
+        <f t="shared" ref="A4:A15" ca="1" si="0">IF(OFFSET(A4,-1,0) ="",OFFSET(A4,-2,0)+1,OFFSET(A4,-1,0)+1 )</f>
         <v>2</v>
       </c>
       <c r="B4" s="30" t="s">
@@ -19030,7 +19044,7 @@
     </row>
     <row r="5" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="27">
-        <f ca="1">IF(OFFSET(A5,-1,0) ="",OFFSET(A5,-2,0)+1,OFFSET(A5,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
       <c r="B5" s="30" t="s">
@@ -19046,7 +19060,7 @@
     </row>
     <row r="6" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27">
-        <f ca="1">IF(OFFSET(A6,-1,0) ="",OFFSET(A6,-2,0)+1,OFFSET(A6,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>4</v>
       </c>
       <c r="B6" s="30" t="s">
@@ -19062,7 +19076,7 @@
     </row>
     <row r="7" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="27">
-        <f ca="1">IF(OFFSET(A7,-1,0) ="",OFFSET(A7,-2,0)+1,OFFSET(A7,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
       <c r="B7" s="30" t="s">
@@ -19078,7 +19092,7 @@
     </row>
     <row r="8" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="27">
-        <f ca="1">IF(OFFSET(A8,-1,0) ="",OFFSET(A8,-2,0)+1,OFFSET(A8,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
       <c r="B8" s="30" t="s">
@@ -19094,7 +19108,7 @@
     </row>
     <row r="9" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="27">
-        <f ca="1">IF(OFFSET(A9,-1,0) ="",OFFSET(A9,-2,0)+1,OFFSET(A9,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>7</v>
       </c>
       <c r="B9" s="30" t="s">
@@ -19112,7 +19126,7 @@
     </row>
     <row r="10" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27">
-        <f ca="1">IF(OFFSET(A10,-1,0) ="",OFFSET(A10,-2,0)+1,OFFSET(A10,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>8</v>
       </c>
       <c r="B10" s="30" t="s">
@@ -19128,7 +19142,7 @@
     </row>
     <row r="11" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="27">
-        <f ca="1">IF(OFFSET(A11,-1,0) ="",OFFSET(A11,-2,0)+1,OFFSET(A11,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>9</v>
       </c>
       <c r="B11" s="30" t="s">
@@ -19144,7 +19158,7 @@
     </row>
     <row r="12" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="27">
-        <f ca="1">IF(OFFSET(A12,-1,0) ="",OFFSET(A12,-2,0)+1,OFFSET(A12,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>10</v>
       </c>
       <c r="B12" s="30" t="s">
@@ -19160,7 +19174,7 @@
     </row>
     <row r="13" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="27">
-        <f ca="1">IF(OFFSET(A13,-1,0) ="",OFFSET(A13,-2,0)+1,OFFSET(A13,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>11</v>
       </c>
       <c r="B13" s="30" t="s">
@@ -19176,7 +19190,7 @@
     </row>
     <row r="14" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="27">
-        <f ca="1">IF(OFFSET(A14,-1,0) ="",OFFSET(A14,-2,0)+1,OFFSET(A14,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>12</v>
       </c>
       <c r="B14" s="30" t="s">
@@ -19192,7 +19206,7 @@
     </row>
     <row r="15" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="27">
-        <f ca="1">IF(OFFSET(A15,-1,0) ="",OFFSET(A15,-2,0)+1,OFFSET(A15,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>13</v>
       </c>
       <c r="B15" s="30" t="s">
@@ -19208,7 +19222,7 @@
     </row>
     <row r="16" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="27">
-        <f t="shared" ref="A16:A107" ca="1" si="0">IF(OFFSET(A16,-1,0) ="",OFFSET(A16,-2,0)+1,OFFSET(A16,-1,0)+1 )</f>
+        <f t="shared" ref="A16:A107" ca="1" si="1">IF(OFFSET(A16,-1,0) ="",OFFSET(A16,-2,0)+1,OFFSET(A16,-1,0)+1 )</f>
         <v>14</v>
       </c>
       <c r="B16" s="30" t="s">
@@ -19224,13 +19238,15 @@
     </row>
     <row r="17" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>15</v>
       </c>
       <c r="B17" s="30" t="s">
         <v>405</v>
       </c>
-      <c r="C17" s="30"/>
+      <c r="C17" s="30" t="s">
+        <v>471</v>
+      </c>
       <c r="D17" s="30"/>
       <c r="E17" s="32"/>
       <c r="F17" s="13"/>
@@ -19240,13 +19256,15 @@
     </row>
     <row r="18" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>16</v>
       </c>
       <c r="B18" s="30" t="s">
         <v>407</v>
       </c>
-      <c r="C18" s="30"/>
+      <c r="C18" s="30" t="s">
+        <v>473</v>
+      </c>
       <c r="D18" s="30"/>
       <c r="E18" s="32"/>
       <c r="F18" s="13"/>
@@ -19256,7 +19274,7 @@
     </row>
     <row r="19" spans="1:9" ht="36.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>17</v>
       </c>
       <c r="B19" s="30" t="s">
@@ -19272,7 +19290,7 @@
     </row>
     <row r="20" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>18</v>
       </c>
       <c r="B20" s="30" t="s">
@@ -19288,7 +19306,7 @@
     </row>
     <row r="21" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>19</v>
       </c>
       <c r="B21" s="30" t="s">
@@ -19304,7 +19322,7 @@
     </row>
     <row r="22" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>20</v>
       </c>
       <c r="B22" s="30" t="s">
@@ -19320,7 +19338,7 @@
     </row>
     <row r="23" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>21</v>
       </c>
       <c r="B23" s="30" t="s">
@@ -19336,7 +19354,7 @@
     </row>
     <row r="24" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>22</v>
       </c>
       <c r="B24" s="30" t="s">
@@ -19352,7 +19370,7 @@
     </row>
     <row r="25" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>23</v>
       </c>
       <c r="B25" s="30" t="s">
@@ -19368,7 +19386,7 @@
     </row>
     <row r="26" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>24</v>
       </c>
       <c r="B26" s="30" t="s">
@@ -19384,7 +19402,7 @@
     </row>
     <row r="27" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>25</v>
       </c>
       <c r="B27" s="30" t="s">
@@ -19400,7 +19418,7 @@
     </row>
     <row r="28" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>26</v>
       </c>
       <c r="B28" s="30" t="s">
@@ -19416,7 +19434,7 @@
     </row>
     <row r="29" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>27</v>
       </c>
       <c r="B29" s="30" t="s">
@@ -19432,7 +19450,7 @@
     </row>
     <row r="30" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>28</v>
       </c>
       <c r="B30" s="30" t="s">
@@ -19448,7 +19466,7 @@
     </row>
     <row r="31" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>29</v>
       </c>
       <c r="B31" s="30" t="s">
@@ -19464,7 +19482,7 @@
     </row>
     <row r="32" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>30</v>
       </c>
       <c r="B32" s="30" t="s">
@@ -19480,7 +19498,7 @@
     </row>
     <row r="33" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>31</v>
       </c>
       <c r="B33" s="30" t="s">
@@ -19496,7 +19514,7 @@
     </row>
     <row r="34" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>32</v>
       </c>
       <c r="B34" s="30" t="s">
@@ -19512,7 +19530,7 @@
     </row>
     <row r="35" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>33</v>
       </c>
       <c r="B35" s="30" t="s">
@@ -19528,7 +19546,7 @@
     </row>
     <row r="36" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>34</v>
       </c>
       <c r="B36" s="30" t="s">
@@ -19544,7 +19562,7 @@
     </row>
     <row r="37" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>35</v>
       </c>
       <c r="B37" s="30" t="s">
@@ -19560,7 +19578,7 @@
     </row>
     <row r="38" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>36</v>
       </c>
       <c r="B38" s="30" t="s">
@@ -19576,7 +19594,7 @@
     </row>
     <row r="39" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>37</v>
       </c>
       <c r="B39" s="30" t="s">
@@ -19627,7 +19645,9 @@
       <c r="B42" s="30" t="s">
         <v>435</v>
       </c>
-      <c r="C42" s="30"/>
+      <c r="C42" s="30" t="s">
+        <v>472</v>
+      </c>
       <c r="D42" s="30"/>
       <c r="E42" s="32"/>
       <c r="F42" s="13"/>
@@ -19653,7 +19673,7 @@
     </row>
     <row r="44" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>41</v>
       </c>
       <c r="B44" s="30" t="s">
@@ -19669,7 +19689,7 @@
     </row>
     <row r="45" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42</v>
       </c>
       <c r="B45" s="30" t="s">
@@ -19685,7 +19705,7 @@
     </row>
     <row r="46" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>43</v>
       </c>
       <c r="B46" s="30" t="s">
@@ -19701,7 +19721,7 @@
     </row>
     <row r="47" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>44</v>
       </c>
       <c r="B47" s="30" t="s">
@@ -19717,7 +19737,7 @@
     </row>
     <row r="48" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>45</v>
       </c>
       <c r="B48" s="30" t="s">
@@ -19733,7 +19753,7 @@
     </row>
     <row r="49" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>46</v>
       </c>
       <c r="B49" s="30" t="s">
@@ -19797,7 +19817,7 @@
     </row>
     <row r="53" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>49</v>
       </c>
       <c r="B53" s="30" t="s">
@@ -19813,7 +19833,7 @@
     </row>
     <row r="54" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>50</v>
       </c>
       <c r="B54" s="30" t="s">
@@ -19829,7 +19849,7 @@
     </row>
     <row r="55" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>51</v>
       </c>
       <c r="B55" s="30" t="s">
@@ -19845,7 +19865,7 @@
     </row>
     <row r="56" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>52</v>
       </c>
       <c r="B56" s="30" t="s">
@@ -19861,7 +19881,7 @@
     </row>
     <row r="57" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>53</v>
       </c>
       <c r="B57" s="30" t="s">
@@ -19877,7 +19897,7 @@
     </row>
     <row r="58" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>54</v>
       </c>
       <c r="B58" s="11" t="s">
@@ -19893,7 +19913,7 @@
     </row>
     <row r="59" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>55</v>
       </c>
       <c r="B59" s="11" t="s">
@@ -19938,7 +19958,7 @@
     </row>
     <row r="62" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>57</v>
       </c>
       <c r="B62" s="29" t="s">
@@ -19954,7 +19974,7 @@
     </row>
     <row r="63" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>58</v>
       </c>
       <c r="B63" s="29" t="s">
@@ -19970,7 +19990,7 @@
     </row>
     <row r="64" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>59</v>
       </c>
       <c r="B64" s="29" t="s">
@@ -19986,7 +20006,7 @@
     </row>
     <row r="65" spans="1:9" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>60</v>
       </c>
       <c r="B65" s="29" t="s">
@@ -20002,7 +20022,7 @@
     </row>
     <row r="66" spans="1:9" ht="25" x14ac:dyDescent="0.25">
       <c r="A66" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>61</v>
       </c>
       <c r="B66" s="29" t="s">
@@ -20018,7 +20038,7 @@
     </row>
     <row r="67" spans="1:9" ht="29.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>62</v>
       </c>
       <c r="B67" s="29" t="s">
@@ -20034,7 +20054,7 @@
     </row>
     <row r="68" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>63</v>
       </c>
       <c r="B68" s="29" t="s">
@@ -20119,7 +20139,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>68</v>
       </c>
       <c r="B74" s="29"/>
@@ -20133,7 +20153,7 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>69</v>
       </c>
       <c r="B75" s="29"/>
@@ -20147,7 +20167,7 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>70</v>
       </c>
       <c r="B76" s="29"/>
@@ -20161,7 +20181,7 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>71</v>
       </c>
       <c r="B77" s="29"/>
@@ -20175,7 +20195,7 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>72</v>
       </c>
       <c r="B78" s="29"/>
@@ -20189,7 +20209,7 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>73</v>
       </c>
       <c r="B79" s="29"/>
@@ -20203,7 +20223,7 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>74</v>
       </c>
       <c r="B80" s="29"/>
@@ -20217,7 +20237,7 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>75</v>
       </c>
       <c r="B81" s="29"/>
@@ -20231,7 +20251,7 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>76</v>
       </c>
       <c r="B82" s="29"/>
@@ -20245,7 +20265,7 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>77</v>
       </c>
       <c r="B83" s="29"/>
@@ -20259,7 +20279,7 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>78</v>
       </c>
       <c r="B84" s="29"/>
@@ -20273,7 +20293,7 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>79</v>
       </c>
       <c r="B85" s="29"/>
@@ -20287,7 +20307,7 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>80</v>
       </c>
       <c r="B86" s="29"/>
@@ -20301,7 +20321,7 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>81</v>
       </c>
       <c r="B87" s="29"/>
@@ -20315,7 +20335,7 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>82</v>
       </c>
       <c r="B88" s="29"/>
@@ -20329,7 +20349,7 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>83</v>
       </c>
       <c r="B89" s="30"/>
@@ -20343,7 +20363,7 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>84</v>
       </c>
       <c r="B90" s="15"/>
@@ -20382,7 +20402,7 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>86</v>
       </c>
       <c r="B93" s="30"/>
@@ -20396,7 +20416,7 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>87</v>
       </c>
       <c r="B94" s="30"/>
@@ -20410,7 +20430,7 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>88</v>
       </c>
       <c r="B95" s="30"/>
@@ -20424,7 +20444,7 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>89</v>
       </c>
       <c r="B96" s="30"/>
@@ -20438,7 +20458,7 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>90</v>
       </c>
       <c r="B97" s="30"/>
@@ -20452,7 +20472,7 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>91</v>
       </c>
       <c r="B98" s="30"/>
@@ -20466,7 +20486,7 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>92</v>
       </c>
       <c r="B99" s="30"/>
@@ -20480,7 +20500,7 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>93</v>
       </c>
       <c r="B100" s="30"/>
@@ -20494,7 +20514,7 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>94</v>
       </c>
       <c r="B101" s="30"/>
@@ -20508,7 +20528,7 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>95</v>
       </c>
       <c r="B102" s="30"/>
@@ -20522,7 +20542,7 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>96</v>
       </c>
       <c r="B103" s="30"/>
@@ -20536,7 +20556,7 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>97</v>
       </c>
       <c r="B104" s="30"/>
@@ -20550,7 +20570,7 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>98</v>
       </c>
       <c r="B105" s="30"/>
@@ -20564,7 +20584,7 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>99</v>
       </c>
       <c r="B106" s="30"/>
@@ -20578,7 +20598,7 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="27">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>100</v>
       </c>
       <c r="B107" s="30"/>
@@ -20834,7 +20854,7 @@
     </row>
     <row r="130" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="27">
-        <f ca="1">IF(OFFSET(A130,-1,0) ="",OFFSET(A130,-2,0)+1,OFFSET(A130,-1,0)+1 )</f>
+        <f t="shared" ref="A130:A138" ca="1" si="2">IF(OFFSET(A130,-1,0) ="",OFFSET(A130,-2,0)+1,OFFSET(A130,-1,0)+1 )</f>
         <v>1</v>
       </c>
       <c r="B130" s="30" t="s">
@@ -20850,7 +20870,7 @@
     </row>
     <row r="131" spans="1:9" ht="26.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="27">
-        <f ca="1">IF(OFFSET(A131,-1,0) ="",OFFSET(A131,-2,0)+1,OFFSET(A131,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="2"/>
         <v>2</v>
       </c>
       <c r="B131" s="30" t="s">
@@ -20866,7 +20886,7 @@
     </row>
     <row r="132" spans="1:9" ht="21.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="27">
-        <f ca="1">IF(OFFSET(A132,-1,0) ="",OFFSET(A132,-2,0)+1,OFFSET(A132,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="2"/>
         <v>3</v>
       </c>
       <c r="B132" s="30" t="s">
@@ -20882,7 +20902,7 @@
     </row>
     <row r="133" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="27">
-        <f ca="1">IF(OFFSET(A133,-1,0) ="",OFFSET(A133,-2,0)+1,OFFSET(A133,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="2"/>
         <v>4</v>
       </c>
       <c r="B133" s="30" t="s">
@@ -20898,7 +20918,7 @@
     </row>
     <row r="134" spans="1:9" ht="30.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="27">
-        <f ca="1">IF(OFFSET(A134,-1,0) ="",OFFSET(A134,-2,0)+1,OFFSET(A134,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="2"/>
         <v>5</v>
       </c>
       <c r="B134" s="30" t="s">
@@ -20914,7 +20934,7 @@
     </row>
     <row r="135" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="27">
-        <f ca="1">IF(OFFSET(A135,-1,0) ="",OFFSET(A135,-2,0)+1,OFFSET(A135,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="2"/>
         <v>6</v>
       </c>
       <c r="B135" s="30" t="s">
@@ -20930,7 +20950,7 @@
     </row>
     <row r="136" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="27">
-        <f ca="1">IF(OFFSET(A136,-1,0) ="",OFFSET(A136,-2,0)+1,OFFSET(A136,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="2"/>
         <v>7</v>
       </c>
       <c r="B136" s="30" t="s">
@@ -20946,7 +20966,7 @@
     </row>
     <row r="137" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="27">
-        <f ca="1">IF(OFFSET(A137,-1,0) ="",OFFSET(A137,-2,0)+1,OFFSET(A137,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="2"/>
         <v>8</v>
       </c>
       <c r="B137" s="30" t="s">
@@ -20962,7 +20982,7 @@
     </row>
     <row r="138" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="27">
-        <f ca="1">IF(OFFSET(A138,-1,0) ="",OFFSET(A138,-2,0)+1,OFFSET(A138,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="2"/>
         <v>9</v>
       </c>
       <c r="B138" s="30" t="s">
@@ -22122,7 +22142,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A171:I171"/>
     <mergeCell ref="A173:I173"/>
     <mergeCell ref="A175:I175"/>
     <mergeCell ref="A41:I41"/>
@@ -22142,6 +22161,7 @@
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A70:I70"/>
     <mergeCell ref="A91:I91"/>
+    <mergeCell ref="A171:I171"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Added "more than 350" cases
</commit_message>
<xml_diff>
--- a/Middle Assignment/TestDesignTechique_PhamHongAnh.xlsx
+++ b/Middle Assignment/TestDesignTechique_PhamHongAnh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NashTech\Rookies\NashTech_Homework\Middle Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7277F12-EAE7-4CEE-9C91-649EF3F311BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5950AFEC-1078-467A-A533-7D84DADB90E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1091,7 +1091,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="592">
   <si>
     <t>ID</t>
   </si>
@@ -3252,6 +3252,9 @@
   </si>
   <si>
     <t>When entering between 2 and 50 alphanumeric characters</t>
+  </si>
+  <si>
+    <t>When entering more than 350 characters</t>
   </si>
 </sst>
 </file>
@@ -3597,6 +3600,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3623,13 +3632,13 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3649,12 +3658,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3936,17 +3939,17 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -3966,17 +3969,17 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -4365,17 +4368,17 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14" spans="1:26" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -4763,17 +4766,17 @@
       <c r="Z24" s="2"/>
     </row>
     <row r="25" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="44"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="45"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="47"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
@@ -4865,17 +4868,17 @@
       <c r="Z27" s="2"/>
     </row>
     <row r="28" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="44"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="44"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="45"/>
+      <c r="B28" s="46"/>
+      <c r="C28" s="46"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="46"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="47"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -4968,17 +4971,17 @@
       <c r="Z30" s="2"/>
     </row>
     <row r="31" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="39" t="s">
+      <c r="A31" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="42"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -4998,17 +5001,17 @@
       <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="37"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="37"/>
-      <c r="H32" s="37"/>
-      <c r="I32" s="38"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="40"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
@@ -5202,17 +5205,17 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="36" t="s">
+      <c r="A42" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B42" s="37"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="37"/>
-      <c r="E42" s="37"/>
-      <c r="F42" s="37"/>
-      <c r="G42" s="37"/>
-      <c r="H42" s="37"/>
-      <c r="I42" s="38"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="39"/>
+      <c r="H42" s="39"/>
+      <c r="I42" s="40"/>
     </row>
     <row r="43" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
@@ -16245,7 +16248,7 @@
       <c r="Z1" s="26"/>
     </row>
     <row r="2" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="41" t="s">
         <v>158</v>
       </c>
       <c r="B2" s="48"/>
@@ -16275,17 +16278,17 @@
       <c r="Z2" s="26"/>
     </row>
     <row r="3" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="43" t="s">
         <v>183</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
       <c r="J3" s="26"/>
       <c r="K3" s="26"/>
       <c r="L3" s="26"/>
@@ -16530,17 +16533,17 @@
       <c r="I14" s="32"/>
     </row>
     <row r="15" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="46" t="s">
+      <c r="A15" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="B15" s="47"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="47"/>
-      <c r="I15" s="47"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
       <c r="J15" s="26"/>
       <c r="K15" s="26"/>
       <c r="L15" s="26"/>
@@ -16760,17 +16763,17 @@
       <c r="I25" s="32"/>
     </row>
     <row r="26" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="46" t="s">
+      <c r="A26" s="50" t="s">
         <v>127</v>
       </c>
-      <c r="B26" s="47"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="47"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
       <c r="J26" s="26"/>
       <c r="K26" s="26"/>
       <c r="L26" s="26"/>
@@ -17190,17 +17193,17 @@
       <c r="I46" s="32"/>
     </row>
     <row r="47" spans="1:9" s="10" customFormat="1" ht="21.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="46" t="s">
+      <c r="A47" s="50" t="s">
         <v>140</v>
       </c>
-      <c r="B47" s="47"/>
-      <c r="C47" s="47"/>
-      <c r="D47" s="47"/>
-      <c r="E47" s="47"/>
-      <c r="F47" s="47"/>
-      <c r="G47" s="47"/>
-      <c r="H47" s="47"/>
-      <c r="I47" s="47"/>
+      <c r="B47" s="49"/>
+      <c r="C47" s="49"/>
+      <c r="D47" s="49"/>
+      <c r="E47" s="49"/>
+      <c r="F47" s="49"/>
+      <c r="G47" s="49"/>
+      <c r="H47" s="49"/>
+      <c r="I47" s="49"/>
     </row>
     <row r="48" spans="1:9" s="10" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="27">
@@ -17523,17 +17526,17 @@
       <c r="I63" s="32"/>
     </row>
     <row r="64" spans="1:9" s="10" customFormat="1" ht="23.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="46" t="s">
+      <c r="A64" s="50" t="s">
         <v>147</v>
       </c>
-      <c r="B64" s="47"/>
-      <c r="C64" s="47"/>
-      <c r="D64" s="47"/>
-      <c r="E64" s="47"/>
-      <c r="F64" s="47"/>
-      <c r="G64" s="47"/>
-      <c r="H64" s="47"/>
-      <c r="I64" s="47"/>
+      <c r="B64" s="49"/>
+      <c r="C64" s="49"/>
+      <c r="D64" s="49"/>
+      <c r="E64" s="49"/>
+      <c r="F64" s="49"/>
+      <c r="G64" s="49"/>
+      <c r="H64" s="49"/>
+      <c r="I64" s="49"/>
     </row>
     <row r="65" spans="1:9" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="27">
@@ -17636,17 +17639,17 @@
       <c r="I69" s="32"/>
     </row>
     <row r="70" spans="1:9" s="10" customFormat="1" ht="23.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="46" t="s">
+      <c r="A70" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="B70" s="47"/>
-      <c r="C70" s="47"/>
-      <c r="D70" s="47"/>
-      <c r="E70" s="47"/>
-      <c r="F70" s="47"/>
-      <c r="G70" s="47"/>
-      <c r="H70" s="47"/>
-      <c r="I70" s="47"/>
+      <c r="B70" s="49"/>
+      <c r="C70" s="49"/>
+      <c r="D70" s="49"/>
+      <c r="E70" s="49"/>
+      <c r="F70" s="49"/>
+      <c r="G70" s="49"/>
+      <c r="H70" s="49"/>
+      <c r="I70" s="49"/>
     </row>
     <row r="71" spans="1:9" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="27">
@@ -17909,7 +17912,7 @@
       <c r="I83" s="32"/>
     </row>
     <row r="84" spans="1:9" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="39" t="s">
+      <c r="A84" s="41" t="s">
         <v>159</v>
       </c>
       <c r="B84" s="48"/>
@@ -17922,17 +17925,17 @@
       <c r="I84" s="48"/>
     </row>
     <row r="85" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="46" t="s">
+      <c r="A85" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="B85" s="47"/>
-      <c r="C85" s="47"/>
-      <c r="D85" s="47"/>
-      <c r="E85" s="47"/>
-      <c r="F85" s="47"/>
-      <c r="G85" s="47"/>
-      <c r="H85" s="47"/>
-      <c r="I85" s="47"/>
+      <c r="B85" s="49"/>
+      <c r="C85" s="49"/>
+      <c r="D85" s="49"/>
+      <c r="E85" s="49"/>
+      <c r="F85" s="49"/>
+      <c r="G85" s="49"/>
+      <c r="H85" s="49"/>
+      <c r="I85" s="49"/>
     </row>
     <row r="86" spans="1:9" s="10" customFormat="1" ht="98.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="27">
@@ -18215,20 +18218,20 @@
       <c r="I99" s="32"/>
     </row>
     <row r="105" spans="1:26" s="10" customFormat="1" ht="32.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="49" t="s">
+      <c r="A105" s="51" t="s">
         <v>190</v>
       </c>
-      <c r="B105" s="50"/>
-      <c r="C105" s="50"/>
-      <c r="D105" s="50"/>
-      <c r="E105" s="50"/>
-      <c r="F105" s="50"/>
-      <c r="G105" s="50"/>
-      <c r="H105" s="50"/>
-      <c r="I105" s="51"/>
+      <c r="B105" s="52"/>
+      <c r="C105" s="52"/>
+      <c r="D105" s="52"/>
+      <c r="E105" s="52"/>
+      <c r="F105" s="52"/>
+      <c r="G105" s="52"/>
+      <c r="H105" s="52"/>
+      <c r="I105" s="53"/>
     </row>
     <row r="106" spans="1:26" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="39" t="s">
+      <c r="A106" s="41" t="s">
         <v>187</v>
       </c>
       <c r="B106" s="48"/>
@@ -18241,17 +18244,17 @@
       <c r="I106" s="48"/>
     </row>
     <row r="107" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="46" t="s">
+      <c r="A107" s="50" t="s">
         <v>168</v>
       </c>
-      <c r="B107" s="47"/>
-      <c r="C107" s="47"/>
-      <c r="D107" s="47"/>
-      <c r="E107" s="47"/>
-      <c r="F107" s="47"/>
-      <c r="G107" s="47"/>
-      <c r="H107" s="47"/>
-      <c r="I107" s="47"/>
+      <c r="B107" s="49"/>
+      <c r="C107" s="49"/>
+      <c r="D107" s="49"/>
+      <c r="E107" s="49"/>
+      <c r="F107" s="49"/>
+      <c r="G107" s="49"/>
+      <c r="H107" s="49"/>
+      <c r="I107" s="49"/>
       <c r="J107" s="26"/>
       <c r="K107" s="26"/>
       <c r="L107" s="26"/>
@@ -18321,17 +18324,17 @@
       <c r="I110" s="32"/>
     </row>
     <row r="111" spans="1:26" s="10" customFormat="1" ht="23.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="46" t="s">
+      <c r="A111" s="50" t="s">
         <v>153</v>
       </c>
-      <c r="B111" s="47"/>
-      <c r="C111" s="47"/>
-      <c r="D111" s="47"/>
-      <c r="E111" s="47"/>
-      <c r="F111" s="47"/>
-      <c r="G111" s="47"/>
-      <c r="H111" s="47"/>
-      <c r="I111" s="47"/>
+      <c r="B111" s="49"/>
+      <c r="C111" s="49"/>
+      <c r="D111" s="49"/>
+      <c r="E111" s="49"/>
+      <c r="F111" s="49"/>
+      <c r="G111" s="49"/>
+      <c r="H111" s="49"/>
+      <c r="I111" s="49"/>
     </row>
     <row r="112" spans="1:26" s="10" customFormat="1" ht="30.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="27" t="e">
@@ -18366,17 +18369,17 @@
       <c r="I113" s="32"/>
     </row>
     <row r="114" spans="1:9" s="10" customFormat="1" ht="23.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="46" t="s">
+      <c r="A114" s="50" t="s">
         <v>156</v>
       </c>
-      <c r="B114" s="47"/>
-      <c r="C114" s="47"/>
-      <c r="D114" s="47"/>
-      <c r="E114" s="47"/>
-      <c r="F114" s="47"/>
-      <c r="G114" s="47"/>
-      <c r="H114" s="47"/>
-      <c r="I114" s="47"/>
+      <c r="B114" s="49"/>
+      <c r="C114" s="49"/>
+      <c r="D114" s="49"/>
+      <c r="E114" s="49"/>
+      <c r="F114" s="49"/>
+      <c r="G114" s="49"/>
+      <c r="H114" s="49"/>
+      <c r="I114" s="49"/>
     </row>
     <row r="115" spans="1:9" s="10" customFormat="1" ht="32.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="27" t="e">
@@ -18395,17 +18398,17 @@
       <c r="I115" s="32"/>
     </row>
     <row r="116" spans="1:9" s="10" customFormat="1" ht="23.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="46" t="s">
+      <c r="A116" s="50" t="s">
         <v>177</v>
       </c>
-      <c r="B116" s="47"/>
-      <c r="C116" s="47"/>
-      <c r="D116" s="47"/>
-      <c r="E116" s="47"/>
-      <c r="F116" s="47"/>
-      <c r="G116" s="47"/>
-      <c r="H116" s="47"/>
-      <c r="I116" s="47"/>
+      <c r="B116" s="49"/>
+      <c r="C116" s="49"/>
+      <c r="D116" s="49"/>
+      <c r="E116" s="49"/>
+      <c r="F116" s="49"/>
+      <c r="G116" s="49"/>
+      <c r="H116" s="49"/>
+      <c r="I116" s="49"/>
     </row>
     <row r="117" spans="1:9" s="10" customFormat="1" ht="32.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="27" t="e">
@@ -18424,17 +18427,17 @@
       <c r="I117" s="32"/>
     </row>
     <row r="118" spans="1:9" s="10" customFormat="1" ht="23.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="46" t="s">
+      <c r="A118" s="50" t="s">
         <v>180</v>
       </c>
-      <c r="B118" s="47"/>
-      <c r="C118" s="47"/>
-      <c r="D118" s="47"/>
-      <c r="E118" s="47"/>
-      <c r="F118" s="47"/>
-      <c r="G118" s="47"/>
-      <c r="H118" s="47"/>
-      <c r="I118" s="47"/>
+      <c r="B118" s="49"/>
+      <c r="C118" s="49"/>
+      <c r="D118" s="49"/>
+      <c r="E118" s="49"/>
+      <c r="F118" s="49"/>
+      <c r="G118" s="49"/>
+      <c r="H118" s="49"/>
+      <c r="I118" s="49"/>
     </row>
     <row r="119" spans="1:9" s="10" customFormat="1" ht="32.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="27" t="e">
@@ -18485,17 +18488,17 @@
       <c r="I121" s="32"/>
     </row>
     <row r="122" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="46" t="s">
+      <c r="A122" s="50" t="s">
         <v>184</v>
       </c>
-      <c r="B122" s="47"/>
-      <c r="C122" s="47"/>
-      <c r="D122" s="47"/>
-      <c r="E122" s="47"/>
-      <c r="F122" s="47"/>
-      <c r="G122" s="47"/>
-      <c r="H122" s="47"/>
-      <c r="I122" s="47"/>
+      <c r="B122" s="49"/>
+      <c r="C122" s="49"/>
+      <c r="D122" s="49"/>
+      <c r="E122" s="49"/>
+      <c r="F122" s="49"/>
+      <c r="G122" s="49"/>
+      <c r="H122" s="49"/>
+      <c r="I122" s="49"/>
     </row>
     <row r="123" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="27" t="e">
@@ -18564,17 +18567,17 @@
       <c r="I126" s="32"/>
     </row>
     <row r="127" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="46" t="s">
+      <c r="A127" s="50" t="s">
         <v>181</v>
       </c>
-      <c r="B127" s="47"/>
-      <c r="C127" s="47"/>
-      <c r="D127" s="47"/>
-      <c r="E127" s="47"/>
-      <c r="F127" s="47"/>
-      <c r="G127" s="47"/>
-      <c r="H127" s="47"/>
-      <c r="I127" s="47"/>
+      <c r="B127" s="49"/>
+      <c r="C127" s="49"/>
+      <c r="D127" s="49"/>
+      <c r="E127" s="49"/>
+      <c r="F127" s="49"/>
+      <c r="G127" s="49"/>
+      <c r="H127" s="49"/>
+      <c r="I127" s="49"/>
     </row>
     <row r="128" spans="1:9" s="10" customFormat="1" ht="32.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="27" t="e">
@@ -18593,17 +18596,17 @@
       <c r="I128" s="32"/>
     </row>
     <row r="129" spans="1:26" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="46" t="s">
+      <c r="A129" s="50" t="s">
         <v>182</v>
       </c>
-      <c r="B129" s="47"/>
-      <c r="C129" s="47"/>
-      <c r="D129" s="47"/>
-      <c r="E129" s="47"/>
-      <c r="F129" s="47"/>
-      <c r="G129" s="47"/>
-      <c r="H129" s="47"/>
-      <c r="I129" s="47"/>
+      <c r="B129" s="49"/>
+      <c r="C129" s="49"/>
+      <c r="D129" s="49"/>
+      <c r="E129" s="49"/>
+      <c r="F129" s="49"/>
+      <c r="G129" s="49"/>
+      <c r="H129" s="49"/>
+      <c r="I129" s="49"/>
     </row>
     <row r="130" spans="1:26" s="10" customFormat="1" ht="32.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="27" t="e">
@@ -18622,17 +18625,17 @@
       <c r="I130" s="32"/>
     </row>
     <row r="131" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A131" s="46" t="s">
+      <c r="A131" s="50" t="s">
         <v>164</v>
       </c>
-      <c r="B131" s="47"/>
-      <c r="C131" s="47"/>
-      <c r="D131" s="47"/>
-      <c r="E131" s="47"/>
-      <c r="F131" s="47"/>
-      <c r="G131" s="47"/>
-      <c r="H131" s="47"/>
-      <c r="I131" s="47"/>
+      <c r="B131" s="49"/>
+      <c r="C131" s="49"/>
+      <c r="D131" s="49"/>
+      <c r="E131" s="49"/>
+      <c r="F131" s="49"/>
+      <c r="G131" s="49"/>
+      <c r="H131" s="49"/>
+      <c r="I131" s="49"/>
       <c r="J131" s="26"/>
       <c r="K131" s="26"/>
       <c r="L131" s="26"/>
@@ -19524,6 +19527,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A131:I131"/>
+    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="A84:I84"/>
+    <mergeCell ref="A47:I47"/>
+    <mergeCell ref="A64:I64"/>
+    <mergeCell ref="A70:I70"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A15:I15"/>
@@ -19538,12 +19547,6 @@
     <mergeCell ref="A116:I116"/>
     <mergeCell ref="A118:I118"/>
     <mergeCell ref="A111:I111"/>
-    <mergeCell ref="A131:I131"/>
-    <mergeCell ref="A26:I26"/>
-    <mergeCell ref="A84:I84"/>
-    <mergeCell ref="A47:I47"/>
-    <mergeCell ref="A64:I64"/>
-    <mergeCell ref="A70:I70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -19602,20 +19605,20 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="54" t="s">
         <v>466</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="54"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="56"/>
     </row>
     <row r="3" spans="1:9" ht="21.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="41" t="s">
         <v>393</v>
       </c>
       <c r="B3" s="48"/>
@@ -20047,7 +20050,7 @@
       <c r="I24" s="32"/>
     </row>
     <row r="25" spans="1:9" ht="21.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="41" t="s">
         <v>432</v>
       </c>
       <c r="B25" s="48"/>
@@ -20382,7 +20385,7 @@
       <c r="I41" s="32"/>
     </row>
     <row r="42" spans="1:9" ht="21.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="41" t="s">
         <v>433</v>
       </c>
       <c r="B42" s="48"/>
@@ -20495,15 +20498,15 @@
       <c r="I47" s="32"/>
     </row>
     <row r="48" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A48" s="46"/>
-      <c r="B48" s="47"/>
-      <c r="C48" s="47"/>
-      <c r="D48" s="47"/>
-      <c r="E48" s="47"/>
-      <c r="F48" s="47"/>
-      <c r="G48" s="47"/>
-      <c r="H48" s="47"/>
-      <c r="I48" s="47"/>
+      <c r="A48" s="50"/>
+      <c r="B48" s="49"/>
+      <c r="C48" s="49"/>
+      <c r="D48" s="49"/>
+      <c r="E48" s="49"/>
+      <c r="F48" s="49"/>
+      <c r="G48" s="49"/>
+      <c r="H48" s="49"/>
+      <c r="I48" s="49"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="27">
@@ -20786,15 +20789,15 @@
       <c r="I68" s="32"/>
     </row>
     <row r="69" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A69" s="46"/>
-      <c r="B69" s="47"/>
-      <c r="C69" s="47"/>
-      <c r="D69" s="47"/>
-      <c r="E69" s="47"/>
-      <c r="F69" s="47"/>
-      <c r="G69" s="47"/>
-      <c r="H69" s="47"/>
-      <c r="I69" s="47"/>
+      <c r="A69" s="50"/>
+      <c r="B69" s="49"/>
+      <c r="C69" s="49"/>
+      <c r="D69" s="49"/>
+      <c r="E69" s="49"/>
+      <c r="F69" s="49"/>
+      <c r="G69" s="49"/>
+      <c r="H69" s="49"/>
+      <c r="I69" s="49"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="27">
@@ -21021,15 +21024,15 @@
       <c r="I85" s="32"/>
     </row>
     <row r="86" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A86" s="46"/>
-      <c r="B86" s="47"/>
-      <c r="C86" s="47"/>
-      <c r="D86" s="47"/>
-      <c r="E86" s="47"/>
-      <c r="F86" s="47"/>
-      <c r="G86" s="47"/>
-      <c r="H86" s="47"/>
-      <c r="I86" s="47"/>
+      <c r="A86" s="50"/>
+      <c r="B86" s="49"/>
+      <c r="C86" s="49"/>
+      <c r="D86" s="49"/>
+      <c r="E86" s="49"/>
+      <c r="F86" s="49"/>
+      <c r="G86" s="49"/>
+      <c r="H86" s="49"/>
+      <c r="I86" s="49"/>
     </row>
     <row r="87" spans="1:9" ht="35.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="27">
@@ -21102,15 +21105,15 @@
       <c r="I91" s="32"/>
     </row>
     <row r="92" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A92" s="46"/>
-      <c r="B92" s="47"/>
-      <c r="C92" s="47"/>
-      <c r="D92" s="47"/>
-      <c r="E92" s="47"/>
-      <c r="F92" s="47"/>
-      <c r="G92" s="47"/>
-      <c r="H92" s="47"/>
-      <c r="I92" s="47"/>
+      <c r="A92" s="50"/>
+      <c r="B92" s="49"/>
+      <c r="C92" s="49"/>
+      <c r="D92" s="49"/>
+      <c r="E92" s="49"/>
+      <c r="F92" s="49"/>
+      <c r="G92" s="49"/>
+      <c r="H92" s="49"/>
+      <c r="I92" s="49"/>
     </row>
     <row r="93" spans="1:9" ht="38.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="13">
@@ -21270,7 +21273,7 @@
       <c r="I105" s="32"/>
     </row>
     <row r="106" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A106" s="39"/>
+      <c r="A106" s="41"/>
       <c r="B106" s="48"/>
       <c r="C106" s="48"/>
       <c r="D106" s="48"/>
@@ -21281,15 +21284,15 @@
       <c r="I106" s="48"/>
     </row>
     <row r="107" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A107" s="46"/>
-      <c r="B107" s="47"/>
-      <c r="C107" s="47"/>
-      <c r="D107" s="47"/>
-      <c r="E107" s="47"/>
-      <c r="F107" s="47"/>
-      <c r="G107" s="47"/>
-      <c r="H107" s="47"/>
-      <c r="I107" s="47"/>
+      <c r="A107" s="50"/>
+      <c r="B107" s="49"/>
+      <c r="C107" s="49"/>
+      <c r="D107" s="49"/>
+      <c r="E107" s="49"/>
+      <c r="F107" s="49"/>
+      <c r="G107" s="49"/>
+      <c r="H107" s="49"/>
+      <c r="I107" s="49"/>
     </row>
     <row r="108" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="27">
@@ -21596,18 +21599,18 @@
       <c r="I126" s="32"/>
     </row>
     <row r="127" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A127" s="49"/>
-      <c r="B127" s="50"/>
-      <c r="C127" s="50"/>
-      <c r="D127" s="50"/>
-      <c r="E127" s="50"/>
-      <c r="F127" s="50"/>
-      <c r="G127" s="50"/>
-      <c r="H127" s="50"/>
-      <c r="I127" s="51"/>
+      <c r="A127" s="51"/>
+      <c r="B127" s="52"/>
+      <c r="C127" s="52"/>
+      <c r="D127" s="52"/>
+      <c r="E127" s="52"/>
+      <c r="F127" s="52"/>
+      <c r="G127" s="52"/>
+      <c r="H127" s="52"/>
+      <c r="I127" s="53"/>
     </row>
     <row r="128" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A128" s="39"/>
+      <c r="A128" s="41"/>
       <c r="B128" s="48"/>
       <c r="C128" s="48"/>
       <c r="D128" s="48"/>
@@ -21618,15 +21621,15 @@
       <c r="I128" s="48"/>
     </row>
     <row r="129" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A129" s="46"/>
-      <c r="B129" s="47"/>
-      <c r="C129" s="47"/>
-      <c r="D129" s="47"/>
-      <c r="E129" s="47"/>
-      <c r="F129" s="47"/>
-      <c r="G129" s="47"/>
-      <c r="H129" s="47"/>
-      <c r="I129" s="47"/>
+      <c r="A129" s="50"/>
+      <c r="B129" s="49"/>
+      <c r="C129" s="49"/>
+      <c r="D129" s="49"/>
+      <c r="E129" s="49"/>
+      <c r="F129" s="49"/>
+      <c r="G129" s="49"/>
+      <c r="H129" s="49"/>
+      <c r="I129" s="49"/>
     </row>
     <row r="130" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="27">
@@ -21725,15 +21728,15 @@
       <c r="I135" s="32"/>
     </row>
     <row r="136" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A136" s="46"/>
-      <c r="B136" s="47"/>
-      <c r="C136" s="47"/>
-      <c r="D136" s="47"/>
-      <c r="E136" s="47"/>
-      <c r="F136" s="47"/>
-      <c r="G136" s="47"/>
-      <c r="H136" s="47"/>
-      <c r="I136" s="47"/>
+      <c r="A136" s="50"/>
+      <c r="B136" s="49"/>
+      <c r="C136" s="49"/>
+      <c r="D136" s="49"/>
+      <c r="E136" s="49"/>
+      <c r="F136" s="49"/>
+      <c r="G136" s="49"/>
+      <c r="H136" s="49"/>
+      <c r="I136" s="49"/>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="27"/>
@@ -21747,15 +21750,15 @@
       <c r="I137" s="32"/>
     </row>
     <row r="138" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A138" s="46"/>
-      <c r="B138" s="47"/>
-      <c r="C138" s="47"/>
-      <c r="D138" s="47"/>
-      <c r="E138" s="47"/>
-      <c r="F138" s="47"/>
-      <c r="G138" s="47"/>
-      <c r="H138" s="47"/>
-      <c r="I138" s="47"/>
+      <c r="A138" s="50"/>
+      <c r="B138" s="49"/>
+      <c r="C138" s="49"/>
+      <c r="D138" s="49"/>
+      <c r="E138" s="49"/>
+      <c r="F138" s="49"/>
+      <c r="G138" s="49"/>
+      <c r="H138" s="49"/>
+      <c r="I138" s="49"/>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="27"/>
@@ -21769,15 +21772,15 @@
       <c r="I139" s="32"/>
     </row>
     <row r="140" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A140" s="46"/>
-      <c r="B140" s="47"/>
-      <c r="C140" s="47"/>
-      <c r="D140" s="47"/>
-      <c r="E140" s="47"/>
-      <c r="F140" s="47"/>
-      <c r="G140" s="47"/>
-      <c r="H140" s="47"/>
-      <c r="I140" s="47"/>
+      <c r="A140" s="50"/>
+      <c r="B140" s="49"/>
+      <c r="C140" s="49"/>
+      <c r="D140" s="49"/>
+      <c r="E140" s="49"/>
+      <c r="F140" s="49"/>
+      <c r="G140" s="49"/>
+      <c r="H140" s="49"/>
+      <c r="I140" s="49"/>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="27"/>
@@ -21813,15 +21816,15 @@
       <c r="I143" s="32"/>
     </row>
     <row r="144" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A144" s="46"/>
-      <c r="B144" s="47"/>
-      <c r="C144" s="47"/>
-      <c r="D144" s="47"/>
-      <c r="E144" s="47"/>
-      <c r="F144" s="47"/>
-      <c r="G144" s="47"/>
-      <c r="H144" s="47"/>
-      <c r="I144" s="47"/>
+      <c r="A144" s="50"/>
+      <c r="B144" s="49"/>
+      <c r="C144" s="49"/>
+      <c r="D144" s="49"/>
+      <c r="E144" s="49"/>
+      <c r="F144" s="49"/>
+      <c r="G144" s="49"/>
+      <c r="H144" s="49"/>
+      <c r="I144" s="49"/>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="27"/>
@@ -21868,15 +21871,15 @@
       <c r="I148" s="32"/>
     </row>
     <row r="149" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A149" s="46"/>
-      <c r="B149" s="47"/>
-      <c r="C149" s="47"/>
-      <c r="D149" s="47"/>
-      <c r="E149" s="47"/>
-      <c r="F149" s="47"/>
-      <c r="G149" s="47"/>
-      <c r="H149" s="47"/>
-      <c r="I149" s="47"/>
+      <c r="A149" s="50"/>
+      <c r="B149" s="49"/>
+      <c r="C149" s="49"/>
+      <c r="D149" s="49"/>
+      <c r="E149" s="49"/>
+      <c r="F149" s="49"/>
+      <c r="G149" s="49"/>
+      <c r="H149" s="49"/>
+      <c r="I149" s="49"/>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="27"/>
@@ -21890,15 +21893,15 @@
       <c r="I150" s="32"/>
     </row>
     <row r="151" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A151" s="46"/>
-      <c r="B151" s="47"/>
-      <c r="C151" s="47"/>
-      <c r="D151" s="47"/>
-      <c r="E151" s="47"/>
-      <c r="F151" s="47"/>
-      <c r="G151" s="47"/>
-      <c r="H151" s="47"/>
-      <c r="I151" s="47"/>
+      <c r="A151" s="50"/>
+      <c r="B151" s="49"/>
+      <c r="C151" s="49"/>
+      <c r="D151" s="49"/>
+      <c r="E151" s="49"/>
+      <c r="F151" s="49"/>
+      <c r="G151" s="49"/>
+      <c r="H151" s="49"/>
+      <c r="I151" s="49"/>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="27"/>
@@ -21912,15 +21915,15 @@
       <c r="I152" s="32"/>
     </row>
     <row r="153" spans="1:9" ht="13" x14ac:dyDescent="0.25">
-      <c r="A153" s="46"/>
-      <c r="B153" s="47"/>
-      <c r="C153" s="47"/>
-      <c r="D153" s="47"/>
-      <c r="E153" s="47"/>
-      <c r="F153" s="47"/>
-      <c r="G153" s="47"/>
-      <c r="H153" s="47"/>
-      <c r="I153" s="47"/>
+      <c r="A153" s="50"/>
+      <c r="B153" s="49"/>
+      <c r="C153" s="49"/>
+      <c r="D153" s="49"/>
+      <c r="E153" s="49"/>
+      <c r="F153" s="49"/>
+      <c r="G153" s="49"/>
+      <c r="H153" s="49"/>
+      <c r="I153" s="49"/>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="27"/>
@@ -22716,11 +22719,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A48:I48"/>
-    <mergeCell ref="A69:I69"/>
-    <mergeCell ref="A149:I149"/>
-    <mergeCell ref="A2:I2"/>
     <mergeCell ref="A151:I151"/>
     <mergeCell ref="A153:I153"/>
     <mergeCell ref="A25:I25"/>
@@ -22736,6 +22734,11 @@
     <mergeCell ref="A107:I107"/>
     <mergeCell ref="A127:I127"/>
     <mergeCell ref="A128:I128"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A48:I48"/>
+    <mergeCell ref="A69:I69"/>
+    <mergeCell ref="A149:I149"/>
+    <mergeCell ref="A2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -22744,10 +22747,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85ECB890-2199-45FD-AD5D-4DE576B93073}">
-  <dimension ref="A1:Z74"/>
+  <dimension ref="A1:Z75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -22806,7 +22809,7 @@
       <c r="Z1" s="26"/>
     </row>
     <row r="2" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="41" t="s">
         <v>158</v>
       </c>
       <c r="B2" s="48"/>
@@ -22836,17 +22839,17 @@
       <c r="Z2" s="26"/>
     </row>
     <row r="3" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="43" t="s">
         <v>148</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
       <c r="J3" s="26"/>
       <c r="K3" s="26"/>
       <c r="L3" s="26"/>
@@ -22917,7 +22920,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>4</v>
       </c>
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="36" t="s">
         <v>589</v>
       </c>
       <c r="C7" s="30"/>
@@ -22949,7 +22952,7 @@
         <f ca="1">IF(OFFSET(A9,-1,0) ="",OFFSET(A9,-2,0)+1,OFFSET(A9,-1,0)+1 )</f>
         <v>6</v>
       </c>
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="36" t="s">
         <v>207</v>
       </c>
       <c r="C9" s="30"/>
@@ -22965,7 +22968,7 @@
         <f ca="1">IF(OFFSET(A10,-1,0) ="",OFFSET(A10,-2,0)+1,OFFSET(A10,-1,0)+1 )</f>
         <v>7</v>
       </c>
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="36" t="s">
         <v>226</v>
       </c>
       <c r="C10" s="30"/>
@@ -22978,10 +22981,10 @@
     </row>
     <row r="11" spans="1:26" s="10" customFormat="1" ht="44.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="27">
-        <f t="shared" ref="A11:A58" ca="1" si="1">IF(OFFSET(A11,-1,0) ="",OFFSET(A11,-2,0)+1,OFFSET(A11,-1,0)+1 )</f>
+        <f t="shared" ref="A11:A59" ca="1" si="1">IF(OFFSET(A11,-1,0) ="",OFFSET(A11,-2,0)+1,OFFSET(A11,-1,0)+1 )</f>
         <v>8</v>
       </c>
-      <c r="B11" s="55" t="s">
+      <c r="B11" s="36" t="s">
         <v>125</v>
       </c>
       <c r="C11" s="30"/>
@@ -23029,7 +23032,7 @@
         <f t="shared" ca="1" si="1"/>
         <v>11</v>
       </c>
-      <c r="B14" s="55" t="s">
+      <c r="B14" s="36" t="s">
         <v>228</v>
       </c>
       <c r="C14" s="30"/>
@@ -23045,7 +23048,7 @@
         <f t="shared" ca="1" si="1"/>
         <v>12</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="37" t="s">
         <v>138</v>
       </c>
       <c r="C15" s="30"/>
@@ -23057,17 +23060,17 @@
       <c r="I15" s="32"/>
     </row>
     <row r="16" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="50" t="s">
         <v>554</v>
       </c>
-      <c r="B16" s="47"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49"/>
       <c r="J16" s="26"/>
       <c r="K16" s="26"/>
       <c r="L16" s="26"/>
@@ -23171,7 +23174,7 @@
         <f t="shared" ca="1" si="1"/>
         <v>18</v>
       </c>
-      <c r="B22" s="55" t="s">
+      <c r="B22" s="36" t="s">
         <v>123</v>
       </c>
       <c r="C22" s="30"/>
@@ -23187,7 +23190,7 @@
         <f t="shared" ca="1" si="1"/>
         <v>19</v>
       </c>
-      <c r="B23" s="55" t="s">
+      <c r="B23" s="36" t="s">
         <v>124</v>
       </c>
       <c r="C23" s="30"/>
@@ -23203,7 +23206,7 @@
         <f t="shared" ca="1" si="1"/>
         <v>20</v>
       </c>
-      <c r="B24" s="55" t="s">
+      <c r="B24" s="36" t="s">
         <v>125</v>
       </c>
       <c r="C24" s="30"/>
@@ -23219,7 +23222,7 @@
         <f t="shared" ca="1" si="1"/>
         <v>21</v>
       </c>
-      <c r="B25" s="55" t="s">
+      <c r="B25" s="36" t="s">
         <v>558</v>
       </c>
       <c r="C25" s="30"/>
@@ -23247,17 +23250,17 @@
       <c r="I26" s="32"/>
     </row>
     <row r="27" spans="1:26" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="46" t="s">
+      <c r="A27" s="50" t="s">
         <v>559</v>
       </c>
-      <c r="B27" s="47"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="47"/>
-      <c r="I27" s="47"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
       <c r="J27" s="26"/>
       <c r="K27" s="26"/>
       <c r="L27" s="26"/>
@@ -23371,13 +23374,13 @@
       <c r="H33" s="13"/>
       <c r="I33" s="32"/>
     </row>
-    <row r="34" spans="1:9" s="10" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="27">
         <f t="shared" ca="1" si="1"/>
         <v>29</v>
       </c>
-      <c r="B34" s="55" t="s">
-        <v>565</v>
+      <c r="B34" s="29" t="s">
+        <v>591</v>
       </c>
       <c r="C34" s="29"/>
       <c r="D34" s="30"/>
@@ -23387,15 +23390,15 @@
       <c r="H34" s="13"/>
       <c r="I34" s="32"/>
     </row>
-    <row r="35" spans="1:9" s="10" customFormat="1" ht="35.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" s="10" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="27">
         <f t="shared" ca="1" si="1"/>
         <v>30</v>
       </c>
-      <c r="B35" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="C35" s="30"/>
+      <c r="B35" s="36" t="s">
+        <v>565</v>
+      </c>
+      <c r="C35" s="29"/>
       <c r="D35" s="30"/>
       <c r="E35" s="32"/>
       <c r="F35" s="13"/>
@@ -23403,42 +23406,42 @@
       <c r="H35" s="13"/>
       <c r="I35" s="32"/>
     </row>
-    <row r="36" spans="1:9" s="10" customFormat="1" ht="21.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="46" t="s">
+    <row r="36" spans="1:9" s="10" customFormat="1" ht="35.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="32"/>
+    </row>
+    <row r="37" spans="1:9" s="10" customFormat="1" ht="21.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="50" t="s">
         <v>566</v>
       </c>
-      <c r="B36" s="47"/>
-      <c r="C36" s="47"/>
-      <c r="D36" s="47"/>
-      <c r="E36" s="47"/>
-      <c r="F36" s="47"/>
-      <c r="G36" s="47"/>
-      <c r="H36" s="47"/>
-      <c r="I36" s="47"/>
-    </row>
-    <row r="37" spans="1:9" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="27">
-        <f ca="1">IF(OFFSET(A37,-2,0) ="",OFFSET(A37,-2,0)+1,OFFSET(A37,-2,0)+1 )</f>
-        <v>31</v>
-      </c>
-      <c r="B37" s="30" t="s">
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="49"/>
+    </row>
+    <row r="38" spans="1:9" s="10" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="27">
+        <f ca="1">IF(OFFSET(A38,-2,0) ="",OFFSET(A38,-2,0)+1,OFFSET(A38,-2,0)+1 )</f>
+        <v>32</v>
+      </c>
+      <c r="B38" s="30" t="s">
         <v>139</v>
-      </c>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="32"/>
-    </row>
-    <row r="38" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>32</v>
-      </c>
-      <c r="B38" s="30" t="s">
-        <v>141</v>
       </c>
       <c r="C38" s="30"/>
       <c r="D38" s="30"/>
@@ -23448,17 +23451,17 @@
       <c r="H38" s="13"/>
       <c r="I38" s="32"/>
     </row>
-    <row r="39" spans="1:9" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" s="10" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="27">
         <f t="shared" ca="1" si="1"/>
         <v>33</v>
       </c>
       <c r="B39" s="30" t="s">
-        <v>567</v>
+        <v>141</v>
       </c>
       <c r="C39" s="30"/>
       <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
+      <c r="E39" s="32"/>
       <c r="F39" s="13"/>
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
@@ -23470,7 +23473,7 @@
         <v>34</v>
       </c>
       <c r="B40" s="30" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C40" s="30"/>
       <c r="D40" s="30"/>
@@ -23480,29 +23483,29 @@
       <c r="H40" s="13"/>
       <c r="I40" s="32"/>
     </row>
-    <row r="41" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="27">
         <f t="shared" ca="1" si="1"/>
         <v>35</v>
       </c>
       <c r="B41" s="30" t="s">
-        <v>569</v>
-      </c>
-      <c r="C41" s="29"/>
+        <v>568</v>
+      </c>
+      <c r="C41" s="30"/>
       <c r="D41" s="30"/>
-      <c r="E41" s="32"/>
+      <c r="E41" s="30"/>
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
       <c r="I41" s="32"/>
     </row>
-    <row r="42" spans="1:9" s="10" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="27">
         <f t="shared" ca="1" si="1"/>
         <v>36</v>
       </c>
-      <c r="B42" s="35" t="s">
-        <v>571</v>
+      <c r="B42" s="30" t="s">
+        <v>569</v>
       </c>
       <c r="C42" s="29"/>
       <c r="D42" s="30"/>
@@ -23512,42 +23515,42 @@
       <c r="H42" s="13"/>
       <c r="I42" s="32"/>
     </row>
-    <row r="43" spans="1:9" s="10" customFormat="1" ht="23.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="46" t="s">
+    <row r="43" spans="1:9" s="10" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="B43" s="35" t="s">
+        <v>571</v>
+      </c>
+      <c r="C43" s="29"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="32"/>
+    </row>
+    <row r="44" spans="1:9" s="10" customFormat="1" ht="23.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="50" t="s">
         <v>570</v>
       </c>
-      <c r="B43" s="47"/>
-      <c r="C43" s="47"/>
-      <c r="D43" s="47"/>
-      <c r="E43" s="47"/>
-      <c r="F43" s="47"/>
-      <c r="G43" s="47"/>
-      <c r="H43" s="47"/>
-      <c r="I43" s="47"/>
-    </row>
-    <row r="44" spans="1:9" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="27">
-        <f ca="1">IF(OFFSET(A44,-2,0) ="",OFFSET(A44,-2,0)+1,OFFSET(A44,-2,0)+1 )</f>
-        <v>37</v>
-      </c>
-      <c r="B44" s="30" t="s">
+      <c r="B44" s="49"/>
+      <c r="C44" s="49"/>
+      <c r="D44" s="49"/>
+      <c r="E44" s="49"/>
+      <c r="F44" s="49"/>
+      <c r="G44" s="49"/>
+      <c r="H44" s="49"/>
+      <c r="I44" s="49"/>
+    </row>
+    <row r="45" spans="1:9" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="27">
+        <f ca="1">IF(OFFSET(A45,-2,0) ="",OFFSET(A45,-2,0)+1,OFFSET(A45,-2,0)+1 )</f>
+        <v>38</v>
+      </c>
+      <c r="B45" s="30" t="s">
         <v>139</v>
-      </c>
-      <c r="C44" s="30"/>
-      <c r="D44" s="30"/>
-      <c r="E44" s="32"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="32"/>
-    </row>
-    <row r="45" spans="1:9" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>38</v>
-      </c>
-      <c r="B45" s="30" t="s">
-        <v>141</v>
       </c>
       <c r="C45" s="30"/>
       <c r="D45" s="30"/>
@@ -23557,13 +23560,13 @@
       <c r="H45" s="13"/>
       <c r="I45" s="32"/>
     </row>
-    <row r="46" spans="1:9" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="27">
         <f t="shared" ca="1" si="1"/>
         <v>39</v>
       </c>
       <c r="B46" s="30" t="s">
-        <v>575</v>
+        <v>141</v>
       </c>
       <c r="C46" s="30"/>
       <c r="D46" s="30"/>
@@ -23573,15 +23576,15 @@
       <c r="H46" s="13"/>
       <c r="I46" s="32"/>
     </row>
-    <row r="47" spans="1:9" s="10" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="27">
         <f t="shared" ca="1" si="1"/>
         <v>40</v>
       </c>
       <c r="B47" s="30" t="s">
-        <v>568</v>
-      </c>
-      <c r="C47" s="29"/>
+        <v>575</v>
+      </c>
+      <c r="C47" s="30"/>
       <c r="D47" s="30"/>
       <c r="E47" s="32"/>
       <c r="F47" s="13"/>
@@ -23595,7 +23598,7 @@
         <v>41</v>
       </c>
       <c r="B48" s="30" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="C48" s="29"/>
       <c r="D48" s="30"/>
@@ -23605,13 +23608,13 @@
       <c r="H48" s="13"/>
       <c r="I48" s="32"/>
     </row>
-    <row r="49" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" s="10" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="27">
         <f t="shared" ca="1" si="1"/>
         <v>42</v>
       </c>
       <c r="B49" s="30" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C49" s="29"/>
       <c r="D49" s="30"/>
@@ -23621,13 +23624,13 @@
       <c r="H49" s="13"/>
       <c r="I49" s="32"/>
     </row>
-    <row r="50" spans="1:9" s="10" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="27">
         <f t="shared" ca="1" si="1"/>
         <v>43</v>
       </c>
-      <c r="B50" s="35" t="s">
-        <v>572</v>
+      <c r="B50" s="30" t="s">
+        <v>574</v>
       </c>
       <c r="C50" s="29"/>
       <c r="D50" s="30"/>
@@ -23637,44 +23640,44 @@
       <c r="H50" s="13"/>
       <c r="I50" s="32"/>
     </row>
-    <row r="51" spans="1:9" s="10" customFormat="1" ht="23.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="46" t="s">
+    <row r="51" spans="1:9" s="10" customFormat="1" ht="35.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="B51" s="35" t="s">
+        <v>572</v>
+      </c>
+      <c r="C51" s="29"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="32"/>
+    </row>
+    <row r="52" spans="1:9" s="10" customFormat="1" ht="23.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="50" t="s">
         <v>576</v>
       </c>
-      <c r="B51" s="47"/>
-      <c r="C51" s="47"/>
-      <c r="D51" s="47"/>
-      <c r="E51" s="47"/>
-      <c r="F51" s="47"/>
-      <c r="G51" s="47"/>
-      <c r="H51" s="47"/>
-      <c r="I51" s="47"/>
-    </row>
-    <row r="52" spans="1:9" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="27">
-        <f ca="1">IF(OFFSET(A52,-2,0) ="",OFFSET(A52,-2,0)+1,OFFSET(A52,-2,0)+1 )</f>
-        <v>44</v>
-      </c>
-      <c r="B52" s="30" t="s">
+      <c r="B52" s="49"/>
+      <c r="C52" s="49"/>
+      <c r="D52" s="49"/>
+      <c r="E52" s="49"/>
+      <c r="F52" s="49"/>
+      <c r="G52" s="49"/>
+      <c r="H52" s="49"/>
+      <c r="I52" s="49"/>
+    </row>
+    <row r="53" spans="1:9" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="27">
+        <f ca="1">IF(OFFSET(A53,-2,0) ="",OFFSET(A53,-2,0)+1,OFFSET(A53,-2,0)+1 )</f>
+        <v>45</v>
+      </c>
+      <c r="B53" s="30" t="s">
         <v>139</v>
       </c>
-      <c r="C52" s="30"/>
-      <c r="D52" s="30"/>
-      <c r="E52" s="32"/>
-      <c r="F52" s="13"/>
-      <c r="G52" s="13"/>
-      <c r="H52" s="13"/>
-      <c r="I52" s="32"/>
-    </row>
-    <row r="53" spans="1:9" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="27">
-        <f t="shared" ca="1" si="1"/>
-        <v>45</v>
-      </c>
-      <c r="B53" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="C53" s="29"/>
+      <c r="C53" s="30"/>
       <c r="D53" s="30"/>
       <c r="E53" s="32"/>
       <c r="F53" s="13"/>
@@ -23682,15 +23685,15 @@
       <c r="H53" s="13"/>
       <c r="I53" s="32"/>
     </row>
-    <row r="54" spans="1:9" s="10" customFormat="1" ht="38.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="27">
         <f t="shared" ca="1" si="1"/>
         <v>46</v>
       </c>
       <c r="B54" s="30" t="s">
-        <v>577</v>
-      </c>
-      <c r="C54" s="30"/>
+        <v>141</v>
+      </c>
+      <c r="C54" s="29"/>
       <c r="D54" s="30"/>
       <c r="E54" s="32"/>
       <c r="F54" s="13"/>
@@ -23698,13 +23701,13 @@
       <c r="H54" s="13"/>
       <c r="I54" s="32"/>
     </row>
-    <row r="55" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" s="10" customFormat="1" ht="38.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="27">
         <f t="shared" ca="1" si="1"/>
         <v>47</v>
       </c>
       <c r="B55" s="30" t="s">
-        <v>568</v>
+        <v>577</v>
       </c>
       <c r="C55" s="30"/>
       <c r="D55" s="30"/>
@@ -23714,13 +23717,13 @@
       <c r="H55" s="13"/>
       <c r="I55" s="32"/>
     </row>
-    <row r="56" spans="1:9" s="10" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" s="10" customFormat="1" ht="33.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="27">
         <f t="shared" ca="1" si="1"/>
         <v>48</v>
       </c>
       <c r="B56" s="30" t="s">
-        <v>578</v>
+        <v>568</v>
       </c>
       <c r="C56" s="30"/>
       <c r="D56" s="30"/>
@@ -23730,13 +23733,13 @@
       <c r="H56" s="13"/>
       <c r="I56" s="32"/>
     </row>
-    <row r="57" spans="1:9" s="10" customFormat="1" ht="24.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" s="10" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="27">
         <f t="shared" ca="1" si="1"/>
         <v>49</v>
       </c>
       <c r="B57" s="30" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C57" s="30"/>
       <c r="D57" s="30"/>
@@ -23746,13 +23749,13 @@
       <c r="H57" s="13"/>
       <c r="I57" s="32"/>
     </row>
-    <row r="58" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" s="10" customFormat="1" ht="24.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="27">
         <f t="shared" ca="1" si="1"/>
         <v>50</v>
       </c>
-      <c r="B58" s="35" t="s">
-        <v>580</v>
+      <c r="B58" s="30" t="s">
+        <v>579</v>
       </c>
       <c r="C58" s="30"/>
       <c r="D58" s="30"/>
@@ -23762,55 +23765,55 @@
       <c r="H58" s="13"/>
       <c r="I58" s="32"/>
     </row>
-    <row r="59" spans="1:9" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="39" t="s">
+    <row r="59" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="B59" s="35" t="s">
+        <v>580</v>
+      </c>
+      <c r="C59" s="30"/>
+      <c r="D59" s="30"/>
+      <c r="E59" s="32"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="32"/>
+    </row>
+    <row r="60" spans="1:9" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="41" t="s">
         <v>159</v>
       </c>
-      <c r="B59" s="48"/>
-      <c r="C59" s="48"/>
-      <c r="D59" s="48"/>
-      <c r="E59" s="48"/>
-      <c r="F59" s="48"/>
-      <c r="G59" s="48"/>
-      <c r="H59" s="48"/>
-      <c r="I59" s="48"/>
-    </row>
-    <row r="60" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="46" t="s">
+      <c r="B60" s="48"/>
+      <c r="C60" s="48"/>
+      <c r="D60" s="48"/>
+      <c r="E60" s="48"/>
+      <c r="F60" s="48"/>
+      <c r="G60" s="48"/>
+      <c r="H60" s="48"/>
+      <c r="I60" s="48"/>
+    </row>
+    <row r="61" spans="1:9" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="50" t="s">
         <v>581</v>
       </c>
-      <c r="B60" s="47"/>
-      <c r="C60" s="47"/>
-      <c r="D60" s="47"/>
-      <c r="E60" s="47"/>
-      <c r="F60" s="47"/>
-      <c r="G60" s="47"/>
-      <c r="H60" s="47"/>
-      <c r="I60" s="47"/>
-    </row>
-    <row r="61" spans="1:9" s="10" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="27">
-        <f ca="1">IF(OFFSET(A61,-3,0) ="",OFFSET(A61,-3,0)+1,OFFSET(A61,-3,0)+1 )</f>
-        <v>51</v>
-      </c>
-      <c r="B61" s="30" t="s">
+      <c r="B61" s="49"/>
+      <c r="C61" s="49"/>
+      <c r="D61" s="49"/>
+      <c r="E61" s="49"/>
+      <c r="F61" s="49"/>
+      <c r="G61" s="49"/>
+      <c r="H61" s="49"/>
+      <c r="I61" s="49"/>
+    </row>
+    <row r="62" spans="1:9" s="10" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="27">
+        <f ca="1">IF(OFFSET(A62,-3,0) ="",OFFSET(A62,-3,0)+1,OFFSET(A62,-3,0)+1 )</f>
+        <v>52</v>
+      </c>
+      <c r="B62" s="30" t="s">
         <v>582</v>
-      </c>
-      <c r="C61" s="30"/>
-      <c r="D61" s="30"/>
-      <c r="E61" s="32"/>
-      <c r="F61" s="13"/>
-      <c r="G61" s="13"/>
-      <c r="H61" s="13"/>
-      <c r="I61" s="32"/>
-    </row>
-    <row r="62" spans="1:9" s="10" customFormat="1" ht="50.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="27">
-        <f t="shared" ref="A62:A74" ca="1" si="2">IF(OFFSET(A62,-1,0) ="",OFFSET(A62,-2,0)+1,OFFSET(A62,-1,0)+1 )</f>
-        <v>52</v>
-      </c>
-      <c r="B62" s="30" t="s">
-        <v>583</v>
       </c>
       <c r="C62" s="30"/>
       <c r="D62" s="30"/>
@@ -23820,13 +23823,13 @@
       <c r="H62" s="13"/>
       <c r="I62" s="32"/>
     </row>
-    <row r="63" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" s="10" customFormat="1" ht="50.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="27">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ref="A63:A75" ca="1" si="2">IF(OFFSET(A63,-1,0) ="",OFFSET(A63,-2,0)+1,OFFSET(A63,-1,0)+1 )</f>
         <v>53</v>
       </c>
       <c r="B63" s="30" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C63" s="30"/>
       <c r="D63" s="30"/>
@@ -23836,13 +23839,13 @@
       <c r="H63" s="13"/>
       <c r="I63" s="32"/>
     </row>
-    <row r="64" spans="1:9" s="10" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="27">
         <f t="shared" ca="1" si="2"/>
         <v>54</v>
       </c>
       <c r="B64" s="30" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C64" s="30"/>
       <c r="D64" s="30"/>
@@ -23852,13 +23855,13 @@
       <c r="H64" s="13"/>
       <c r="I64" s="32"/>
     </row>
-    <row r="65" spans="1:9" s="10" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" s="10" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="27">
         <f t="shared" ca="1" si="2"/>
         <v>55</v>
       </c>
       <c r="B65" s="30" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C65" s="30"/>
       <c r="D65" s="30"/>
@@ -23868,13 +23871,13 @@
       <c r="H65" s="13"/>
       <c r="I65" s="32"/>
     </row>
-    <row r="66" spans="1:9" s="10" customFormat="1" ht="63.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" s="10" customFormat="1" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="27">
         <f t="shared" ca="1" si="2"/>
         <v>56</v>
       </c>
       <c r="B66" s="30" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C66" s="30"/>
       <c r="D66" s="30"/>
@@ -23884,12 +23887,14 @@
       <c r="H66" s="13"/>
       <c r="I66" s="32"/>
     </row>
-    <row r="67" spans="1:9" s="10" customFormat="1" ht="56.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" s="10" customFormat="1" ht="63.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="27">
         <f t="shared" ca="1" si="2"/>
         <v>57</v>
       </c>
-      <c r="B67" s="30"/>
+      <c r="B67" s="30" t="s">
+        <v>587</v>
+      </c>
       <c r="C67" s="30"/>
       <c r="D67" s="30"/>
       <c r="E67" s="32"/>
@@ -23898,11 +23903,12 @@
       <c r="H67" s="13"/>
       <c r="I67" s="32"/>
     </row>
-    <row r="68" spans="1:9" s="10" customFormat="1" ht="32.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" s="10" customFormat="1" ht="56.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="27">
         <f t="shared" ca="1" si="2"/>
         <v>58</v>
       </c>
+      <c r="B68" s="30"/>
       <c r="C68" s="30"/>
       <c r="D68" s="30"/>
       <c r="E68" s="32"/>
@@ -23916,7 +23922,6 @@
         <f t="shared" ca="1" si="2"/>
         <v>59</v>
       </c>
-      <c r="B69" s="30"/>
       <c r="C69" s="30"/>
       <c r="D69" s="30"/>
       <c r="E69" s="32"/>
@@ -23925,12 +23930,12 @@
       <c r="H69" s="13"/>
       <c r="I69" s="32"/>
     </row>
-    <row r="70" spans="1:9" s="10" customFormat="1" ht="33.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" s="10" customFormat="1" ht="32.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="27">
         <f t="shared" ca="1" si="2"/>
         <v>60</v>
       </c>
-      <c r="B70" s="29"/>
+      <c r="B70" s="30"/>
       <c r="C70" s="30"/>
       <c r="D70" s="30"/>
       <c r="E70" s="32"/>
@@ -23995,17 +24000,31 @@
       <c r="H74" s="13"/>
       <c r="I74" s="32"/>
     </row>
+    <row r="75" spans="1:9" s="10" customFormat="1" ht="33.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="27">
+        <f t="shared" ca="1" si="2"/>
+        <v>65</v>
+      </c>
+      <c r="B75" s="29"/>
+      <c r="C75" s="30"/>
+      <c r="D75" s="30"/>
+      <c r="E75" s="32"/>
+      <c r="F75" s="13"/>
+      <c r="G75" s="13"/>
+      <c r="H75" s="13"/>
+      <c r="I75" s="32"/>
+    </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A51:I51"/>
-    <mergeCell ref="A59:I59"/>
+    <mergeCell ref="A52:I52"/>
     <mergeCell ref="A60:I60"/>
+    <mergeCell ref="A61:I61"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A16:I16"/>
     <mergeCell ref="A27:I27"/>
-    <mergeCell ref="A36:I36"/>
-    <mergeCell ref="A43:I43"/>
+    <mergeCell ref="A37:I37"/>
+    <mergeCell ref="A44:I44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Updated TC5 (9 cases)
</commit_message>
<xml_diff>
--- a/Middle Assignment/TestDesignTechique_PhamHongAnh.xlsx
+++ b/Middle Assignment/TestDesignTechique_PhamHongAnh.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NashTech\Rookies\NashTech_Homework\Middle Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CCC162-C055-4D16-BC33-35C437EB55AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17ACD5B5-B890-428F-B0D1-DFCE456B8AA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11715" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11715" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment 1" sheetId="1" r:id="rId1"/>
@@ -1175,7 +1175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="836">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="836">
   <si>
     <t>ID</t>
   </si>
@@ -26301,7 +26301,7 @@
   <dimension ref="A1:XFD85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26514,28 +26514,40 @@
       <c r="H10" s="13"/>
       <c r="I10" s="32"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="47.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>9</v>
       </c>
-      <c r="B11" s="35"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
+      <c r="B11" s="36" t="s">
+        <v>755</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>768</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>769</v>
+      </c>
+      <c r="E11" s="32"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
       <c r="I11" s="32"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="27">
         <f t="shared" ca="1" si="0"/>
         <v>10</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
+      <c r="B12" s="36" t="s">
+        <v>752</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>768</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>770</v>
+      </c>
       <c r="E12" s="32"/>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>

</xml_diff>